<commit_message>
updated reg files with better weighting
</commit_message>
<xml_diff>
--- a/input/reg_health_mental.xlsx
+++ b/input/reg_health_mental.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\andy_local\SimPaths project files\SimPaths\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43B1EAC9-423A-43FB-B4D6-8A9E7509A719}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E39558C1-59CF-44AF-94E9-2ECEEAEE101C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,9 +18,9 @@
     <sheet name="UK_HM1_C" sheetId="7" r:id="rId3"/>
     <sheet name="UK_HM2_Males_C" sheetId="8" r:id="rId4"/>
     <sheet name="UK_HM2_Females_C" sheetId="9" r:id="rId5"/>
-    <sheet name="UK_HM1_L" sheetId="19" r:id="rId6"/>
-    <sheet name="UK_HM2_Males_L" sheetId="20" r:id="rId7"/>
-    <sheet name="UK_HM2_Females_L" sheetId="21" r:id="rId8"/>
+    <sheet name="UK_HM1_L" sheetId="22" r:id="rId6"/>
+    <sheet name="UK_HM2_Males_L" sheetId="23" r:id="rId7"/>
+    <sheet name="UK_HM2_Females_L" sheetId="24" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -4766,7 +4766,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8245F431-0F24-4624-A6D5-5D6AADF13317}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD05762E-8E4A-4531-8778-2DDE3401ADAE}">
   <dimension ref="A1:AE30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -4877,94 +4877,94 @@
         <v>19</v>
       </c>
       <c r="B2" s="8">
-        <v>2.4195958501664401E-2</v>
+        <v>5.6748988544512704E-3</v>
       </c>
       <c r="C2" s="8">
-        <v>5.4919605445868502E-4</v>
+        <v>6.3126110626850901E-4</v>
       </c>
       <c r="D2" s="8">
-        <v>4.0512308198994502E-4</v>
+        <v>4.6396264246978099E-4</v>
       </c>
       <c r="E2" s="8">
-        <v>-1.08715793209818E-4</v>
+        <v>-1.3004541165257099E-4</v>
       </c>
       <c r="F2" s="8">
-        <v>-8.4676651776102694E-5</v>
+        <v>-9.6397417107954396E-5</v>
       </c>
       <c r="G2" s="8">
-        <v>-6.9108178710131996E-5</v>
+        <v>-8.1400804213283898E-5</v>
       </c>
       <c r="H2" s="8">
-        <v>-1.0892821700986599E-4</v>
+        <v>-1.25125408959879E-4</v>
       </c>
       <c r="I2" s="8">
-        <v>-7.4275442937390003E-5</v>
+        <v>-8.5622027362546E-5</v>
       </c>
       <c r="J2" s="8">
-        <v>-8.2828945375216302E-5</v>
+        <v>-9.4587619678724195E-5</v>
       </c>
       <c r="K2" s="8">
-        <v>-6.18713044141723E-5</v>
+        <v>-7.4270576203027097E-5</v>
       </c>
       <c r="L2" s="8">
-        <v>-8.1341707694572899E-5</v>
+        <v>-9.2852913357332201E-5</v>
       </c>
       <c r="M2" s="8">
-        <v>-8.5239585287131899E-5</v>
+        <v>-9.7723831375078806E-5</v>
       </c>
       <c r="N2" s="8">
-        <v>-7.93702801573131E-5</v>
+        <v>-8.9147371597648803E-5</v>
       </c>
       <c r="O2" s="8">
-        <v>-8.2836745822835502E-5</v>
+        <v>-9.6704789632620197E-5</v>
       </c>
       <c r="P2" s="8">
-        <v>-5.5035653519916099E-6</v>
+        <v>-3.35944138396503E-6</v>
       </c>
       <c r="Q2" s="8">
-        <v>1.6792741570474201E-5</v>
+        <v>2.6694639089029299E-5</v>
       </c>
       <c r="R2" s="8">
-        <v>-2.8762216933361899E-5</v>
+        <v>-3.4739667835109602E-5</v>
       </c>
       <c r="S2" s="8">
-        <v>-8.2780689322515501E-6</v>
+        <v>-9.9279137317001898E-6</v>
       </c>
       <c r="T2" s="8">
-        <v>-4.0592578385189901E-5</v>
+        <v>-4.1350089656322197E-5</v>
       </c>
       <c r="U2" s="8">
-        <v>3.9379643112702798E-6</v>
+        <v>1.91318083550039E-6</v>
       </c>
       <c r="V2" s="8">
-        <v>8.3171355284270804E-6</v>
+        <v>3.3041349502523199E-6</v>
       </c>
       <c r="W2" s="8">
-        <v>4.2359405450572197E-5</v>
+        <v>4.6952328925989297E-5</v>
       </c>
       <c r="X2" s="8">
-        <v>1.1310542853406799E-4</v>
+        <v>1.26673590139778E-4</v>
       </c>
       <c r="Y2" s="8">
-        <v>3.8098118934446802E-6</v>
+        <v>4.5839887235734501E-6</v>
       </c>
       <c r="Z2" s="8">
-        <v>2.3186605375299799E-6</v>
+        <v>1.45013491727407E-6</v>
       </c>
       <c r="AA2" s="8">
-        <v>-2.96876384478013E-8</v>
+        <v>-2.47772683099099E-8</v>
       </c>
       <c r="AB2" s="8">
-        <v>3.1793643979944501E-6</v>
+        <v>4.2520475251047098E-6</v>
       </c>
       <c r="AC2" s="8">
-        <v>1.78226410581721E-6</v>
+        <v>2.1251460495041098E-6</v>
       </c>
       <c r="AD2" s="8">
-        <v>-3.0175895987922599E-6</v>
+        <v>-1.9128150086190201E-6</v>
       </c>
       <c r="AE2" s="8">
-        <v>-5.4423565653146603E-4</v>
+        <v>-6.0671325234516705E-4</v>
       </c>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.25">
@@ -4972,94 +4972,94 @@
         <v>20</v>
       </c>
       <c r="B3" s="8">
-        <v>7.9922808730543707E-2</v>
+        <v>4.58104364426219E-2</v>
       </c>
       <c r="C3" s="8">
-        <v>4.0512308198994502E-4</v>
+        <v>4.6396264246978099E-4</v>
       </c>
       <c r="D3" s="8">
-        <v>1.1175392770619E-3</v>
+        <v>1.31059947545629E-3</v>
       </c>
       <c r="E3" s="8">
-        <v>-8.3576142469411201E-5</v>
+        <v>-9.4289079430570294E-5</v>
       </c>
       <c r="F3" s="8">
-        <v>-6.0294579305028402E-5</v>
+        <v>-6.0208371812228003E-5</v>
       </c>
       <c r="G3" s="8">
-        <v>-6.6940974705391993E-5</v>
+        <v>-7.0781895239614901E-5</v>
       </c>
       <c r="H3" s="8">
-        <v>-1.12820541444904E-4</v>
+        <v>-1.2473366291214101E-4</v>
       </c>
       <c r="I3" s="8">
-        <v>-8.3977193400694195E-5</v>
+        <v>-9.3338907756125307E-5</v>
       </c>
       <c r="J3" s="8">
-        <v>-8.4577966213917604E-5</v>
+        <v>-9.4309582073782804E-5</v>
       </c>
       <c r="K3" s="8">
-        <v>-4.3207434944475701E-5</v>
+        <v>-4.4411074543662501E-5</v>
       </c>
       <c r="L3" s="8">
-        <v>-5.3063497433085801E-5</v>
+        <v>-5.4190283143972801E-5</v>
       </c>
       <c r="M3" s="8">
-        <v>-8.0749002867724906E-5</v>
+        <v>-9.2512056332152902E-5</v>
       </c>
       <c r="N3" s="8">
-        <v>-4.0465518631359199E-5</v>
+        <v>-4.3534145061445298E-5</v>
       </c>
       <c r="O3" s="8">
-        <v>-1.15661976859249E-4</v>
+        <v>-1.3578467718021399E-4</v>
       </c>
       <c r="P3" s="8">
-        <v>2.12307898133759E-6</v>
+        <v>3.2340782466820501E-6</v>
       </c>
       <c r="Q3" s="8">
-        <v>7.3934289024519E-5</v>
+        <v>9.1837794212754694E-5</v>
       </c>
       <c r="R3" s="8">
-        <v>-7.4290236969621802E-6</v>
+        <v>-4.24053282701221E-6</v>
       </c>
       <c r="S3" s="8">
-        <v>-1.8698510442086401E-6</v>
+        <v>-2.13462856629145E-6</v>
       </c>
       <c r="T3" s="8">
-        <v>-2.1221594112663101E-5</v>
+        <v>-1.42209370920578E-5</v>
       </c>
       <c r="U3" s="8">
-        <v>3.0996645130731401E-5</v>
+        <v>3.5814952747186198E-5</v>
       </c>
       <c r="V3" s="8">
-        <v>7.9350084145568799E-5</v>
+        <v>8.9611846726394003E-5</v>
       </c>
       <c r="W3" s="8">
-        <v>1.4105827746942399E-4</v>
+        <v>1.6642486668752901E-4</v>
       </c>
       <c r="X3" s="8">
-        <v>2.3307138367297499E-4</v>
+        <v>2.72846330738831E-4</v>
       </c>
       <c r="Y3" s="8">
-        <v>1.1502362711482E-5</v>
+        <v>1.32370347400556E-5</v>
       </c>
       <c r="Z3" s="8">
-        <v>4.5098950532457102E-6</v>
+        <v>4.93913349409411E-6</v>
       </c>
       <c r="AA3" s="8">
-        <v>-1.10974150357213E-7</v>
+        <v>-1.2776962150714601E-7</v>
       </c>
       <c r="AB3" s="8">
-        <v>1.78599217928677E-6</v>
+        <v>2.6595676599196199E-6</v>
       </c>
       <c r="AC3" s="8">
-        <v>3.8572680684296296E-6</v>
+        <v>4.3413988867913702E-6</v>
       </c>
       <c r="AD3" s="8">
-        <v>1.5613719487008001E-5</v>
+        <v>2.25295374613286E-5</v>
       </c>
       <c r="AE3" s="8">
-        <v>-8.3290283417442003E-4</v>
+        <v>-9.6085385193366804E-4</v>
       </c>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.25">
@@ -5067,94 +5067,94 @@
         <v>23</v>
       </c>
       <c r="B4" s="8">
-        <v>0.15593164654545399</v>
+        <v>5.7585650605830097E-2</v>
       </c>
       <c r="C4" s="8">
-        <v>-1.08715793209818E-4</v>
+        <v>-1.3004541165257099E-4</v>
       </c>
       <c r="D4" s="8">
-        <v>-8.3576142469411201E-5</v>
+        <v>-9.4289079430570294E-5</v>
       </c>
       <c r="E4" s="8">
-        <v>3.65124643539515E-3</v>
+        <v>4.2421007873033297E-3</v>
       </c>
       <c r="F4" s="8">
-        <v>1.07134850522502E-3</v>
+        <v>1.30136794406968E-3</v>
       </c>
       <c r="G4" s="8">
-        <v>1.06881146678558E-3</v>
+        <v>1.2982998800629699E-3</v>
       </c>
       <c r="H4" s="8">
-        <v>1.0772090686666301E-3</v>
+        <v>1.3094530308266801E-3</v>
       </c>
       <c r="I4" s="8">
-        <v>1.0722043200595999E-3</v>
+        <v>1.30494669899701E-3</v>
       </c>
       <c r="J4" s="8">
-        <v>1.0664441415601401E-3</v>
+        <v>1.29621750655437E-3</v>
       </c>
       <c r="K4" s="8">
-        <v>1.0594285005420701E-3</v>
+        <v>1.2886934092175401E-3</v>
       </c>
       <c r="L4" s="8">
-        <v>1.07590161658082E-3</v>
+        <v>1.3066161794066499E-3</v>
       </c>
       <c r="M4" s="8">
-        <v>1.0845393177464299E-3</v>
+        <v>1.3189121274853801E-3</v>
       </c>
       <c r="N4" s="8">
-        <v>1.0720587591444E-3</v>
+        <v>1.3026680835184199E-3</v>
       </c>
       <c r="O4" s="8">
-        <v>1.07241075551539E-3</v>
+        <v>1.3041465695219901E-3</v>
       </c>
       <c r="P4" s="8">
-        <v>-3.9711514492125398E-6</v>
+        <v>-2.75340398856397E-6</v>
       </c>
       <c r="Q4" s="8">
-        <v>-1.1880154133844001E-4</v>
+        <v>-1.40446383635702E-4</v>
       </c>
       <c r="R4" s="8">
-        <v>5.6169581710956697E-5</v>
+        <v>6.8412831530912995E-5</v>
       </c>
       <c r="S4" s="8">
-        <v>-4.9240868057766601E-6</v>
+        <v>-1.20138070365011E-5</v>
       </c>
       <c r="T4" s="8">
-        <v>3.68857457939547E-5</v>
+        <v>4.7438658382716498E-5</v>
       </c>
       <c r="U4" s="8">
-        <v>4.1729103326868701E-6</v>
+        <v>2.79489533657508E-6</v>
       </c>
       <c r="V4" s="8">
-        <v>2.0962883283508201E-5</v>
+        <v>2.2573849262117901E-5</v>
       </c>
       <c r="W4" s="8">
-        <v>4.4104427172820198E-5</v>
+        <v>5.2391126157177499E-5</v>
       </c>
       <c r="X4" s="8">
-        <v>7.5498205724560394E-5</v>
+        <v>8.9592986289246894E-5</v>
       </c>
       <c r="Y4" s="8">
-        <v>1.8836165493875299E-6</v>
+        <v>3.1332567222028001E-6</v>
       </c>
       <c r="Z4" s="8">
-        <v>1.4540394072156199E-6</v>
+        <v>7.68817234143558E-7</v>
       </c>
       <c r="AA4" s="8">
-        <v>-2.0871386532620001E-8</v>
+        <v>-1.6172177507542401E-8</v>
       </c>
       <c r="AB4" s="8">
-        <v>-3.6280323879363201E-6</v>
+        <v>-3.80156139540954E-6</v>
       </c>
       <c r="AC4" s="8">
-        <v>-3.5091664866875298E-7</v>
+        <v>-4.9403178871451397E-7</v>
       </c>
       <c r="AD4" s="8">
-        <v>-3.5306746234211701E-6</v>
+        <v>-5.7051324325327504E-6</v>
       </c>
       <c r="AE4" s="8">
-        <v>-9.2716630111859696E-4</v>
+        <v>-1.12083588291062E-3</v>
       </c>
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.25">
@@ -5162,94 +5162,94 @@
         <v>24</v>
       </c>
       <c r="B5" s="8">
-        <v>0.102371208426618</v>
+        <v>7.1134763037591101E-2</v>
       </c>
       <c r="C5" s="8">
-        <v>-8.4676651776102694E-5</v>
+        <v>-9.6397417107954396E-5</v>
       </c>
       <c r="D5" s="8">
-        <v>-6.0294579305028402E-5</v>
+        <v>-6.0208371812228003E-5</v>
       </c>
       <c r="E5" s="8">
-        <v>1.07134850522502E-3</v>
+        <v>1.30136794406968E-3</v>
       </c>
       <c r="F5" s="8">
-        <v>2.0514056808268702E-3</v>
+        <v>2.4701481765281698E-3</v>
       </c>
       <c r="G5" s="8">
-        <v>1.06535105216462E-3</v>
+        <v>1.2923295063619401E-3</v>
       </c>
       <c r="H5" s="8">
-        <v>1.07129659042635E-3</v>
+        <v>1.3000347035909399E-3</v>
       </c>
       <c r="I5" s="8">
-        <v>1.0608049460324499E-3</v>
+        <v>1.28907040787262E-3</v>
       </c>
       <c r="J5" s="8">
-        <v>1.0594521715121901E-3</v>
+        <v>1.2854996651937001E-3</v>
       </c>
       <c r="K5" s="8">
-        <v>1.0566308302990401E-3</v>
+        <v>1.2837201742287401E-3</v>
       </c>
       <c r="L5" s="8">
-        <v>1.06876690399174E-3</v>
+        <v>1.2961002392839699E-3</v>
       </c>
       <c r="M5" s="8">
-        <v>1.0695018880522199E-3</v>
+        <v>1.2981937161402001E-3</v>
       </c>
       <c r="N5" s="8">
-        <v>1.0666111982737599E-3</v>
+        <v>1.2936548458679601E-3</v>
       </c>
       <c r="O5" s="8">
-        <v>1.0624004163837699E-3</v>
+        <v>1.28832358926761E-3</v>
       </c>
       <c r="P5" s="8">
-        <v>-4.4443045675280199E-7</v>
+        <v>-2.71926192311181E-6</v>
       </c>
       <c r="Q5" s="8">
-        <v>-1.1342860769951601E-4</v>
+        <v>-1.27013501833536E-4</v>
       </c>
       <c r="R5" s="8">
-        <v>6.5990720673164303E-5</v>
+        <v>8.7608382022937703E-5</v>
       </c>
       <c r="S5" s="8">
-        <v>-1.7057351646447302E-5</v>
+        <v>-2.0077626985483901E-5</v>
       </c>
       <c r="T5" s="8">
-        <v>4.3090844192620901E-5</v>
+        <v>5.5217612501320798E-5</v>
       </c>
       <c r="U5" s="8">
-        <v>-6.2880685016332799E-6</v>
+        <v>-1.1855162827996501E-5</v>
       </c>
       <c r="V5" s="8">
-        <v>3.7063233851829799E-6</v>
+        <v>-2.5019864470842898E-7</v>
       </c>
       <c r="W5" s="8">
-        <v>1.46164008306629E-5</v>
+        <v>1.3362115106098899E-5</v>
       </c>
       <c r="X5" s="8">
-        <v>4.9556502837882102E-5</v>
+        <v>5.09529760875342E-5</v>
       </c>
       <c r="Y5" s="8">
-        <v>2.5089513554834998E-6</v>
+        <v>3.04745386287188E-6</v>
       </c>
       <c r="Z5" s="8">
-        <v>3.79991630210079E-6</v>
+        <v>4.2571390162228302E-6</v>
       </c>
       <c r="AA5" s="8">
-        <v>-3.8508510245791399E-8</v>
+        <v>-4.27724312176736E-8</v>
       </c>
       <c r="AB5" s="8">
-        <v>-3.1825181167266798E-6</v>
+        <v>-4.1990539914227599E-6</v>
       </c>
       <c r="AC5" s="8">
-        <v>-8.7565731745256198E-7</v>
+        <v>-8.8823586269393703E-7</v>
       </c>
       <c r="AD5" s="8">
-        <v>-6.3180303899050102E-6</v>
+        <v>-6.9770188772042104E-6</v>
       </c>
       <c r="AE5" s="8">
-        <v>-9.8121077930040301E-4</v>
+        <v>-1.1979880361858901E-3</v>
       </c>
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.25">
@@ -5257,94 +5257,94 @@
         <v>25</v>
       </c>
       <c r="B6" s="8">
-        <v>0.11481191545149699</v>
+        <v>8.6622452509374198E-2</v>
       </c>
       <c r="C6" s="8">
-        <v>-6.9108178710131996E-5</v>
+        <v>-8.1400804213283898E-5</v>
       </c>
       <c r="D6" s="8">
-        <v>-6.6940974705391993E-5</v>
+        <v>-7.0781895239614901E-5</v>
       </c>
       <c r="E6" s="8">
-        <v>1.06881146678558E-3</v>
+        <v>1.2982998800629699E-3</v>
       </c>
       <c r="F6" s="8">
-        <v>1.06535105216462E-3</v>
+        <v>1.2923295063619401E-3</v>
       </c>
       <c r="G6" s="8">
-        <v>2.3493264176958702E-3</v>
+        <v>2.7685921900003599E-3</v>
       </c>
       <c r="H6" s="8">
-        <v>1.06728626420667E-3</v>
+        <v>1.29597561384749E-3</v>
       </c>
       <c r="I6" s="8">
-        <v>1.06439887862101E-3</v>
+        <v>1.2941437470714899E-3</v>
       </c>
       <c r="J6" s="8">
-        <v>1.0586726749900199E-3</v>
+        <v>1.2850841153339799E-3</v>
       </c>
       <c r="K6" s="8">
-        <v>1.0510322067392699E-3</v>
+        <v>1.2769342224300099E-3</v>
       </c>
       <c r="L6" s="8">
-        <v>1.06819819643432E-3</v>
+        <v>1.29579702184705E-3</v>
       </c>
       <c r="M6" s="8">
-        <v>1.0737556292180299E-3</v>
+        <v>1.3049583145837401E-3</v>
       </c>
       <c r="N6" s="8">
-        <v>1.0636654886629199E-3</v>
+        <v>1.2902867839833501E-3</v>
       </c>
       <c r="O6" s="8">
-        <v>1.0643575540057299E-3</v>
+        <v>1.2925493656614001E-3</v>
       </c>
       <c r="P6" s="8">
-        <v>4.2682048551782797E-6</v>
+        <v>7.02354558046071E-6</v>
       </c>
       <c r="Q6" s="8">
-        <v>-1.1758409006427301E-4</v>
+        <v>-1.3232814886348501E-4</v>
       </c>
       <c r="R6" s="8">
-        <v>7.2368730689026899E-5</v>
+        <v>9.4873922142014601E-5</v>
       </c>
       <c r="S6" s="8">
-        <v>-9.4587375159042708E-6</v>
+        <v>-2.6096533285045499E-6</v>
       </c>
       <c r="T6" s="8">
-        <v>6.2817937381026402E-5</v>
+        <v>7.1240931926224804E-5</v>
       </c>
       <c r="U6" s="8">
-        <v>1.8615676280719099E-5</v>
+        <v>2.11530738951042E-5</v>
       </c>
       <c r="V6" s="8">
-        <v>4.1551083322488797E-5</v>
+        <v>4.4813463677083998E-5</v>
       </c>
       <c r="W6" s="8">
-        <v>4.9928669776200099E-5</v>
+        <v>6.0259661667862401E-5</v>
       </c>
       <c r="X6" s="8">
-        <v>1.08346350261165E-4</v>
+        <v>1.2557094002796701E-4</v>
       </c>
       <c r="Y6" s="8">
-        <v>1.20824045247566E-7</v>
+        <v>1.4649771969649601E-6</v>
       </c>
       <c r="Z6" s="8">
-        <v>4.0937818072402197E-6</v>
+        <v>5.2401916774154498E-6</v>
       </c>
       <c r="AA6" s="8">
-        <v>-3.5236699134234201E-8</v>
+        <v>-4.5394718343653701E-8</v>
       </c>
       <c r="AB6" s="8">
-        <v>-3.0401644107485802E-6</v>
+        <v>-4.1673943924848104E-6</v>
       </c>
       <c r="AC6" s="8">
-        <v>-5.6668883152103797E-7</v>
+        <v>-4.8435834400380895E-7</v>
       </c>
       <c r="AD6" s="8">
-        <v>-1.7288507969710001E-5</v>
+        <v>-1.70374440643536E-5</v>
       </c>
       <c r="AE6" s="8">
-        <v>-1.0252062148062601E-3</v>
+        <v>-1.28786286519915E-3</v>
       </c>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.25">
@@ -5352,94 +5352,94 @@
         <v>26</v>
       </c>
       <c r="B7" s="8">
-        <v>6.6516399285546896E-2</v>
+        <v>4.2575284947759001E-2</v>
       </c>
       <c r="C7" s="8">
-        <v>-1.0892821700986599E-4</v>
+        <v>-1.25125408959879E-4</v>
       </c>
       <c r="D7" s="8">
-        <v>-1.12820541444904E-4</v>
+        <v>-1.2473366291214101E-4</v>
       </c>
       <c r="E7" s="8">
-        <v>1.0772090686666301E-3</v>
+        <v>1.3094530308266801E-3</v>
       </c>
       <c r="F7" s="8">
-        <v>1.07129659042635E-3</v>
+        <v>1.3000347035909399E-3</v>
       </c>
       <c r="G7" s="8">
-        <v>1.06728626420667E-3</v>
+        <v>1.29597561384749E-3</v>
       </c>
       <c r="H7" s="8">
-        <v>2.2996228878462998E-3</v>
+        <v>2.7251852433988499E-3</v>
       </c>
       <c r="I7" s="8">
-        <v>1.0714023883662601E-3</v>
+        <v>1.3027014332871599E-3</v>
       </c>
       <c r="J7" s="8">
-        <v>1.0635623447113401E-3</v>
+        <v>1.29190877873002E-3</v>
       </c>
       <c r="K7" s="8">
-        <v>1.05792308198684E-3</v>
+        <v>1.28652734718206E-3</v>
       </c>
       <c r="L7" s="8">
-        <v>1.0716188194651E-3</v>
+        <v>1.30154538545347E-3</v>
       </c>
       <c r="M7" s="8">
-        <v>1.07711531534498E-3</v>
+        <v>1.3091991139447599E-3</v>
       </c>
       <c r="N7" s="8">
-        <v>1.0698258347399099E-3</v>
+        <v>1.29894915018373E-3</v>
       </c>
       <c r="O7" s="8">
-        <v>1.0693271426213101E-3</v>
+        <v>1.2993399505758199E-3</v>
       </c>
       <c r="P7" s="8">
-        <v>2.4612120449845999E-6</v>
+        <v>1.7633481725585801E-6</v>
       </c>
       <c r="Q7" s="8">
-        <v>-1.14024379385681E-4</v>
+        <v>-1.3592364033937401E-4</v>
       </c>
       <c r="R7" s="8">
-        <v>7.3084651599329405E-5</v>
+        <v>9.1749551588639203E-5</v>
       </c>
       <c r="S7" s="8">
-        <v>-2.0299650416265399E-6</v>
+        <v>9.31943054430196E-7</v>
       </c>
       <c r="T7" s="8">
-        <v>4.2571056359572699E-5</v>
+        <v>4.73286276623642E-5</v>
       </c>
       <c r="U7" s="8">
-        <v>2.1918353506485799E-5</v>
+        <v>2.6467123511162898E-5</v>
       </c>
       <c r="V7" s="8">
-        <v>1.8416293187680999E-5</v>
+        <v>2.4321109081398299E-5</v>
       </c>
       <c r="W7" s="8">
-        <v>3.08288208863186E-5</v>
+        <v>3.89303830469338E-5</v>
       </c>
       <c r="X7" s="8">
-        <v>6.3945139421550705E-5</v>
+        <v>7.6712856723919597E-5</v>
       </c>
       <c r="Y7" s="8">
-        <v>2.7648007721724699E-6</v>
+        <v>4.0837088237694404E-6</v>
       </c>
       <c r="Z7" s="8">
-        <v>3.0291747018516901E-6</v>
+        <v>3.2968869255359699E-6</v>
       </c>
       <c r="AA7" s="8">
-        <v>-2.8249601511346799E-8</v>
+        <v>-3.2034436076023703E-8</v>
       </c>
       <c r="AB7" s="8">
-        <v>-3.8748260008656702E-6</v>
+        <v>-4.49737515273092E-6</v>
       </c>
       <c r="AC7" s="8">
-        <v>-1.23893189632272E-6</v>
+        <v>-1.47788742481273E-6</v>
       </c>
       <c r="AD7" s="8">
-        <v>-5.3886009459041703E-6</v>
+        <v>-3.5177038467101101E-6</v>
       </c>
       <c r="AE7" s="8">
-        <v>-9.46868246233951E-4</v>
+        <v>-1.1607506186542299E-3</v>
       </c>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.25">
@@ -5447,94 +5447,94 @@
         <v>27</v>
       </c>
       <c r="B8" s="8">
-        <v>0.168611879419586</v>
+        <v>0.14894778892507099</v>
       </c>
       <c r="C8" s="8">
-        <v>-7.4275442937390003E-5</v>
+        <v>-8.5622027362546E-5</v>
       </c>
       <c r="D8" s="8">
-        <v>-8.3977193400694195E-5</v>
+        <v>-9.3338907756125307E-5</v>
       </c>
       <c r="E8" s="8">
-        <v>1.0722043200595999E-3</v>
+        <v>1.30494669899701E-3</v>
       </c>
       <c r="F8" s="8">
-        <v>1.0608049460324499E-3</v>
+        <v>1.28907040787262E-3</v>
       </c>
       <c r="G8" s="8">
-        <v>1.06439887862101E-3</v>
+        <v>1.2941437470714899E-3</v>
       </c>
       <c r="H8" s="8">
-        <v>1.0714023883662601E-3</v>
+        <v>1.3027014332871599E-3</v>
       </c>
       <c r="I8" s="8">
-        <v>2.3313161082928299E-3</v>
+        <v>2.7911699856796599E-3</v>
       </c>
       <c r="J8" s="8">
-        <v>1.0585565472686299E-3</v>
+        <v>1.28761235851701E-3</v>
       </c>
       <c r="K8" s="8">
-        <v>1.05544258104537E-3</v>
+        <v>1.2835759116033799E-3</v>
       </c>
       <c r="L8" s="8">
-        <v>1.0680527343293899E-3</v>
+        <v>1.2986781211494301E-3</v>
       </c>
       <c r="M8" s="8">
-        <v>1.07095912505945E-3</v>
+        <v>1.30359998232332E-3</v>
       </c>
       <c r="N8" s="8">
-        <v>1.0642940426958201E-3</v>
+        <v>1.29386872098737E-3</v>
       </c>
       <c r="O8" s="8">
-        <v>1.0631640325484599E-3</v>
+        <v>1.2932212755147701E-3</v>
       </c>
       <c r="P8" s="8">
-        <v>-6.8139856577085899E-6</v>
+        <v>-5.6837817329262897E-6</v>
       </c>
       <c r="Q8" s="8">
-        <v>-1.16354025419592E-4</v>
+        <v>-1.3652221546392999E-4</v>
       </c>
       <c r="R8" s="8">
-        <v>5.71666205316695E-5</v>
+        <v>7.8347330977951007E-5</v>
       </c>
       <c r="S8" s="8">
-        <v>2.2368717647622999E-5</v>
+        <v>3.5997478630352902E-5</v>
       </c>
       <c r="T8" s="8">
-        <v>3.9823040541493802E-5</v>
+        <v>4.56440488905475E-5</v>
       </c>
       <c r="U8" s="8">
-        <v>-6.7536704301496198E-6</v>
+        <v>-9.1603580059529405E-6</v>
       </c>
       <c r="V8" s="8">
-        <v>1.2937959954825E-5</v>
+        <v>1.3821006156554199E-5</v>
       </c>
       <c r="W8" s="8">
-        <v>1.8937014308333901E-6</v>
+        <v>4.8494212442156504E-7</v>
       </c>
       <c r="X8" s="8">
-        <v>5.0605238158786502E-5</v>
+        <v>6.1647497147890998E-5</v>
       </c>
       <c r="Y8" s="8">
-        <v>1.6978409151919101E-6</v>
+        <v>3.1059261802282901E-6</v>
       </c>
       <c r="Z8" s="8">
-        <v>4.0541324596371204E-6</v>
+        <v>5.2875855157522297E-6</v>
       </c>
       <c r="AA8" s="8">
-        <v>-4.1247948738422799E-8</v>
+        <v>-5.46574582925461E-8</v>
       </c>
       <c r="AB8" s="8">
-        <v>-5.1389272628331798E-6</v>
+        <v>-5.8298771570024597E-6</v>
       </c>
       <c r="AC8" s="8">
-        <v>-1.11565094254127E-6</v>
+        <v>-1.2703351873162499E-6</v>
       </c>
       <c r="AD8" s="8">
-        <v>1.9934169083980701E-6</v>
+        <v>8.1542893743484107E-6</v>
       </c>
       <c r="AE8" s="8">
-        <v>-9.4153885507760205E-4</v>
+        <v>-1.18797263085647E-3</v>
       </c>
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.25">
@@ -5542,94 +5542,94 @@
         <v>28</v>
       </c>
       <c r="B9" s="8">
-        <v>4.9914055548995903E-2</v>
+        <v>8.5719182047086003E-3</v>
       </c>
       <c r="C9" s="8">
-        <v>-8.2828945375216302E-5</v>
+        <v>-9.4587619678724195E-5</v>
       </c>
       <c r="D9" s="8">
-        <v>-8.4577966213917604E-5</v>
+        <v>-9.4309582073782804E-5</v>
       </c>
       <c r="E9" s="8">
-        <v>1.0664441415601401E-3</v>
+        <v>1.29621750655437E-3</v>
       </c>
       <c r="F9" s="8">
-        <v>1.0594521715121901E-3</v>
+        <v>1.2854996651937001E-3</v>
       </c>
       <c r="G9" s="8">
-        <v>1.0586726749900199E-3</v>
+        <v>1.2850841153339799E-3</v>
       </c>
       <c r="H9" s="8">
-        <v>1.0635623447113401E-3</v>
+        <v>1.29190877873002E-3</v>
       </c>
       <c r="I9" s="8">
-        <v>1.0585565472686299E-3</v>
+        <v>1.28761235851701E-3</v>
       </c>
       <c r="J9" s="8">
-        <v>2.0480274010865902E-3</v>
+        <v>2.44439763622546E-3</v>
       </c>
       <c r="K9" s="8">
-        <v>1.05312525633786E-3</v>
+        <v>1.2797589590688801E-3</v>
       </c>
       <c r="L9" s="8">
-        <v>1.0658135325970299E-3</v>
+        <v>1.29370124832082E-3</v>
       </c>
       <c r="M9" s="8">
-        <v>1.06704525412538E-3</v>
+        <v>1.2966647950291401E-3</v>
       </c>
       <c r="N9" s="8">
-        <v>1.06147314880007E-3</v>
+        <v>1.28855726345915E-3</v>
       </c>
       <c r="O9" s="8">
-        <v>1.05490432450641E-3</v>
+        <v>1.2815773325711901E-3</v>
       </c>
       <c r="P9" s="8">
-        <v>3.3651608958302601E-6</v>
+        <v>2.2048112825075198E-6</v>
       </c>
       <c r="Q9" s="8">
-        <v>-9.2877503285804903E-5</v>
+        <v>-1.02328471792849E-4</v>
       </c>
       <c r="R9" s="8">
-        <v>7.8412020494100998E-5</v>
+        <v>9.7611343526744199E-5</v>
       </c>
       <c r="S9" s="8">
-        <v>1.32228971508395E-5</v>
+        <v>1.9209982023377301E-5</v>
       </c>
       <c r="T9" s="8">
-        <v>3.7981668450014302E-5</v>
+        <v>4.5609701434661802E-5</v>
       </c>
       <c r="U9" s="8">
-        <v>5.0968749236754097E-6</v>
+        <v>6.5073196545890401E-6</v>
       </c>
       <c r="V9" s="8">
-        <v>7.2767229358422396E-6</v>
+        <v>6.7853092412037403E-6</v>
       </c>
       <c r="W9" s="8">
-        <v>3.3932315697247498E-6</v>
+        <v>5.7886321222854198E-6</v>
       </c>
       <c r="X9" s="8">
-        <v>2.5266040376806101E-5</v>
+        <v>2.7925954255685498E-5</v>
       </c>
       <c r="Y9" s="8">
-        <v>2.9313715455486101E-6</v>
+        <v>4.1408426350238101E-6</v>
       </c>
       <c r="Z9" s="8">
-        <v>5.2899874033586298E-6</v>
+        <v>5.85062025927404E-6</v>
       </c>
       <c r="AA9" s="8">
-        <v>-6.1720025210646596E-8</v>
+        <v>-7.0482077364380495E-8</v>
       </c>
       <c r="AB9" s="8">
-        <v>-5.0673218306440097E-6</v>
+        <v>-5.8203358262003099E-6</v>
       </c>
       <c r="AC9" s="8">
-        <v>-2.3905009615432402E-6</v>
+        <v>-2.8497022323475301E-6</v>
       </c>
       <c r="AD9" s="8">
-        <v>9.8637187167365297E-6</v>
+        <v>1.39895452850547E-5</v>
       </c>
       <c r="AE9" s="8">
-        <v>-9.1321204151468096E-4</v>
+        <v>-1.1193177506530899E-3</v>
       </c>
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.25">
@@ -5637,94 +5637,94 @@
         <v>29</v>
       </c>
       <c r="B10" s="8">
-        <v>0.111545811158379</v>
+        <v>6.7588677234638794E-2</v>
       </c>
       <c r="C10" s="8">
-        <v>-6.18713044141723E-5</v>
+        <v>-7.4270576203027097E-5</v>
       </c>
       <c r="D10" s="8">
-        <v>-4.3207434944475701E-5</v>
+        <v>-4.4411074543662501E-5</v>
       </c>
       <c r="E10" s="8">
-        <v>1.0594285005420701E-3</v>
+        <v>1.2886934092175401E-3</v>
       </c>
       <c r="F10" s="8">
-        <v>1.0566308302990401E-3</v>
+        <v>1.2837201742287401E-3</v>
       </c>
       <c r="G10" s="8">
-        <v>1.0510322067392699E-3</v>
+        <v>1.2769342224300099E-3</v>
       </c>
       <c r="H10" s="8">
-        <v>1.05792308198684E-3</v>
+        <v>1.28652734718206E-3</v>
       </c>
       <c r="I10" s="8">
-        <v>1.05544258104537E-3</v>
+        <v>1.2835759116033799E-3</v>
       </c>
       <c r="J10" s="8">
-        <v>1.05312525633786E-3</v>
+        <v>1.2797589590688801E-3</v>
       </c>
       <c r="K10" s="8">
-        <v>1.7700452766392001E-3</v>
+        <v>2.1131102698408498E-3</v>
       </c>
       <c r="L10" s="8">
-        <v>1.06460003156113E-3</v>
+        <v>1.29251967562771E-3</v>
       </c>
       <c r="M10" s="8">
-        <v>1.06133899408222E-3</v>
+        <v>1.29063952169142E-3</v>
       </c>
       <c r="N10" s="8">
-        <v>1.0620796379857201E-3</v>
+        <v>1.29081836736936E-3</v>
       </c>
       <c r="O10" s="8">
-        <v>1.049480629283E-3</v>
+        <v>1.27566869938552E-3</v>
       </c>
       <c r="P10" s="8">
-        <v>4.1089378182980204E-6</v>
+        <v>6.6994596507262299E-6</v>
       </c>
       <c r="Q10" s="8">
-        <v>-1.05048461668122E-4</v>
+        <v>-1.23213370572212E-4</v>
       </c>
       <c r="R10" s="8">
-        <v>7.3434985859314203E-5</v>
+        <v>9.1650821502225707E-5</v>
       </c>
       <c r="S10" s="8">
-        <v>1.56302883109403E-6</v>
+        <v>9.1357707325113E-7</v>
       </c>
       <c r="T10" s="8">
-        <v>4.2835056594919702E-5</v>
+        <v>5.1540039121004997E-5</v>
       </c>
       <c r="U10" s="8">
-        <v>1.42429998842197E-6</v>
+        <v>7.29068227473261E-7</v>
       </c>
       <c r="V10" s="8">
-        <v>-6.6221732725682299E-6</v>
+        <v>-1.0732893964541201E-5</v>
       </c>
       <c r="W10" s="8">
-        <v>-1.02458102563469E-5</v>
+        <v>-1.1850561039834101E-5</v>
       </c>
       <c r="X10" s="8">
-        <v>-2.4041000478841299E-6</v>
+        <v>-3.4716528760721099E-6</v>
       </c>
       <c r="Y10" s="8">
-        <v>4.18596249083941E-6</v>
+        <v>5.7973963116998801E-6</v>
       </c>
       <c r="Z10" s="8">
-        <v>5.1717440034410497E-6</v>
+        <v>5.9177157680461901E-6</v>
       </c>
       <c r="AA10" s="8">
-        <v>-6.12287384370235E-8</v>
+        <v>-7.1322725498930402E-8</v>
       </c>
       <c r="AB10" s="8">
-        <v>-4.2648896152328296E-6</v>
+        <v>-5.1533565550716299E-6</v>
       </c>
       <c r="AC10" s="8">
-        <v>-1.3962082477912201E-6</v>
+        <v>-1.5945129661537801E-6</v>
       </c>
       <c r="AD10" s="8">
-        <v>-2.0619336032878901E-6</v>
+        <v>1.3448601534204401E-6</v>
       </c>
       <c r="AE10" s="8">
-        <v>-9.7214891034458199E-4</v>
+        <v>-1.19392147305834E-3</v>
       </c>
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.25">
@@ -5732,94 +5732,94 @@
         <v>30</v>
       </c>
       <c r="B11" s="8">
-        <v>0.104748569415406</v>
+        <v>6.0921118677200098E-2</v>
       </c>
       <c r="C11" s="8">
-        <v>-8.1341707694572899E-5</v>
+        <v>-9.2852913357332201E-5</v>
       </c>
       <c r="D11" s="8">
-        <v>-5.3063497433085801E-5</v>
+        <v>-5.4190283143972801E-5</v>
       </c>
       <c r="E11" s="8">
-        <v>1.07590161658082E-3</v>
+        <v>1.3066161794066499E-3</v>
       </c>
       <c r="F11" s="8">
-        <v>1.06876690399174E-3</v>
+        <v>1.2961002392839699E-3</v>
       </c>
       <c r="G11" s="8">
-        <v>1.06819819643432E-3</v>
+        <v>1.29579702184705E-3</v>
       </c>
       <c r="H11" s="8">
-        <v>1.0716188194651E-3</v>
+        <v>1.30154538545347E-3</v>
       </c>
       <c r="I11" s="8">
-        <v>1.0680527343293899E-3</v>
+        <v>1.2986781211494301E-3</v>
       </c>
       <c r="J11" s="8">
-        <v>1.0658135325970299E-3</v>
+        <v>1.29370124832082E-3</v>
       </c>
       <c r="K11" s="8">
-        <v>1.06460003156113E-3</v>
+        <v>1.29251967562771E-3</v>
       </c>
       <c r="L11" s="8">
-        <v>2.2027979163011702E-3</v>
+        <v>2.59413864167336E-3</v>
       </c>
       <c r="M11" s="8">
-        <v>1.0770131841103599E-3</v>
+        <v>1.3084285592283799E-3</v>
       </c>
       <c r="N11" s="8">
-        <v>1.074265617153E-3</v>
+        <v>1.3029770389990599E-3</v>
       </c>
       <c r="O11" s="8">
-        <v>1.0646054133561099E-3</v>
+        <v>1.29267062937917E-3</v>
       </c>
       <c r="P11" s="8">
-        <v>2.2844992792592602E-6</v>
+        <v>1.4424023571250501E-7</v>
       </c>
       <c r="Q11" s="8">
-        <v>-1.09352644459758E-4</v>
+        <v>-1.2748629259561799E-4</v>
       </c>
       <c r="R11" s="8">
-        <v>8.4281749864339705E-5</v>
+        <v>1.11274825643679E-4</v>
       </c>
       <c r="S11" s="8">
-        <v>1.9511115008202899E-5</v>
+        <v>2.7147849673577502E-5</v>
       </c>
       <c r="T11" s="8">
-        <v>5.7067095962278198E-5</v>
+        <v>6.7701892225327306E-5</v>
       </c>
       <c r="U11" s="8">
-        <v>1.4664818340628501E-5</v>
+        <v>1.9143069186142902E-5</v>
       </c>
       <c r="V11" s="8">
-        <v>2.3388040519728401E-5</v>
+        <v>2.56481346570062E-5</v>
       </c>
       <c r="W11" s="8">
-        <v>2.9969985197550901E-5</v>
+        <v>3.7107748931661102E-5</v>
       </c>
       <c r="X11" s="8">
-        <v>5.8356956344715599E-5</v>
+        <v>6.7646001507972196E-5</v>
       </c>
       <c r="Y11" s="8">
-        <v>4.6693648620851297E-6</v>
+        <v>6.3004410475683398E-6</v>
       </c>
       <c r="Z11" s="8">
-        <v>3.3546060489813401E-6</v>
+        <v>3.8526359116769196E-6</v>
       </c>
       <c r="AA11" s="8">
-        <v>-4.4709434046324701E-8</v>
+        <v>-4.9945772065316302E-8</v>
       </c>
       <c r="AB11" s="8">
-        <v>-1.9645808338728002E-6</v>
+        <v>-1.4690678157870599E-6</v>
       </c>
       <c r="AC11" s="8">
-        <v>-1.8362383144126799E-6</v>
+        <v>-2.1073328005879299E-6</v>
       </c>
       <c r="AD11" s="8">
-        <v>3.0558602225527002E-6</v>
+        <v>1.0200241825056899E-5</v>
       </c>
       <c r="AE11" s="8">
-        <v>-9.7367395144997305E-4</v>
+        <v>-1.21760671370202E-3</v>
       </c>
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.25">
@@ -5827,94 +5827,94 @@
         <v>31</v>
       </c>
       <c r="B12" s="8">
-        <v>0.21110987410382601</v>
+        <v>0.148302382075158</v>
       </c>
       <c r="C12" s="8">
-        <v>-8.5239585287131899E-5</v>
+        <v>-9.7723831375078806E-5</v>
       </c>
       <c r="D12" s="8">
-        <v>-8.0749002867724906E-5</v>
+        <v>-9.2512056332152902E-5</v>
       </c>
       <c r="E12" s="8">
-        <v>1.0845393177464299E-3</v>
+        <v>1.3189121274853801E-3</v>
       </c>
       <c r="F12" s="8">
-        <v>1.0695018880522199E-3</v>
+        <v>1.2981937161402001E-3</v>
       </c>
       <c r="G12" s="8">
-        <v>1.0737556292180299E-3</v>
+        <v>1.3049583145837401E-3</v>
       </c>
       <c r="H12" s="8">
-        <v>1.07711531534498E-3</v>
+        <v>1.3091991139447599E-3</v>
       </c>
       <c r="I12" s="8">
-        <v>1.07095912505945E-3</v>
+        <v>1.30359998232332E-3</v>
       </c>
       <c r="J12" s="8">
-        <v>1.06704525412538E-3</v>
+        <v>1.2966647950291401E-3</v>
       </c>
       <c r="K12" s="8">
-        <v>1.06133899408222E-3</v>
+        <v>1.29063952169142E-3</v>
       </c>
       <c r="L12" s="8">
-        <v>1.0770131841103599E-3</v>
+        <v>1.3084285592283799E-3</v>
       </c>
       <c r="M12" s="8">
-        <v>2.5309394696671102E-3</v>
+        <v>3.0335787278375301E-3</v>
       </c>
       <c r="N12" s="8">
-        <v>1.0741241837760899E-3</v>
+        <v>1.3036665411146899E-3</v>
       </c>
       <c r="O12" s="8">
-        <v>1.07244876463635E-3</v>
+        <v>1.3040664415036301E-3</v>
       </c>
       <c r="P12" s="8">
-        <v>1.5792869687528399E-6</v>
+        <v>2.3862405777066701E-6</v>
       </c>
       <c r="Q12" s="8">
-        <v>-1.19271212132121E-4</v>
+        <v>-1.3852243966605299E-4</v>
       </c>
       <c r="R12" s="8">
-        <v>6.4629497977963099E-5</v>
+        <v>8.74754242440102E-5</v>
       </c>
       <c r="S12" s="8">
-        <v>-7.3371464742691503E-7</v>
+        <v>6.6818445092609104E-6</v>
       </c>
       <c r="T12" s="8">
-        <v>4.6379169406659901E-5</v>
+        <v>6.1627571517514302E-5</v>
       </c>
       <c r="U12" s="8">
-        <v>-1.9755155230674201E-5</v>
+        <v>-2.5422105778243801E-5</v>
       </c>
       <c r="V12" s="8">
-        <v>-2.7764603458460301E-6</v>
+        <v>-3.45555222942537E-6</v>
       </c>
       <c r="W12" s="8">
-        <v>2.1540222536876999E-6</v>
+        <v>3.3956283051879098E-6</v>
       </c>
       <c r="X12" s="8">
-        <v>5.8464918096278697E-5</v>
+        <v>7.0502876225044396E-5</v>
       </c>
       <c r="Y12" s="8">
-        <v>3.6520359783675901E-6</v>
+        <v>4.8920983458875596E-6</v>
       </c>
       <c r="Z12" s="8">
-        <v>3.82789490967876E-6</v>
+        <v>4.9961814672834201E-6</v>
       </c>
       <c r="AA12" s="8">
-        <v>-4.2882555618993997E-8</v>
+        <v>-5.4976619710327598E-8</v>
       </c>
       <c r="AB12" s="8">
-        <v>-3.4770945725069898E-6</v>
+        <v>-3.4019366937590902E-6</v>
       </c>
       <c r="AC12" s="8">
-        <v>-2.1280198036761101E-7</v>
+        <v>-1.6643838646635601E-7</v>
       </c>
       <c r="AD12" s="8">
-        <v>-8.67647462065072E-6</v>
+        <v>-7.4381384278055399E-6</v>
       </c>
       <c r="AE12" s="8">
-        <v>-1.01258741841183E-3</v>
+        <v>-1.2731586149253901E-3</v>
       </c>
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.25">
@@ -5922,94 +5922,94 @@
         <v>32</v>
       </c>
       <c r="B13" s="8">
-        <v>2.0268142650692801E-2</v>
+        <v>-2.0758980700733801E-2</v>
       </c>
       <c r="C13" s="8">
-        <v>-7.93702801573131E-5</v>
+        <v>-8.9147371597648803E-5</v>
       </c>
       <c r="D13" s="8">
-        <v>-4.0465518631359199E-5</v>
+        <v>-4.3534145061445298E-5</v>
       </c>
       <c r="E13" s="8">
-        <v>1.0720587591444E-3</v>
+        <v>1.3026680835184199E-3</v>
       </c>
       <c r="F13" s="8">
-        <v>1.0666111982737599E-3</v>
+        <v>1.2936548458679601E-3</v>
       </c>
       <c r="G13" s="8">
-        <v>1.0636654886629199E-3</v>
+        <v>1.2902867839833501E-3</v>
       </c>
       <c r="H13" s="8">
-        <v>1.0698258347399099E-3</v>
+        <v>1.29894915018373E-3</v>
       </c>
       <c r="I13" s="8">
-        <v>1.0642940426958201E-3</v>
+        <v>1.29386872098737E-3</v>
       </c>
       <c r="J13" s="8">
-        <v>1.06147314880007E-3</v>
+        <v>1.28855726345915E-3</v>
       </c>
       <c r="K13" s="8">
-        <v>1.0620796379857201E-3</v>
+        <v>1.29081836736936E-3</v>
       </c>
       <c r="L13" s="8">
-        <v>1.074265617153E-3</v>
+        <v>1.3029770389990599E-3</v>
       </c>
       <c r="M13" s="8">
-        <v>1.0741241837760899E-3</v>
+        <v>1.3036665411146899E-3</v>
       </c>
       <c r="N13" s="8">
-        <v>2.1107633397341899E-3</v>
+        <v>2.5302177579442E-3</v>
       </c>
       <c r="O13" s="8">
-        <v>1.06363211766726E-3</v>
+        <v>1.2912300793394E-3</v>
       </c>
       <c r="P13" s="8">
-        <v>4.6035507731302401E-6</v>
+        <v>7.4036241391915499E-6</v>
       </c>
       <c r="Q13" s="8">
-        <v>-1.1631228352142E-4</v>
+        <v>-1.3606083045981601E-4</v>
       </c>
       <c r="R13" s="8">
-        <v>4.65785004082273E-5</v>
+        <v>5.9030668521752803E-5</v>
       </c>
       <c r="S13" s="8">
-        <v>2.9332047475643201E-6</v>
+        <v>-1.16746316912147E-6</v>
       </c>
       <c r="T13" s="8">
-        <v>4.1272600779181599E-5</v>
+        <v>4.5440106257838403E-5</v>
       </c>
       <c r="U13" s="8">
-        <v>-3.3705999597703201E-6</v>
+        <v>-4.5794108509856701E-6</v>
       </c>
       <c r="V13" s="8">
-        <v>6.37494368668692E-7</v>
+        <v>-2.83720642714685E-7</v>
       </c>
       <c r="W13" s="8">
-        <v>-1.2536478976609201E-6</v>
+        <v>-1.26631378195263E-6</v>
       </c>
       <c r="X13" s="8">
-        <v>3.8916144388137498E-5</v>
+        <v>4.3319296740491001E-5</v>
       </c>
       <c r="Y13" s="8">
-        <v>4.75101959656989E-6</v>
+        <v>5.4380420427733802E-6</v>
       </c>
       <c r="Z13" s="8">
-        <v>2.02507699844905E-6</v>
+        <v>1.47030293991179E-6</v>
       </c>
       <c r="AA13" s="8">
-        <v>-3.5302999281871103E-8</v>
+        <v>-3.3706719453285902E-8</v>
       </c>
       <c r="AB13" s="8">
-        <v>-2.3712226015979299E-6</v>
+        <v>-2.6203158692545499E-6</v>
       </c>
       <c r="AC13" s="8">
-        <v>-1.14107054237594E-6</v>
+        <v>-1.32505428609314E-6</v>
       </c>
       <c r="AD13" s="8">
-        <v>-6.1454669693396202E-6</v>
+        <v>-4.9611933504497303E-6</v>
       </c>
       <c r="AE13" s="8">
-        <v>-9.3059806897005605E-4</v>
+        <v>-1.1148422422248799E-3</v>
       </c>
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.25">
@@ -6017,94 +6017,94 @@
         <v>33</v>
       </c>
       <c r="B14" s="8">
-        <v>-7.1929886686078207E-2</v>
+        <v>-9.82459964541533E-2</v>
       </c>
       <c r="C14" s="8">
-        <v>-8.2836745822835502E-5</v>
+        <v>-9.6704789632620197E-5</v>
       </c>
       <c r="D14" s="8">
-        <v>-1.15661976859249E-4</v>
+        <v>-1.3578467718021399E-4</v>
       </c>
       <c r="E14" s="8">
-        <v>1.07241075551539E-3</v>
+        <v>1.3041465695219901E-3</v>
       </c>
       <c r="F14" s="8">
-        <v>1.0624004163837699E-3</v>
+        <v>1.28832358926761E-3</v>
       </c>
       <c r="G14" s="8">
-        <v>1.0643575540057299E-3</v>
+        <v>1.2925493656614001E-3</v>
       </c>
       <c r="H14" s="8">
-        <v>1.0693271426213101E-3</v>
+        <v>1.2993399505758199E-3</v>
       </c>
       <c r="I14" s="8">
-        <v>1.0631640325484599E-3</v>
+        <v>1.2932212755147701E-3</v>
       </c>
       <c r="J14" s="8">
-        <v>1.05490432450641E-3</v>
+        <v>1.2815773325711901E-3</v>
       </c>
       <c r="K14" s="8">
-        <v>1.049480629283E-3</v>
+        <v>1.27566869938552E-3</v>
       </c>
       <c r="L14" s="8">
-        <v>1.0646054133561099E-3</v>
+        <v>1.29267062937917E-3</v>
       </c>
       <c r="M14" s="8">
-        <v>1.07244876463635E-3</v>
+        <v>1.3040664415036301E-3</v>
       </c>
       <c r="N14" s="8">
-        <v>1.06363211766726E-3</v>
+        <v>1.2912300793394E-3</v>
       </c>
       <c r="O14" s="8">
-        <v>2.5194527768404198E-3</v>
+        <v>3.0787666932401898E-3</v>
       </c>
       <c r="P14" s="8">
-        <v>-2.2718046621029501E-5</v>
+        <v>-2.5543163594054799E-5</v>
       </c>
       <c r="Q14" s="8">
-        <v>-1.19892018771152E-4</v>
+        <v>-1.3085217877330401E-4</v>
       </c>
       <c r="R14" s="8">
-        <v>2.7195167544381301E-7</v>
+        <v>8.8456103967881892E-6</v>
       </c>
       <c r="S14" s="8">
-        <v>-2.9584728819421901E-5</v>
+        <v>-3.6702645094146201E-5</v>
       </c>
       <c r="T14" s="8">
-        <v>4.1433272052927503E-5</v>
+        <v>4.0131854807533302E-5</v>
       </c>
       <c r="U14" s="8">
-        <v>1.67683286339425E-5</v>
+        <v>2.0148854559633401E-5</v>
       </c>
       <c r="V14" s="8">
-        <v>1.04724336218278E-5</v>
+        <v>9.9248871066617208E-6</v>
       </c>
       <c r="W14" s="8">
-        <v>2.01425835441656E-5</v>
+        <v>2.5526520505940499E-5</v>
       </c>
       <c r="X14" s="8">
-        <v>7.6898295914402893E-5</v>
+        <v>9.1333861271211605E-5</v>
       </c>
       <c r="Y14" s="8">
-        <v>4.4315271554711699E-6</v>
+        <v>5.73017255860853E-6</v>
       </c>
       <c r="Z14" s="8">
-        <v>2.4645913414325602E-6</v>
+        <v>3.00894646192022E-6</v>
       </c>
       <c r="AA14" s="8">
-        <v>-2.4497648314825999E-8</v>
+        <v>-3.2335581412306199E-8</v>
       </c>
       <c r="AB14" s="8">
-        <v>-7.2015279948186899E-7</v>
+        <v>-1.4195240517000101E-6</v>
       </c>
       <c r="AC14" s="8">
-        <v>-6.5869545494226599E-7</v>
+        <v>-4.2340734423215199E-7</v>
       </c>
       <c r="AD14" s="8">
-        <v>1.1550375042323801E-5</v>
+        <v>1.40510150203083E-5</v>
       </c>
       <c r="AE14" s="8">
-        <v>-9.9301734847927702E-4</v>
+        <v>-1.2355023172130101E-3</v>
       </c>
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.25">
@@ -6112,94 +6112,94 @@
         <v>34</v>
       </c>
       <c r="B15" s="8">
-        <v>0.171051515607232</v>
+        <v>0.15445920579865899</v>
       </c>
       <c r="C15" s="8">
-        <v>-5.5035653519916099E-6</v>
+        <v>-3.35944138396503E-6</v>
       </c>
       <c r="D15" s="8">
-        <v>2.12307898133759E-6</v>
+        <v>3.2340782466820501E-6</v>
       </c>
       <c r="E15" s="8">
-        <v>-3.9711514492125398E-6</v>
+        <v>-2.75340398856397E-6</v>
       </c>
       <c r="F15" s="8">
-        <v>-4.4443045675280199E-7</v>
+        <v>-2.71926192311181E-6</v>
       </c>
       <c r="G15" s="8">
-        <v>4.2682048551782797E-6</v>
+        <v>7.02354558046071E-6</v>
       </c>
       <c r="H15" s="8">
-        <v>2.4612120449845999E-6</v>
+        <v>1.7633481725585801E-6</v>
       </c>
       <c r="I15" s="8">
-        <v>-6.8139856577085899E-6</v>
+        <v>-5.6837817329262897E-6</v>
       </c>
       <c r="J15" s="8">
-        <v>3.3651608958302601E-6</v>
+        <v>2.2048112825075198E-6</v>
       </c>
       <c r="K15" s="8">
-        <v>4.1089378182980204E-6</v>
+        <v>6.6994596507262299E-6</v>
       </c>
       <c r="L15" s="8">
-        <v>2.2844992792592602E-6</v>
+        <v>1.4424023571250501E-7</v>
       </c>
       <c r="M15" s="8">
-        <v>1.5792869687528399E-6</v>
+        <v>2.3862405777066701E-6</v>
       </c>
       <c r="N15" s="8">
-        <v>4.6035507731302401E-6</v>
+        <v>7.4036241391915499E-6</v>
       </c>
       <c r="O15" s="8">
-        <v>-2.2718046621029501E-5</v>
+        <v>-2.5543163594054799E-5</v>
       </c>
       <c r="P15" s="8">
-        <v>4.7797723882584E-4</v>
+        <v>5.5139287901010802E-4</v>
       </c>
       <c r="Q15" s="8">
-        <v>-9.2274239526330093E-6</v>
+        <v>-1.22243367497054E-5</v>
       </c>
       <c r="R15" s="8">
-        <v>8.4301794162856006E-5</v>
+        <v>1.00926604144321E-4</v>
       </c>
       <c r="S15" s="8">
-        <v>3.8754489998824402E-5</v>
+        <v>4.5175697167543002E-5</v>
       </c>
       <c r="T15" s="8">
-        <v>-9.7531415604059697E-5</v>
+        <v>-1.1116496459388299E-4</v>
       </c>
       <c r="U15" s="8">
-        <v>-7.8454978079788295E-6</v>
+        <v>-7.9562596322946299E-6</v>
       </c>
       <c r="V15" s="8">
-        <v>2.4290310032538301E-5</v>
+        <v>2.6046774834424301E-5</v>
       </c>
       <c r="W15" s="8">
-        <v>7.0165346316770796E-5</v>
+        <v>7.9411022508725301E-5</v>
       </c>
       <c r="X15" s="8">
-        <v>1.3157493114683699E-4</v>
+        <v>1.50806604864911E-4</v>
       </c>
       <c r="Y15" s="8">
-        <v>3.7917113160447001E-6</v>
+        <v>4.0475815549796298E-6</v>
       </c>
       <c r="Z15" s="8">
-        <v>1.1125106328094E-5</v>
+        <v>1.3188581899491499E-5</v>
       </c>
       <c r="AA15" s="8">
-        <v>-1.3599779644869E-7</v>
+        <v>-1.61178425341575E-7</v>
       </c>
       <c r="AB15" s="8">
-        <v>-3.6190391913122701E-7</v>
+        <v>1.08003792716457E-7</v>
       </c>
       <c r="AC15" s="8">
-        <v>1.3826337980897599E-7</v>
+        <v>4.0612989300254797E-8</v>
       </c>
       <c r="AD15" s="8">
-        <v>1.9509696246996999E-5</v>
+        <v>2.2312841529307998E-5</v>
       </c>
       <c r="AE15" s="8">
-        <v>-6.2722640802023505E-4</v>
+        <v>-7.24661402033632E-4</v>
       </c>
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.25">
@@ -6207,94 +6207,94 @@
         <v>51</v>
       </c>
       <c r="B16" s="8">
-        <v>-0.38224181014282299</v>
+        <v>-0.38246461430940898</v>
       </c>
       <c r="C16" s="8">
-        <v>1.6792741570474201E-5</v>
+        <v>2.6694639089029299E-5</v>
       </c>
       <c r="D16" s="8">
-        <v>7.3934289024519E-5</v>
+        <v>9.1837794212754694E-5</v>
       </c>
       <c r="E16" s="8">
-        <v>-1.1880154133844001E-4</v>
+        <v>-1.40446383635702E-4</v>
       </c>
       <c r="F16" s="8">
-        <v>-1.1342860769951601E-4</v>
+        <v>-1.27013501833536E-4</v>
       </c>
       <c r="G16" s="8">
-        <v>-1.1758409006427301E-4</v>
+        <v>-1.3232814886348501E-4</v>
       </c>
       <c r="H16" s="8">
-        <v>-1.14024379385681E-4</v>
+        <v>-1.3592364033937401E-4</v>
       </c>
       <c r="I16" s="8">
-        <v>-1.16354025419592E-4</v>
+        <v>-1.3652221546392999E-4</v>
       </c>
       <c r="J16" s="8">
-        <v>-9.2877503285804903E-5</v>
+        <v>-1.02328471792849E-4</v>
       </c>
       <c r="K16" s="8">
-        <v>-1.05048461668122E-4</v>
+        <v>-1.23213370572212E-4</v>
       </c>
       <c r="L16" s="8">
-        <v>-1.09352644459758E-4</v>
+        <v>-1.2748629259561799E-4</v>
       </c>
       <c r="M16" s="8">
-        <v>-1.19271212132121E-4</v>
+        <v>-1.3852243966605299E-4</v>
       </c>
       <c r="N16" s="8">
-        <v>-1.1631228352142E-4</v>
+        <v>-1.3606083045981601E-4</v>
       </c>
       <c r="O16" s="8">
-        <v>-1.19892018771152E-4</v>
+        <v>-1.3085217877330401E-4</v>
       </c>
       <c r="P16" s="8">
-        <v>-9.2274239526330093E-6</v>
+        <v>-1.22243367497054E-5</v>
       </c>
       <c r="Q16" s="8">
-        <v>6.9936253419591095E-4</v>
+        <v>8.526481737517E-4</v>
       </c>
       <c r="R16" s="8">
-        <v>3.5489149242826497E-5</v>
+        <v>4.4593789898424797E-5</v>
       </c>
       <c r="S16" s="8">
-        <v>8.0031535455390605E-5</v>
+        <v>9.0764600119650697E-5</v>
       </c>
       <c r="T16" s="8">
-        <v>-5.5940677296196703E-5</v>
+        <v>-6.21584990709412E-5</v>
       </c>
       <c r="U16" s="8">
-        <v>-5.9407540007460198E-5</v>
+        <v>-7.0927252510696604E-5</v>
       </c>
       <c r="V16" s="8">
-        <v>-1.0782803402241E-4</v>
+        <v>-1.2588526729479999E-4</v>
       </c>
       <c r="W16" s="8">
-        <v>-1.4840980140309399E-4</v>
+        <v>-1.72374252316291E-4</v>
       </c>
       <c r="X16" s="8">
-        <v>-1.7070011691610099E-4</v>
+        <v>-1.95533003974164E-4</v>
       </c>
       <c r="Y16" s="8">
-        <v>4.0793567108096299E-8</v>
+        <v>8.9358621184339395E-7</v>
       </c>
       <c r="Z16" s="8">
-        <v>-5.2504939103552898E-6</v>
+        <v>-6.1393077011780697E-6</v>
       </c>
       <c r="AA16" s="8">
-        <v>1.35152459553038E-8</v>
+        <v>1.67171893853106E-8</v>
       </c>
       <c r="AB16" s="8">
-        <v>4.32723605173755E-6</v>
+        <v>6.0791082894465997E-6</v>
       </c>
       <c r="AC16" s="8">
-        <v>-2.0474639855476699E-6</v>
+        <v>-2.5556461319865701E-6</v>
       </c>
       <c r="AD16" s="8">
-        <v>1.4837851068342901E-5</v>
+        <v>2.01561690940573E-5</v>
       </c>
       <c r="AE16" s="8">
-        <v>-1.01398648324365E-4</v>
+        <v>-1.7533681058695E-4</v>
       </c>
     </row>
     <row r="17" spans="1:31" x14ac:dyDescent="0.25">
@@ -6302,94 +6302,94 @@
         <v>52</v>
       </c>
       <c r="B17" s="8">
-        <v>0.18626231644498101</v>
+        <v>0.16876760694648901</v>
       </c>
       <c r="C17" s="8">
-        <v>-2.8762216933361899E-5</v>
+        <v>-3.4739667835109602E-5</v>
       </c>
       <c r="D17" s="8">
-        <v>-7.4290236969621802E-6</v>
+        <v>-4.24053282701221E-6</v>
       </c>
       <c r="E17" s="8">
-        <v>5.6169581710956697E-5</v>
+        <v>6.8412831530912995E-5</v>
       </c>
       <c r="F17" s="8">
-        <v>6.5990720673164303E-5</v>
+        <v>8.7608382022937703E-5</v>
       </c>
       <c r="G17" s="8">
-        <v>7.2368730689026899E-5</v>
+        <v>9.4873922142014601E-5</v>
       </c>
       <c r="H17" s="8">
-        <v>7.3084651599329405E-5</v>
+        <v>9.1749551588639203E-5</v>
       </c>
       <c r="I17" s="8">
-        <v>5.71666205316695E-5</v>
+        <v>7.8347330977951007E-5</v>
       </c>
       <c r="J17" s="8">
-        <v>7.8412020494100998E-5</v>
+        <v>9.7611343526744199E-5</v>
       </c>
       <c r="K17" s="8">
-        <v>7.3434985859314203E-5</v>
+        <v>9.1650821502225707E-5</v>
       </c>
       <c r="L17" s="8">
-        <v>8.4281749864339705E-5</v>
+        <v>1.11274825643679E-4</v>
       </c>
       <c r="M17" s="8">
-        <v>6.4629497977963099E-5</v>
+        <v>8.74754242440102E-5</v>
       </c>
       <c r="N17" s="8">
-        <v>4.65785004082273E-5</v>
+        <v>5.9030668521752803E-5</v>
       </c>
       <c r="O17" s="8">
-        <v>2.7195167544381301E-7</v>
+        <v>8.8456103967881892E-6</v>
       </c>
       <c r="P17" s="8">
-        <v>8.4301794162856006E-5</v>
+        <v>1.00926604144321E-4</v>
       </c>
       <c r="Q17" s="8">
-        <v>3.5489149242826497E-5</v>
+        <v>4.4593789898424797E-5</v>
       </c>
       <c r="R17" s="8">
-        <v>1.06877176172172E-3</v>
+        <v>1.27141641491935E-3</v>
       </c>
       <c r="S17" s="8">
-        <v>1.13645727183976E-4</v>
+        <v>1.3331231485431199E-4</v>
       </c>
       <c r="T17" s="8">
-        <v>-7.1773973147808801E-5</v>
+        <v>-7.7289099348945803E-5</v>
       </c>
       <c r="U17" s="8">
-        <v>1.5779516431669299E-5</v>
+        <v>2.61524329992401E-5</v>
       </c>
       <c r="V17" s="8">
-        <v>3.6352346873185998E-5</v>
+        <v>4.9679280082472199E-5</v>
       </c>
       <c r="W17" s="8">
-        <v>5.5365947700756198E-5</v>
+        <v>7.3722909038106301E-5</v>
       </c>
       <c r="X17" s="8">
-        <v>6.5183864173259105E-5</v>
+        <v>8.4890527292015696E-5</v>
       </c>
       <c r="Y17" s="8">
-        <v>-2.2452118188708799E-6</v>
+        <v>-2.9009467812494298E-6</v>
       </c>
       <c r="Z17" s="8">
-        <v>5.5084366721645302E-5</v>
+        <v>6.3330501774483893E-5</v>
       </c>
       <c r="AA17" s="8">
-        <v>-4.66521038580232E-7</v>
+        <v>-5.3640170479163096E-7</v>
       </c>
       <c r="AB17" s="8">
-        <v>-3.85206566010371E-7</v>
+        <v>3.2967375013854098E-7</v>
       </c>
       <c r="AC17" s="8">
-        <v>-1.92370469454462E-7</v>
+        <v>-3.9180601223586898E-7</v>
       </c>
       <c r="AD17" s="8">
-        <v>-1.6105896076746599E-5</v>
+        <v>-1.97430502566085E-5</v>
       </c>
       <c r="AE17" s="8">
-        <v>-1.74327434238358E-3</v>
+        <v>-2.02747983557493E-3</v>
       </c>
     </row>
     <row r="18" spans="1:31" x14ac:dyDescent="0.25">
@@ -6397,94 +6397,94 @@
         <v>53</v>
       </c>
       <c r="B18" s="8">
-        <v>8.6609891146125106E-2</v>
+        <v>0.100193867695943</v>
       </c>
       <c r="C18" s="8">
-        <v>-8.2780689322515501E-6</v>
+        <v>-9.9279137317001898E-6</v>
       </c>
       <c r="D18" s="8">
-        <v>-1.8698510442086401E-6</v>
+        <v>-2.13462856629145E-6</v>
       </c>
       <c r="E18" s="8">
-        <v>-4.9240868057766601E-6</v>
+        <v>-1.20138070365011E-5</v>
       </c>
       <c r="F18" s="8">
-        <v>-1.7057351646447302E-5</v>
+        <v>-2.0077626985483901E-5</v>
       </c>
       <c r="G18" s="8">
-        <v>-9.4587375159042708E-6</v>
+        <v>-2.6096533285045499E-6</v>
       </c>
       <c r="H18" s="8">
-        <v>-2.0299650416265399E-6</v>
+        <v>9.31943054430196E-7</v>
       </c>
       <c r="I18" s="8">
-        <v>2.2368717647622999E-5</v>
+        <v>3.5997478630352902E-5</v>
       </c>
       <c r="J18" s="8">
-        <v>1.32228971508395E-5</v>
+        <v>1.9209982023377301E-5</v>
       </c>
       <c r="K18" s="8">
-        <v>1.56302883109403E-6</v>
+        <v>9.1357707325113E-7</v>
       </c>
       <c r="L18" s="8">
-        <v>1.9511115008202899E-5</v>
+        <v>2.7147849673577502E-5</v>
       </c>
       <c r="M18" s="8">
-        <v>-7.3371464742691503E-7</v>
+        <v>6.6818445092609104E-6</v>
       </c>
       <c r="N18" s="8">
-        <v>2.9332047475643201E-6</v>
+        <v>-1.16746316912147E-6</v>
       </c>
       <c r="O18" s="8">
-        <v>-2.9584728819421901E-5</v>
+        <v>-3.6702645094146201E-5</v>
       </c>
       <c r="P18" s="8">
-        <v>3.8754489998824402E-5</v>
+        <v>4.5175697167543002E-5</v>
       </c>
       <c r="Q18" s="8">
-        <v>8.0031535455390605E-5</v>
+        <v>9.0764600119650697E-5</v>
       </c>
       <c r="R18" s="8">
-        <v>1.13645727183976E-4</v>
+        <v>1.3331231485431199E-4</v>
       </c>
       <c r="S18" s="8">
-        <v>1.0382522966528899E-3</v>
+        <v>1.18927491267012E-3</v>
       </c>
       <c r="T18" s="8">
-        <v>-5.7121262786169802E-6</v>
+        <v>-4.0794433910680801E-6</v>
       </c>
       <c r="U18" s="8">
-        <v>2.02444919915333E-5</v>
+        <v>2.9071024613942401E-5</v>
       </c>
       <c r="V18" s="8">
-        <v>4.0740378426400499E-5</v>
+        <v>5.0188364917226199E-5</v>
       </c>
       <c r="W18" s="8">
-        <v>5.8952562926472798E-5</v>
+        <v>7.3108646647776794E-5</v>
       </c>
       <c r="X18" s="8">
-        <v>8.7215365226699996E-5</v>
+        <v>1.09129645541733E-4</v>
       </c>
       <c r="Y18" s="8">
-        <v>4.3593039336208697E-6</v>
+        <v>5.4847932434880296E-6</v>
       </c>
       <c r="Z18" s="8">
-        <v>1.18728662371079E-5</v>
+        <v>1.42629328627203E-5</v>
       </c>
       <c r="AA18" s="8">
-        <v>-1.7554585675004099E-7</v>
+        <v>-2.0701672798139601E-7</v>
       </c>
       <c r="AB18" s="8">
-        <v>-2.40755746117661E-6</v>
+        <v>-2.4172064832221799E-6</v>
       </c>
       <c r="AC18" s="8">
-        <v>5.5415978971095695E-7</v>
+        <v>6.1002342600027205E-7</v>
       </c>
       <c r="AD18" s="8">
-        <v>6.6251454878027795E-5</v>
+        <v>7.7126497176866198E-5</v>
       </c>
       <c r="AE18" s="8">
-        <v>-4.8300055975499298E-4</v>
+        <v>-5.8930728573233597E-4</v>
       </c>
     </row>
     <row r="19" spans="1:31" x14ac:dyDescent="0.25">
@@ -6492,94 +6492,94 @@
         <v>16</v>
       </c>
       <c r="B19" s="8">
-        <v>-1.9839525651406099E-3</v>
+        <v>-2.2352681955837301E-2</v>
       </c>
       <c r="C19" s="8">
-        <v>-4.0592578385189901E-5</v>
+        <v>-4.1350089656322197E-5</v>
       </c>
       <c r="D19" s="8">
-        <v>-2.1221594112663101E-5</v>
+        <v>-1.42209370920578E-5</v>
       </c>
       <c r="E19" s="8">
-        <v>3.68857457939547E-5</v>
+        <v>4.7438658382716498E-5</v>
       </c>
       <c r="F19" s="8">
-        <v>4.3090844192620901E-5</v>
+        <v>5.5217612501320798E-5</v>
       </c>
       <c r="G19" s="8">
-        <v>6.2817937381026402E-5</v>
+        <v>7.1240931926224804E-5</v>
       </c>
       <c r="H19" s="8">
-        <v>4.2571056359572699E-5</v>
+        <v>4.73286276623642E-5</v>
       </c>
       <c r="I19" s="8">
-        <v>3.9823040541493802E-5</v>
+        <v>4.56440488905475E-5</v>
       </c>
       <c r="J19" s="8">
-        <v>3.7981668450014302E-5</v>
+        <v>4.5609701434661802E-5</v>
       </c>
       <c r="K19" s="8">
-        <v>4.2835056594919702E-5</v>
+        <v>5.1540039121004997E-5</v>
       </c>
       <c r="L19" s="8">
-        <v>5.7067095962278198E-5</v>
+        <v>6.7701892225327306E-5</v>
       </c>
       <c r="M19" s="8">
-        <v>4.6379169406659901E-5</v>
+        <v>6.1627571517514302E-5</v>
       </c>
       <c r="N19" s="8">
-        <v>4.1272600779181599E-5</v>
+        <v>4.5440106257838403E-5</v>
       </c>
       <c r="O19" s="8">
-        <v>4.1433272052927503E-5</v>
+        <v>4.0131854807533302E-5</v>
       </c>
       <c r="P19" s="8">
-        <v>-9.7531415604059697E-5</v>
+        <v>-1.1116496459388299E-4</v>
       </c>
       <c r="Q19" s="8">
-        <v>-5.5940677296196703E-5</v>
+        <v>-6.21584990709412E-5</v>
       </c>
       <c r="R19" s="8">
-        <v>-7.1773973147808801E-5</v>
+        <v>-7.7289099348945803E-5</v>
       </c>
       <c r="S19" s="8">
-        <v>-5.7121262786169802E-6</v>
+        <v>-4.0794433910680801E-6</v>
       </c>
       <c r="T19" s="8">
-        <v>8.41823407019094E-4</v>
+        <v>1.0236473165117499E-3</v>
       </c>
       <c r="U19" s="8">
-        <v>2.11976795404442E-5</v>
+        <v>2.2627095769220101E-5</v>
       </c>
       <c r="V19" s="8">
-        <v>4.0364142365726502E-5</v>
+        <v>4.3429198083065101E-5</v>
       </c>
       <c r="W19" s="8">
-        <v>5.4400876860029798E-5</v>
+        <v>6.4314317233292296E-5</v>
       </c>
       <c r="X19" s="8">
-        <v>5.62125285714999E-5</v>
+        <v>6.7791680830807098E-5</v>
       </c>
       <c r="Y19" s="8">
-        <v>1.24211277206181E-6</v>
+        <v>3.4875306348864399E-6</v>
       </c>
       <c r="Z19" s="8">
-        <v>9.3900223970164906E-6</v>
+        <v>8.2888908876588401E-6</v>
       </c>
       <c r="AA19" s="8">
-        <v>-5.4292044381871703E-8</v>
+        <v>-3.9323794267271799E-8</v>
       </c>
       <c r="AB19" s="8">
-        <v>-6.3523162173816995E-7</v>
+        <v>-1.5749482770519299E-6</v>
       </c>
       <c r="AC19" s="8">
-        <v>-7.9574462340996304E-7</v>
+        <v>-7.3721064632517403E-7</v>
       </c>
       <c r="AD19" s="8">
-        <v>-9.3157366746979495E-6</v>
+        <v>-9.0163730052424107E-6</v>
       </c>
       <c r="AE19" s="8">
-        <v>-2.9285221741463498E-4</v>
+        <v>-3.2003691452027298E-4</v>
       </c>
     </row>
     <row r="20" spans="1:31" x14ac:dyDescent="0.25">
@@ -6587,94 +6587,94 @@
         <v>36</v>
       </c>
       <c r="B20" s="8">
-        <v>-1.8711310319162101E-2</v>
+        <v>2.2309259737625101E-2</v>
       </c>
       <c r="C20" s="8">
-        <v>3.9379643112702798E-6</v>
+        <v>1.91318083550039E-6</v>
       </c>
       <c r="D20" s="8">
-        <v>3.0996645130731401E-5</v>
+        <v>3.5814952747186198E-5</v>
       </c>
       <c r="E20" s="8">
-        <v>4.1729103326868701E-6</v>
+        <v>2.79489533657508E-6</v>
       </c>
       <c r="F20" s="8">
-        <v>-6.2880685016332799E-6</v>
+        <v>-1.1855162827996501E-5</v>
       </c>
       <c r="G20" s="8">
-        <v>1.8615676280719099E-5</v>
+        <v>2.11530738951042E-5</v>
       </c>
       <c r="H20" s="8">
-        <v>2.1918353506485799E-5</v>
+        <v>2.6467123511162898E-5</v>
       </c>
       <c r="I20" s="8">
-        <v>-6.7536704301496198E-6</v>
+        <v>-9.1603580059529405E-6</v>
       </c>
       <c r="J20" s="8">
-        <v>5.0968749236754097E-6</v>
+        <v>6.5073196545890401E-6</v>
       </c>
       <c r="K20" s="8">
-        <v>1.42429998842197E-6</v>
+        <v>7.29068227473261E-7</v>
       </c>
       <c r="L20" s="8">
-        <v>1.4664818340628501E-5</v>
+        <v>1.9143069186142902E-5</v>
       </c>
       <c r="M20" s="8">
-        <v>-1.9755155230674201E-5</v>
+        <v>-2.5422105778243801E-5</v>
       </c>
       <c r="N20" s="8">
-        <v>-3.3705999597703201E-6</v>
+        <v>-4.5794108509856701E-6</v>
       </c>
       <c r="O20" s="8">
-        <v>1.67683286339425E-5</v>
+        <v>2.0148854559633401E-5</v>
       </c>
       <c r="P20" s="8">
-        <v>-7.8454978079788295E-6</v>
+        <v>-7.9562596322946299E-6</v>
       </c>
       <c r="Q20" s="8">
-        <v>-5.9407540007460198E-5</v>
+        <v>-7.0927252510696604E-5</v>
       </c>
       <c r="R20" s="8">
-        <v>1.5779516431669299E-5</v>
+        <v>2.61524329992401E-5</v>
       </c>
       <c r="S20" s="8">
-        <v>2.02444919915333E-5</v>
+        <v>2.9071024613942401E-5</v>
       </c>
       <c r="T20" s="8">
-        <v>2.11976795404442E-5</v>
+        <v>2.2627095769220101E-5</v>
       </c>
       <c r="U20" s="8">
-        <v>9.8888022089552792E-4</v>
+        <v>1.15659631093541E-3</v>
       </c>
       <c r="V20" s="8">
-        <v>5.81317468807532E-4</v>
+        <v>6.8600375327326399E-4</v>
       </c>
       <c r="W20" s="8">
-        <v>5.8165133657198098E-4</v>
+        <v>6.8789877969865898E-4</v>
       </c>
       <c r="X20" s="8">
-        <v>5.8621389328490496E-4</v>
+        <v>6.9197556917172001E-4</v>
       </c>
       <c r="Y20" s="8">
-        <v>8.2176604300124797E-7</v>
+        <v>1.0755515773576001E-6</v>
       </c>
       <c r="Z20" s="8">
-        <v>-1.78319282383282E-6</v>
+        <v>-1.6790683410450901E-6</v>
       </c>
       <c r="AA20" s="8">
-        <v>2.0830984649913701E-8</v>
+        <v>2.1457284703336802E-8</v>
       </c>
       <c r="AB20" s="8">
-        <v>9.9531707865136996E-7</v>
+        <v>4.3895491149337898E-7</v>
       </c>
       <c r="AC20" s="8">
-        <v>-3.2592074558167801E-7</v>
+        <v>-4.2427498088028702E-7</v>
       </c>
       <c r="AD20" s="8">
-        <v>-1.4135019686785101E-6</v>
+        <v>-2.3246166410971702E-6</v>
       </c>
       <c r="AE20" s="8">
-        <v>-5.0830524459590995E-4</v>
+        <v>-6.0343873500080401E-4</v>
       </c>
     </row>
     <row r="21" spans="1:31" x14ac:dyDescent="0.25">
@@ -6682,94 +6682,94 @@
         <v>37</v>
       </c>
       <c r="B21" s="8">
-        <v>-3.6328834021091397E-2</v>
+        <v>-2.0425244106391498E-2</v>
       </c>
       <c r="C21" s="8">
-        <v>8.3171355284270804E-6</v>
+        <v>3.3041349502523199E-6</v>
       </c>
       <c r="D21" s="8">
-        <v>7.9350084145568799E-5</v>
+        <v>8.9611846726394003E-5</v>
       </c>
       <c r="E21" s="8">
-        <v>2.0962883283508201E-5</v>
+        <v>2.2573849262117901E-5</v>
       </c>
       <c r="F21" s="8">
-        <v>3.7063233851829799E-6</v>
+        <v>-2.5019864470842898E-7</v>
       </c>
       <c r="G21" s="8">
-        <v>4.1551083322488797E-5</v>
+        <v>4.4813463677083998E-5</v>
       </c>
       <c r="H21" s="8">
-        <v>1.8416293187680999E-5</v>
+        <v>2.4321109081398299E-5</v>
       </c>
       <c r="I21" s="8">
-        <v>1.2937959954825E-5</v>
+        <v>1.3821006156554199E-5</v>
       </c>
       <c r="J21" s="8">
-        <v>7.2767229358422396E-6</v>
+        <v>6.7853092412037403E-6</v>
       </c>
       <c r="K21" s="8">
-        <v>-6.6221732725682299E-6</v>
+        <v>-1.0732893964541201E-5</v>
       </c>
       <c r="L21" s="8">
-        <v>2.3388040519728401E-5</v>
+        <v>2.56481346570062E-5</v>
       </c>
       <c r="M21" s="8">
-        <v>-2.7764603458460301E-6</v>
+        <v>-3.45555222942537E-6</v>
       </c>
       <c r="N21" s="8">
-        <v>6.37494368668692E-7</v>
+        <v>-2.83720642714685E-7</v>
       </c>
       <c r="O21" s="8">
-        <v>1.04724336218278E-5</v>
+        <v>9.9248871066617208E-6</v>
       </c>
       <c r="P21" s="8">
-        <v>2.4290310032538301E-5</v>
+        <v>2.6046774834424301E-5</v>
       </c>
       <c r="Q21" s="8">
-        <v>-1.0782803402241E-4</v>
+        <v>-1.2588526729479999E-4</v>
       </c>
       <c r="R21" s="8">
-        <v>3.6352346873185998E-5</v>
+        <v>4.9679280082472199E-5</v>
       </c>
       <c r="S21" s="8">
-        <v>4.0740378426400499E-5</v>
+        <v>5.0188364917226199E-5</v>
       </c>
       <c r="T21" s="8">
-        <v>4.0364142365726502E-5</v>
+        <v>4.3429198083065101E-5</v>
       </c>
       <c r="U21" s="8">
-        <v>5.81317468807532E-4</v>
+        <v>6.8600375327326399E-4</v>
       </c>
       <c r="V21" s="8">
-        <v>1.0029711438783999E-3</v>
+        <v>1.1650979497605999E-3</v>
       </c>
       <c r="W21" s="8">
-        <v>6.45302930388035E-4</v>
+        <v>7.6258045902615596E-4</v>
       </c>
       <c r="X21" s="8">
-        <v>6.5218866189764905E-4</v>
+        <v>7.6432702239074602E-4</v>
       </c>
       <c r="Y21" s="8">
-        <v>1.5626081936833E-6</v>
+        <v>1.6172225943054599E-6</v>
       </c>
       <c r="Z21" s="8">
-        <v>-2.3892239740048601E-6</v>
+        <v>-2.0082828324227799E-6</v>
       </c>
       <c r="AA21" s="8">
-        <v>2.8856063094321E-8</v>
+        <v>2.7251499691834201E-8</v>
       </c>
       <c r="AB21" s="8">
-        <v>6.9973055967448603E-7</v>
+        <v>3.1611865645414502E-7</v>
       </c>
       <c r="AC21" s="8">
-        <v>-4.6478548740327398E-7</v>
+        <v>-6.7520325707067597E-7</v>
       </c>
       <c r="AD21" s="8">
-        <v>-2.8050407074725201E-6</v>
+        <v>-3.7027571161401702E-6</v>
       </c>
       <c r="AE21" s="8">
-        <v>-5.5009015460508301E-4</v>
+        <v>-6.4662214277764096E-4</v>
       </c>
     </row>
     <row r="22" spans="1:31" x14ac:dyDescent="0.25">
@@ -6777,94 +6777,94 @@
         <v>39</v>
       </c>
       <c r="B22" s="8">
-        <v>-9.7171783858513494E-2</v>
+        <v>-7.3517302034389304E-2</v>
       </c>
       <c r="C22" s="8">
-        <v>4.2359405450572197E-5</v>
+        <v>4.6952328925989297E-5</v>
       </c>
       <c r="D22" s="8">
-        <v>1.4105827746942399E-4</v>
+        <v>1.6642486668752901E-4</v>
       </c>
       <c r="E22" s="8">
-        <v>4.4104427172820198E-5</v>
+        <v>5.2391126157177499E-5</v>
       </c>
       <c r="F22" s="8">
-        <v>1.46164008306629E-5</v>
+        <v>1.3362115106098899E-5</v>
       </c>
       <c r="G22" s="8">
-        <v>4.9928669776200099E-5</v>
+        <v>6.0259661667862401E-5</v>
       </c>
       <c r="H22" s="8">
-        <v>3.08288208863186E-5</v>
+        <v>3.89303830469338E-5</v>
       </c>
       <c r="I22" s="8">
-        <v>1.8937014308333901E-6</v>
+        <v>4.8494212442156504E-7</v>
       </c>
       <c r="J22" s="8">
-        <v>3.3932315697247498E-6</v>
+        <v>5.7886321222854198E-6</v>
       </c>
       <c r="K22" s="8">
-        <v>-1.02458102563469E-5</v>
+        <v>-1.1850561039834101E-5</v>
       </c>
       <c r="L22" s="8">
-        <v>2.9969985197550901E-5</v>
+        <v>3.7107748931661102E-5</v>
       </c>
       <c r="M22" s="8">
-        <v>2.1540222536876999E-6</v>
+        <v>3.3956283051879098E-6</v>
       </c>
       <c r="N22" s="8">
-        <v>-1.2536478976609201E-6</v>
+        <v>-1.26631378195263E-6</v>
       </c>
       <c r="O22" s="8">
-        <v>2.01425835441656E-5</v>
+        <v>2.5526520505940499E-5</v>
       </c>
       <c r="P22" s="8">
-        <v>7.0165346316770796E-5</v>
+        <v>7.9411022508725301E-5</v>
       </c>
       <c r="Q22" s="8">
-        <v>-1.4840980140309399E-4</v>
+        <v>-1.72374252316291E-4</v>
       </c>
       <c r="R22" s="8">
-        <v>5.5365947700756198E-5</v>
+        <v>7.3722909038106301E-5</v>
       </c>
       <c r="S22" s="8">
-        <v>5.8952562926472798E-5</v>
+        <v>7.3108646647776794E-5</v>
       </c>
       <c r="T22" s="8">
-        <v>5.4400876860029798E-5</v>
+        <v>6.4314317233292296E-5</v>
       </c>
       <c r="U22" s="8">
-        <v>5.8165133657198098E-4</v>
+        <v>6.8789877969865898E-4</v>
       </c>
       <c r="V22" s="8">
-        <v>6.45302930388035E-4</v>
+        <v>7.6258045902615596E-4</v>
       </c>
       <c r="W22" s="8">
-        <v>1.0310637481631599E-3</v>
+        <v>1.20493905098047E-3</v>
       </c>
       <c r="X22" s="8">
-        <v>7.2036765567116598E-4</v>
+        <v>8.5029326638424801E-4</v>
       </c>
       <c r="Y22" s="8">
-        <v>2.5600043925631599E-6</v>
+        <v>3.23297719815847E-6</v>
       </c>
       <c r="Z22" s="8">
-        <v>-3.3699752045690399E-6</v>
+        <v>-3.5967480327397998E-6</v>
       </c>
       <c r="AA22" s="8">
-        <v>3.8758076920986897E-8</v>
+        <v>4.2421803351244302E-8</v>
       </c>
       <c r="AB22" s="8">
-        <v>1.05914080754865E-6</v>
+        <v>1.05480574777121E-6</v>
       </c>
       <c r="AC22" s="8">
-        <v>-1.2237123332555901E-6</v>
+        <v>-1.5233223652456701E-6</v>
       </c>
       <c r="AD22" s="8">
-        <v>-5.42418415515061E-6</v>
+        <v>-5.8971570598778703E-6</v>
       </c>
       <c r="AE22" s="8">
-        <v>-5.7855919248601603E-4</v>
+        <v>-6.8990241620984203E-4</v>
       </c>
     </row>
     <row r="23" spans="1:31" x14ac:dyDescent="0.25">
@@ -6872,94 +6872,94 @@
         <v>40</v>
       </c>
       <c r="B23" s="8">
-        <v>-0.13099351771815301</v>
+        <v>-0.111862436797608</v>
       </c>
       <c r="C23" s="8">
-        <v>1.1310542853406799E-4</v>
+        <v>1.26673590139778E-4</v>
       </c>
       <c r="D23" s="8">
-        <v>2.3307138367297499E-4</v>
+        <v>2.72846330738831E-4</v>
       </c>
       <c r="E23" s="8">
-        <v>7.5498205724560394E-5</v>
+        <v>8.9592986289246894E-5</v>
       </c>
       <c r="F23" s="8">
-        <v>4.9556502837882102E-5</v>
+        <v>5.09529760875342E-5</v>
       </c>
       <c r="G23" s="8">
-        <v>1.08346350261165E-4</v>
+        <v>1.2557094002796701E-4</v>
       </c>
       <c r="H23" s="8">
-        <v>6.3945139421550705E-5</v>
+        <v>7.6712856723919597E-5</v>
       </c>
       <c r="I23" s="8">
-        <v>5.0605238158786502E-5</v>
+        <v>6.1647497147890998E-5</v>
       </c>
       <c r="J23" s="8">
-        <v>2.5266040376806101E-5</v>
+        <v>2.7925954255685498E-5</v>
       </c>
       <c r="K23" s="8">
-        <v>-2.4041000478841299E-6</v>
+        <v>-3.4716528760721099E-6</v>
       </c>
       <c r="L23" s="8">
-        <v>5.8356956344715599E-5</v>
+        <v>6.7646001507972196E-5</v>
       </c>
       <c r="M23" s="8">
-        <v>5.8464918096278697E-5</v>
+        <v>7.0502876225044396E-5</v>
       </c>
       <c r="N23" s="8">
-        <v>3.8916144388137498E-5</v>
+        <v>4.3319296740491001E-5</v>
       </c>
       <c r="O23" s="8">
-        <v>7.6898295914402893E-5</v>
+        <v>9.1333861271211605E-5</v>
       </c>
       <c r="P23" s="8">
-        <v>1.3157493114683699E-4</v>
+        <v>1.50806604864911E-4</v>
       </c>
       <c r="Q23" s="8">
-        <v>-1.7070011691610099E-4</v>
+        <v>-1.95533003974164E-4</v>
       </c>
       <c r="R23" s="8">
-        <v>6.5183864173259105E-5</v>
+        <v>8.4890527292015696E-5</v>
       </c>
       <c r="S23" s="8">
-        <v>8.7215365226699996E-5</v>
+        <v>1.09129645541733E-4</v>
       </c>
       <c r="T23" s="8">
-        <v>5.62125285714999E-5</v>
+        <v>6.7791680830807098E-5</v>
       </c>
       <c r="U23" s="8">
-        <v>5.8621389328490496E-4</v>
+        <v>6.9197556917172001E-4</v>
       </c>
       <c r="V23" s="8">
-        <v>6.5218866189764905E-4</v>
+        <v>7.6432702239074602E-4</v>
       </c>
       <c r="W23" s="8">
-        <v>7.2036765567116598E-4</v>
+        <v>8.5029326638424801E-4</v>
       </c>
       <c r="X23" s="8">
-        <v>1.10544808444687E-3</v>
+        <v>1.2805826737165599E-3</v>
       </c>
       <c r="Y23" s="8">
-        <v>4.7974937510505502E-6</v>
+        <v>5.9471859720296402E-6</v>
       </c>
       <c r="Z23" s="8">
-        <v>-4.0606313243392302E-6</v>
+        <v>-4.4497951762676798E-6</v>
       </c>
       <c r="AA23" s="8">
-        <v>3.4313051256944299E-8</v>
+        <v>3.70618181247553E-8</v>
       </c>
       <c r="AB23" s="8">
-        <v>2.29593528240283E-6</v>
+        <v>2.1344625515066801E-6</v>
       </c>
       <c r="AC23" s="8">
-        <v>-1.7896033229644601E-6</v>
+        <v>-2.10778213698244E-6</v>
       </c>
       <c r="AD23" s="8">
-        <v>-1.32007956271289E-5</v>
+        <v>-1.56869463954917E-5</v>
       </c>
       <c r="AE23" s="8">
-        <v>-6.9069536585095203E-4</v>
+        <v>-8.1528135790835102E-4</v>
       </c>
     </row>
     <row r="24" spans="1:31" x14ac:dyDescent="0.25">
@@ -6967,94 +6967,94 @@
         <v>38</v>
       </c>
       <c r="B24" s="8">
-        <v>2.8886070233809801E-2</v>
+        <v>3.1499827611078501E-2</v>
       </c>
       <c r="C24" s="8">
-        <v>3.8098118934446802E-6</v>
+        <v>4.5839887235734501E-6</v>
       </c>
       <c r="D24" s="8">
-        <v>1.1502362711482E-5</v>
+        <v>1.32370347400556E-5</v>
       </c>
       <c r="E24" s="8">
-        <v>1.8836165493875299E-6</v>
+        <v>3.1332567222028001E-6</v>
       </c>
       <c r="F24" s="8">
-        <v>2.5089513554834998E-6</v>
+        <v>3.04745386287188E-6</v>
       </c>
       <c r="G24" s="8">
-        <v>1.20824045247566E-7</v>
+        <v>1.4649771969649601E-6</v>
       </c>
       <c r="H24" s="8">
-        <v>2.7648007721724699E-6</v>
+        <v>4.0837088237694404E-6</v>
       </c>
       <c r="I24" s="8">
-        <v>1.6978409151919101E-6</v>
+        <v>3.1059261802282901E-6</v>
       </c>
       <c r="J24" s="8">
-        <v>2.9313715455486101E-6</v>
+        <v>4.1408426350238101E-6</v>
       </c>
       <c r="K24" s="8">
-        <v>4.18596249083941E-6</v>
+        <v>5.7973963116998801E-6</v>
       </c>
       <c r="L24" s="8">
-        <v>4.6693648620851297E-6</v>
+        <v>6.3004410475683398E-6</v>
       </c>
       <c r="M24" s="8">
-        <v>3.6520359783675901E-6</v>
+        <v>4.8920983458875596E-6</v>
       </c>
       <c r="N24" s="8">
-        <v>4.75101959656989E-6</v>
+        <v>5.4380420427733802E-6</v>
       </c>
       <c r="O24" s="8">
-        <v>4.4315271554711699E-6</v>
+        <v>5.73017255860853E-6</v>
       </c>
       <c r="P24" s="8">
-        <v>3.7917113160447001E-6</v>
+        <v>4.0475815549796298E-6</v>
       </c>
       <c r="Q24" s="8">
-        <v>4.0793567108096299E-8</v>
+        <v>8.9358621184339395E-7</v>
       </c>
       <c r="R24" s="8">
-        <v>-2.2452118188708799E-6</v>
+        <v>-2.9009467812494298E-6</v>
       </c>
       <c r="S24" s="8">
-        <v>4.3593039336208697E-6</v>
+        <v>5.4847932434880296E-6</v>
       </c>
       <c r="T24" s="8">
-        <v>1.24211277206181E-6</v>
+        <v>3.4875306348864399E-6</v>
       </c>
       <c r="U24" s="8">
-        <v>8.2176604300124797E-7</v>
+        <v>1.0755515773576001E-6</v>
       </c>
       <c r="V24" s="8">
-        <v>1.5626081936833E-6</v>
+        <v>1.6172225943054599E-6</v>
       </c>
       <c r="W24" s="8">
-        <v>2.5600043925631599E-6</v>
+        <v>3.23297719815847E-6</v>
       </c>
       <c r="X24" s="8">
-        <v>4.7974937510505502E-6</v>
+        <v>5.9471859720296402E-6</v>
       </c>
       <c r="Y24" s="8">
-        <v>9.0000178853402292E-6</v>
+        <v>1.0350666141442901E-5</v>
       </c>
       <c r="Z24" s="8">
-        <v>9.7594479553951604E-8</v>
+        <v>-1.14461256540696E-7</v>
       </c>
       <c r="AA24" s="8">
-        <v>-4.3118766664605099E-9</v>
+        <v>-3.02704311298918E-9</v>
       </c>
       <c r="AB24" s="8">
-        <v>1.50544835564094E-8</v>
+        <v>-1.04691264626086E-7</v>
       </c>
       <c r="AC24" s="8">
-        <v>-4.8749717131876203E-8</v>
+        <v>1.9117712640044601E-8</v>
       </c>
       <c r="AD24" s="8">
-        <v>4.01314544029872E-7</v>
+        <v>7.5244011205111602E-7</v>
       </c>
       <c r="AE24" s="8">
-        <v>-1.3216703652810699E-4</v>
+        <v>-1.5302013977393599E-4</v>
       </c>
     </row>
     <row r="25" spans="1:31" x14ac:dyDescent="0.25">
@@ -7062,94 +7062,94 @@
         <v>48</v>
       </c>
       <c r="B25" s="8">
-        <v>4.2413202472385302E-2</v>
+        <v>4.5049355726028799E-2</v>
       </c>
       <c r="C25" s="8">
-        <v>2.3186605375299799E-6</v>
+        <v>1.45013491727407E-6</v>
       </c>
       <c r="D25" s="8">
-        <v>4.5098950532457102E-6</v>
+        <v>4.93913349409411E-6</v>
       </c>
       <c r="E25" s="8">
-        <v>1.4540394072156199E-6</v>
+        <v>7.68817234143558E-7</v>
       </c>
       <c r="F25" s="8">
-        <v>3.79991630210079E-6</v>
+        <v>4.2571390162228302E-6</v>
       </c>
       <c r="G25" s="8">
-        <v>4.0937818072402197E-6</v>
+        <v>5.2401916774154498E-6</v>
       </c>
       <c r="H25" s="8">
-        <v>3.0291747018516901E-6</v>
+        <v>3.2968869255359699E-6</v>
       </c>
       <c r="I25" s="8">
-        <v>4.0541324596371204E-6</v>
+        <v>5.2875855157522297E-6</v>
       </c>
       <c r="J25" s="8">
-        <v>5.2899874033586298E-6</v>
+        <v>5.85062025927404E-6</v>
       </c>
       <c r="K25" s="8">
-        <v>5.1717440034410497E-6</v>
+        <v>5.9177157680461901E-6</v>
       </c>
       <c r="L25" s="8">
-        <v>3.3546060489813401E-6</v>
+        <v>3.8526359116769196E-6</v>
       </c>
       <c r="M25" s="8">
-        <v>3.82789490967876E-6</v>
+        <v>4.9961814672834201E-6</v>
       </c>
       <c r="N25" s="8">
-        <v>2.02507699844905E-6</v>
+        <v>1.47030293991179E-6</v>
       </c>
       <c r="O25" s="8">
-        <v>2.4645913414325602E-6</v>
+        <v>3.00894646192022E-6</v>
       </c>
       <c r="P25" s="8">
-        <v>1.1125106328094E-5</v>
+        <v>1.3188581899491499E-5</v>
       </c>
       <c r="Q25" s="8">
-        <v>-5.2504939103552898E-6</v>
+        <v>-6.1393077011780697E-6</v>
       </c>
       <c r="R25" s="8">
-        <v>5.5084366721645302E-5</v>
+        <v>6.3330501774483893E-5</v>
       </c>
       <c r="S25" s="8">
-        <v>1.18728662371079E-5</v>
+        <v>1.42629328627203E-5</v>
       </c>
       <c r="T25" s="8">
-        <v>9.3900223970164906E-6</v>
+        <v>8.2888908876588401E-6</v>
       </c>
       <c r="U25" s="8">
-        <v>-1.78319282383282E-6</v>
+        <v>-1.6790683410450901E-6</v>
       </c>
       <c r="V25" s="8">
-        <v>-2.3892239740048601E-6</v>
+        <v>-2.0082828324227799E-6</v>
       </c>
       <c r="W25" s="8">
-        <v>-3.3699752045690399E-6</v>
+        <v>-3.5967480327397998E-6</v>
       </c>
       <c r="X25" s="8">
-        <v>-4.0606313243392302E-6</v>
+        <v>-4.4497951762676798E-6</v>
       </c>
       <c r="Y25" s="8">
-        <v>9.7594479553951604E-8</v>
+        <v>-1.14461256540696E-7</v>
       </c>
       <c r="Z25" s="8">
-        <v>1.14729184850013E-5</v>
+        <v>1.39805020942688E-5</v>
       </c>
       <c r="AA25" s="8">
-        <v>-1.08857396665175E-7</v>
+        <v>-1.32089135050812E-7</v>
       </c>
       <c r="AB25" s="8">
-        <v>-3.52323561291942E-7</v>
+        <v>-3.6573957757971702E-7</v>
       </c>
       <c r="AC25" s="8">
-        <v>-3.3814954034462999E-7</v>
+        <v>-4.1793257396012402E-7</v>
       </c>
       <c r="AD25" s="8">
-        <v>2.9400583148254502E-7</v>
+        <v>3.1822258948493501E-7</v>
       </c>
       <c r="AE25" s="8">
-        <v>-2.6492355287693702E-4</v>
+        <v>-3.2109578282953202E-4</v>
       </c>
     </row>
     <row r="26" spans="1:31" x14ac:dyDescent="0.25">
@@ -7157,94 +7157,94 @@
         <v>49</v>
       </c>
       <c r="B26" s="8">
-        <v>-6.4330597660827704E-4</v>
+        <v>-6.7431571214193698E-4</v>
       </c>
       <c r="C26" s="8">
-        <v>-2.96876384478013E-8</v>
+        <v>-2.47772683099099E-8</v>
       </c>
       <c r="D26" s="8">
-        <v>-1.10974150357213E-7</v>
+        <v>-1.2776962150714601E-7</v>
       </c>
       <c r="E26" s="8">
-        <v>-2.0871386532620001E-8</v>
+        <v>-1.6172177507542401E-8</v>
       </c>
       <c r="F26" s="8">
-        <v>-3.8508510245791399E-8</v>
+        <v>-4.27724312176736E-8</v>
       </c>
       <c r="G26" s="8">
-        <v>-3.5236699134234201E-8</v>
+        <v>-4.5394718343653701E-8</v>
       </c>
       <c r="H26" s="8">
-        <v>-2.8249601511346799E-8</v>
+        <v>-3.2034436076023703E-8</v>
       </c>
       <c r="I26" s="8">
-        <v>-4.1247948738422799E-8</v>
+        <v>-5.46574582925461E-8</v>
       </c>
       <c r="J26" s="8">
-        <v>-6.1720025210646596E-8</v>
+        <v>-7.0482077364380495E-8</v>
       </c>
       <c r="K26" s="8">
-        <v>-6.12287384370235E-8</v>
+        <v>-7.1322725498930402E-8</v>
       </c>
       <c r="L26" s="8">
-        <v>-4.4709434046324701E-8</v>
+        <v>-4.9945772065316302E-8</v>
       </c>
       <c r="M26" s="8">
-        <v>-4.2882555618993997E-8</v>
+        <v>-5.4976619710327598E-8</v>
       </c>
       <c r="N26" s="8">
-        <v>-3.5302999281871103E-8</v>
+        <v>-3.3706719453285902E-8</v>
       </c>
       <c r="O26" s="8">
-        <v>-2.4497648314825999E-8</v>
+        <v>-3.2335581412306199E-8</v>
       </c>
       <c r="P26" s="8">
-        <v>-1.3599779644869E-7</v>
+        <v>-1.61178425341575E-7</v>
       </c>
       <c r="Q26" s="8">
-        <v>1.35152459553038E-8</v>
+        <v>1.67171893853106E-8</v>
       </c>
       <c r="R26" s="8">
-        <v>-4.66521038580232E-7</v>
+        <v>-5.3640170479163096E-7</v>
       </c>
       <c r="S26" s="8">
-        <v>-1.7554585675004099E-7</v>
+        <v>-2.0701672798139601E-7</v>
       </c>
       <c r="T26" s="8">
-        <v>-5.4292044381871703E-8</v>
+        <v>-3.9323794267271799E-8</v>
       </c>
       <c r="U26" s="8">
-        <v>2.0830984649913701E-8</v>
+        <v>2.1457284703336802E-8</v>
       </c>
       <c r="V26" s="8">
-        <v>2.8856063094321E-8</v>
+        <v>2.7251499691834201E-8</v>
       </c>
       <c r="W26" s="8">
-        <v>3.8758076920986897E-8</v>
+        <v>4.2421803351244302E-8</v>
       </c>
       <c r="X26" s="8">
-        <v>3.4313051256944299E-8</v>
+        <v>3.70618181247553E-8</v>
       </c>
       <c r="Y26" s="8">
-        <v>-4.3118766664605099E-9</v>
+        <v>-3.02704311298918E-9</v>
       </c>
       <c r="Z26" s="8">
-        <v>-1.08857396665175E-7</v>
+        <v>-1.32089135050812E-7</v>
       </c>
       <c r="AA26" s="8">
-        <v>1.08402391177238E-9</v>
+        <v>1.30749754927767E-9</v>
       </c>
       <c r="AB26" s="8">
-        <v>6.1210753017434302E-9</v>
+        <v>6.9132346830288197E-9</v>
       </c>
       <c r="AC26" s="8">
-        <v>5.8975396229339404E-9</v>
+        <v>7.0457598686589896E-9</v>
       </c>
       <c r="AD26" s="8">
-        <v>-1.12901224784365E-8</v>
+        <v>-1.2779040095727899E-8</v>
       </c>
       <c r="AE26" s="8">
-        <v>2.32104981362895E-6</v>
+        <v>2.8115420070873301E-6</v>
       </c>
     </row>
     <row r="27" spans="1:31" x14ac:dyDescent="0.25">
@@ -7252,94 +7252,94 @@
         <v>18</v>
       </c>
       <c r="B27" s="8">
-        <v>0.51913686387735403</v>
+        <v>0.51922278051236304</v>
       </c>
       <c r="C27" s="8">
-        <v>3.1793643979944501E-6</v>
+        <v>4.2520475251047098E-6</v>
       </c>
       <c r="D27" s="8">
-        <v>1.78599217928677E-6</v>
+        <v>2.6595676599196199E-6</v>
       </c>
       <c r="E27" s="8">
-        <v>-3.6280323879363201E-6</v>
+        <v>-3.80156139540954E-6</v>
       </c>
       <c r="F27" s="8">
-        <v>-3.1825181167266798E-6</v>
+        <v>-4.1990539914227599E-6</v>
       </c>
       <c r="G27" s="8">
-        <v>-3.0401644107485802E-6</v>
+        <v>-4.1673943924848104E-6</v>
       </c>
       <c r="H27" s="8">
-        <v>-3.8748260008656702E-6</v>
+        <v>-4.49737515273092E-6</v>
       </c>
       <c r="I27" s="8">
-        <v>-5.1389272628331798E-6</v>
+        <v>-5.8298771570024597E-6</v>
       </c>
       <c r="J27" s="8">
-        <v>-5.0673218306440097E-6</v>
+        <v>-5.8203358262003099E-6</v>
       </c>
       <c r="K27" s="8">
-        <v>-4.2648896152328296E-6</v>
+        <v>-5.1533565550716299E-6</v>
       </c>
       <c r="L27" s="8">
-        <v>-1.9645808338728002E-6</v>
+        <v>-1.4690678157870599E-6</v>
       </c>
       <c r="M27" s="8">
-        <v>-3.4770945725069898E-6</v>
+        <v>-3.4019366937590902E-6</v>
       </c>
       <c r="N27" s="8">
-        <v>-2.3712226015979299E-6</v>
+        <v>-2.6203158692545499E-6</v>
       </c>
       <c r="O27" s="8">
-        <v>-7.2015279948186899E-7</v>
+        <v>-1.4195240517000101E-6</v>
       </c>
       <c r="P27" s="8">
-        <v>-3.6190391913122701E-7</v>
+        <v>1.08003792716457E-7</v>
       </c>
       <c r="Q27" s="8">
-        <v>4.32723605173755E-6</v>
+        <v>6.0791082894465997E-6</v>
       </c>
       <c r="R27" s="8">
-        <v>-3.85206566010371E-7</v>
+        <v>3.2967375013854098E-7</v>
       </c>
       <c r="S27" s="8">
-        <v>-2.40755746117661E-6</v>
+        <v>-2.4172064832221799E-6</v>
       </c>
       <c r="T27" s="8">
-        <v>-6.3523162173816995E-7</v>
+        <v>-1.5749482770519299E-6</v>
       </c>
       <c r="U27" s="8">
-        <v>9.9531707865136996E-7</v>
+        <v>4.3895491149337898E-7</v>
       </c>
       <c r="V27" s="8">
-        <v>6.9973055967448603E-7</v>
+        <v>3.1611865645414502E-7</v>
       </c>
       <c r="W27" s="8">
-        <v>1.05914080754865E-6</v>
+        <v>1.05480574777121E-6</v>
       </c>
       <c r="X27" s="8">
-        <v>2.29593528240283E-6</v>
+        <v>2.1344625515066801E-6</v>
       </c>
       <c r="Y27" s="8">
-        <v>1.50544835564094E-8</v>
+        <v>-1.04691264626086E-7</v>
       </c>
       <c r="Z27" s="8">
-        <v>-3.52323561291942E-7</v>
+        <v>-3.6573957757971702E-7</v>
       </c>
       <c r="AA27" s="8">
-        <v>6.1210753017434302E-9</v>
+        <v>6.9132346830288197E-9</v>
       </c>
       <c r="AB27" s="8">
-        <v>8.6044931768418205E-6</v>
+        <v>1.0418663537171999E-5</v>
       </c>
       <c r="AC27" s="8">
-        <v>4.8400922793545499E-7</v>
+        <v>5.6560584577999205E-7</v>
       </c>
       <c r="AD27" s="8">
-        <v>8.3881869935954499E-6</v>
+        <v>1.02766494514438E-5</v>
       </c>
       <c r="AE27" s="8">
-        <v>-1.17206090624502E-4</v>
+        <v>-1.41865162949764E-4</v>
       </c>
     </row>
     <row r="28" spans="1:31" x14ac:dyDescent="0.25">
@@ -7347,94 +7347,94 @@
         <v>50</v>
       </c>
       <c r="B28" s="8">
-        <v>-5.5512248208991401E-2</v>
+        <v>-5.51414225038949E-2</v>
       </c>
       <c r="C28" s="8">
-        <v>1.78226410581721E-6</v>
+        <v>2.1251460495041098E-6</v>
       </c>
       <c r="D28" s="8">
-        <v>3.8572680684296296E-6</v>
+        <v>4.3413988867913702E-6</v>
       </c>
       <c r="E28" s="8">
-        <v>-3.5091664866875298E-7</v>
+        <v>-4.9403178871451397E-7</v>
       </c>
       <c r="F28" s="8">
-        <v>-8.7565731745256198E-7</v>
+        <v>-8.8823586269393703E-7</v>
       </c>
       <c r="G28" s="8">
-        <v>-5.6668883152103797E-7</v>
+        <v>-4.8435834400380895E-7</v>
       </c>
       <c r="H28" s="8">
-        <v>-1.23893189632272E-6</v>
+        <v>-1.47788742481273E-6</v>
       </c>
       <c r="I28" s="8">
-        <v>-1.11565094254127E-6</v>
+        <v>-1.2703351873162499E-6</v>
       </c>
       <c r="J28" s="8">
-        <v>-2.3905009615432402E-6</v>
+        <v>-2.8497022323475301E-6</v>
       </c>
       <c r="K28" s="8">
-        <v>-1.3962082477912201E-6</v>
+        <v>-1.5945129661537801E-6</v>
       </c>
       <c r="L28" s="8">
-        <v>-1.8362383144126799E-6</v>
+        <v>-2.1073328005879299E-6</v>
       </c>
       <c r="M28" s="8">
-        <v>-2.1280198036761101E-7</v>
+        <v>-1.6643838646635601E-7</v>
       </c>
       <c r="N28" s="8">
-        <v>-1.14107054237594E-6</v>
+        <v>-1.32505428609314E-6</v>
       </c>
       <c r="O28" s="8">
-        <v>-6.5869545494226599E-7</v>
+        <v>-4.2340734423215199E-7</v>
       </c>
       <c r="P28" s="8">
-        <v>1.3826337980897599E-7</v>
+        <v>4.0612989300254797E-8</v>
       </c>
       <c r="Q28" s="8">
-        <v>-2.0474639855476699E-6</v>
+        <v>-2.5556461319865701E-6</v>
       </c>
       <c r="R28" s="8">
-        <v>-1.92370469454462E-7</v>
+        <v>-3.9180601223586898E-7</v>
       </c>
       <c r="S28" s="8">
-        <v>5.5415978971095695E-7</v>
+        <v>6.1002342600027205E-7</v>
       </c>
       <c r="T28" s="8">
-        <v>-7.9574462340996304E-7</v>
+        <v>-7.3721064632517403E-7</v>
       </c>
       <c r="U28" s="8">
-        <v>-3.2592074558167801E-7</v>
+        <v>-4.2427498088028702E-7</v>
       </c>
       <c r="V28" s="8">
-        <v>-4.6478548740327398E-7</v>
+        <v>-6.7520325707067597E-7</v>
       </c>
       <c r="W28" s="8">
-        <v>-1.2237123332555901E-6</v>
+        <v>-1.5233223652456701E-6</v>
       </c>
       <c r="X28" s="8">
-        <v>-1.7896033229644601E-6</v>
+        <v>-2.10778213698244E-6</v>
       </c>
       <c r="Y28" s="8">
-        <v>-4.8749717131876203E-8</v>
+        <v>1.9117712640044601E-8</v>
       </c>
       <c r="Z28" s="8">
-        <v>-3.3814954034462999E-7</v>
+        <v>-4.1793257396012402E-7</v>
       </c>
       <c r="AA28" s="8">
-        <v>5.8975396229339404E-9</v>
+        <v>7.0457598686589896E-9</v>
       </c>
       <c r="AB28" s="8">
-        <v>4.8400922793545499E-7</v>
+        <v>5.6560584577999205E-7</v>
       </c>
       <c r="AC28" s="8">
-        <v>1.3538114266097801E-6</v>
+        <v>1.5956473406324001E-6</v>
       </c>
       <c r="AD28" s="8">
-        <v>-1.68541188471055E-7</v>
+        <v>-2.93388171338196E-7</v>
       </c>
       <c r="AE28" s="8">
-        <v>-7.1271563733205098E-5</v>
+        <v>-8.4235765194742295E-5</v>
       </c>
     </row>
     <row r="29" spans="1:31" x14ac:dyDescent="0.25">
@@ -7442,94 +7442,94 @@
         <v>4</v>
       </c>
       <c r="B29" s="8">
-        <v>-0.44871074747336698</v>
+        <v>-0.44139471763670501</v>
       </c>
       <c r="C29" s="8">
-        <v>-3.0175895987922599E-6</v>
+        <v>-1.9128150086190201E-6</v>
       </c>
       <c r="D29" s="8">
-        <v>1.5613719487008001E-5</v>
+        <v>2.25295374613286E-5</v>
       </c>
       <c r="E29" s="8">
-        <v>-3.5306746234211701E-6</v>
+        <v>-5.7051324325327504E-6</v>
       </c>
       <c r="F29" s="8">
-        <v>-6.3180303899050102E-6</v>
+        <v>-6.9770188772042104E-6</v>
       </c>
       <c r="G29" s="8">
-        <v>-1.7288507969710001E-5</v>
+        <v>-1.70374440643536E-5</v>
       </c>
       <c r="H29" s="8">
-        <v>-5.3886009459041703E-6</v>
+        <v>-3.5177038467101101E-6</v>
       </c>
       <c r="I29" s="8">
-        <v>1.9934169083980701E-6</v>
+        <v>8.1542893743484107E-6</v>
       </c>
       <c r="J29" s="8">
-        <v>9.8637187167365297E-6</v>
+        <v>1.39895452850547E-5</v>
       </c>
       <c r="K29" s="8">
-        <v>-2.0619336032878901E-6</v>
+        <v>1.3448601534204401E-6</v>
       </c>
       <c r="L29" s="8">
-        <v>3.0558602225527002E-6</v>
+        <v>1.0200241825056899E-5</v>
       </c>
       <c r="M29" s="8">
-        <v>-8.67647462065072E-6</v>
+        <v>-7.4381384278055399E-6</v>
       </c>
       <c r="N29" s="8">
-        <v>-6.1454669693396202E-6</v>
+        <v>-4.9611933504497303E-6</v>
       </c>
       <c r="O29" s="8">
-        <v>1.1550375042323801E-5</v>
+        <v>1.40510150203083E-5</v>
       </c>
       <c r="P29" s="8">
-        <v>1.9509696246996999E-5</v>
+        <v>2.2312841529307998E-5</v>
       </c>
       <c r="Q29" s="8">
-        <v>1.4837851068342901E-5</v>
+        <v>2.01561690940573E-5</v>
       </c>
       <c r="R29" s="8">
-        <v>-1.6105896076746599E-5</v>
+        <v>-1.97430502566085E-5</v>
       </c>
       <c r="S29" s="8">
-        <v>6.6251454878027795E-5</v>
+        <v>7.7126497176866198E-5</v>
       </c>
       <c r="T29" s="8">
-        <v>-9.3157366746979495E-6</v>
+        <v>-9.0163730052424107E-6</v>
       </c>
       <c r="U29" s="8">
-        <v>-1.4135019686785101E-6</v>
+        <v>-2.3246166410971702E-6</v>
       </c>
       <c r="V29" s="8">
-        <v>-2.8050407074725201E-6</v>
+        <v>-3.7027571161401702E-6</v>
       </c>
       <c r="W29" s="8">
-        <v>-5.42418415515061E-6</v>
+        <v>-5.8971570598778703E-6</v>
       </c>
       <c r="X29" s="8">
-        <v>-1.32007956271289E-5</v>
+        <v>-1.56869463954917E-5</v>
       </c>
       <c r="Y29" s="8">
-        <v>4.01314544029872E-7</v>
+        <v>7.5244011205111602E-7</v>
       </c>
       <c r="Z29" s="8">
-        <v>2.9400583148254502E-7</v>
+        <v>3.1822258948493501E-7</v>
       </c>
       <c r="AA29" s="8">
-        <v>-1.12901224784365E-8</v>
+        <v>-1.2779040095727899E-8</v>
       </c>
       <c r="AB29" s="8">
-        <v>8.3881869935954499E-6</v>
+        <v>1.02766494514438E-5</v>
       </c>
       <c r="AC29" s="8">
-        <v>-1.68541188471055E-7</v>
+        <v>-2.93388171338196E-7</v>
       </c>
       <c r="AD29" s="8">
-        <v>3.9728325592211798E-4</v>
+        <v>4.6776097726605802E-4</v>
       </c>
       <c r="AE29" s="8">
-        <v>-2.8216205491348497E-4</v>
+        <v>-3.4106762755969298E-4</v>
       </c>
     </row>
     <row r="30" spans="1:31" x14ac:dyDescent="0.25">
@@ -7537,94 +7537,94 @@
         <v>8</v>
       </c>
       <c r="B30" s="8">
-        <v>7.6113041729709003</v>
+        <v>7.5327132209720302</v>
       </c>
       <c r="C30" s="8">
-        <v>-5.4423565653146603E-4</v>
+        <v>-6.0671325234516705E-4</v>
       </c>
       <c r="D30" s="8">
-        <v>-8.3290283417442003E-4</v>
+        <v>-9.6085385193366804E-4</v>
       </c>
       <c r="E30" s="8">
-        <v>-9.2716630111859696E-4</v>
+        <v>-1.12083588291062E-3</v>
       </c>
       <c r="F30" s="8">
-        <v>-9.8121077930040301E-4</v>
+        <v>-1.1979880361858901E-3</v>
       </c>
       <c r="G30" s="8">
-        <v>-1.0252062148062601E-3</v>
+        <v>-1.28786286519915E-3</v>
       </c>
       <c r="H30" s="8">
-        <v>-9.46868246233951E-4</v>
+        <v>-1.1607506186542299E-3</v>
       </c>
       <c r="I30" s="8">
-        <v>-9.4153885507760205E-4</v>
+        <v>-1.18797263085647E-3</v>
       </c>
       <c r="J30" s="8">
-        <v>-9.1321204151468096E-4</v>
+        <v>-1.1193177506530899E-3</v>
       </c>
       <c r="K30" s="8">
-        <v>-9.7214891034458199E-4</v>
+        <v>-1.19392147305834E-3</v>
       </c>
       <c r="L30" s="8">
-        <v>-9.7367395144997305E-4</v>
+        <v>-1.21760671370202E-3</v>
       </c>
       <c r="M30" s="8">
-        <v>-1.01258741841183E-3</v>
+        <v>-1.2731586149253901E-3</v>
       </c>
       <c r="N30" s="8">
-        <v>-9.3059806897005605E-4</v>
+        <v>-1.1148422422248799E-3</v>
       </c>
       <c r="O30" s="8">
-        <v>-9.9301734847927702E-4</v>
+        <v>-1.2355023172130101E-3</v>
       </c>
       <c r="P30" s="8">
-        <v>-6.2722640802023505E-4</v>
+        <v>-7.24661402033632E-4</v>
       </c>
       <c r="Q30" s="8">
-        <v>-1.01398648324365E-4</v>
+        <v>-1.7533681058695E-4</v>
       </c>
       <c r="R30" s="8">
-        <v>-1.74327434238358E-3</v>
+        <v>-2.02747983557493E-3</v>
       </c>
       <c r="S30" s="8">
-        <v>-4.8300055975499298E-4</v>
+        <v>-5.8930728573233597E-4</v>
       </c>
       <c r="T30" s="8">
-        <v>-2.9285221741463498E-4</v>
+        <v>-3.2003691452027298E-4</v>
       </c>
       <c r="U30" s="8">
-        <v>-5.0830524459590995E-4</v>
+        <v>-6.0343873500080401E-4</v>
       </c>
       <c r="V30" s="8">
-        <v>-5.5009015460508301E-4</v>
+        <v>-6.4662214277764096E-4</v>
       </c>
       <c r="W30" s="8">
-        <v>-5.7855919248601603E-4</v>
+        <v>-6.8990241620984203E-4</v>
       </c>
       <c r="X30" s="8">
-        <v>-6.9069536585095203E-4</v>
+        <v>-8.1528135790835102E-4</v>
       </c>
       <c r="Y30" s="8">
-        <v>-1.3216703652810699E-4</v>
+        <v>-1.5302013977393599E-4</v>
       </c>
       <c r="Z30" s="8">
-        <v>-2.6492355287693702E-4</v>
+        <v>-3.2109578282953202E-4</v>
       </c>
       <c r="AA30" s="8">
-        <v>2.32104981362895E-6</v>
+        <v>2.8115420070873301E-6</v>
       </c>
       <c r="AB30" s="8">
-        <v>-1.17206090624502E-4</v>
+        <v>-1.41865162949764E-4</v>
       </c>
       <c r="AC30" s="8">
-        <v>-7.1271563733205098E-5</v>
+        <v>-8.4235765194742295E-5</v>
       </c>
       <c r="AD30" s="8">
-        <v>-2.8216205491348497E-4</v>
+        <v>-3.4106762755969298E-4</v>
       </c>
       <c r="AE30" s="8">
-        <v>1.6358261251644499E-2</v>
+        <v>1.9665745745903001E-2</v>
       </c>
     </row>
   </sheetData>
@@ -7634,7 +7634,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0CE9B1D-DDDD-4CC5-B8EB-BE67C12DCD75}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B47509E5-1D6F-4320-9093-19C3760C2BB0}">
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -7682,10 +7682,10 @@
         <v>9</v>
       </c>
       <c r="B2" s="8">
-        <v>2.76096156880056</v>
+        <v>2.7622687751800701</v>
       </c>
       <c r="C2" s="8">
-        <v>3.1702156572194898E-2</v>
+        <v>3.3858357918848003E-2</v>
       </c>
       <c r="D2" s="8">
         <v>0</v>
@@ -7714,13 +7714,13 @@
         <v>10</v>
       </c>
       <c r="B3" s="8">
-        <v>1.21110374615701E-2</v>
+        <v>-3.5538705948887798E-2</v>
       </c>
       <c r="C3" s="8">
         <v>0</v>
       </c>
       <c r="D3" s="8">
-        <v>2.0699342854157001E-2</v>
+        <v>2.2439382908269301E-2</v>
       </c>
       <c r="E3" s="8">
         <v>0</v>
@@ -7746,7 +7746,7 @@
         <v>11</v>
       </c>
       <c r="B4" s="8">
-        <v>2.41968210914537</v>
+        <v>2.4179001655162198</v>
       </c>
       <c r="C4" s="8">
         <v>0</v>
@@ -7755,7 +7755,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="8">
-        <v>4.5360562581079497E-2</v>
+        <v>4.7363239388380697E-2</v>
       </c>
       <c r="F4" s="8">
         <v>0</v>
@@ -7778,7 +7778,7 @@
         <v>12</v>
       </c>
       <c r="B5" s="8">
-        <v>0.32639751224881902</v>
+        <v>0.28837240198177899</v>
       </c>
       <c r="C5" s="8">
         <v>0</v>
@@ -7790,7 +7790,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="8">
-        <v>1.0677563461392699E-2</v>
+        <v>1.1776504736085399E-2</v>
       </c>
       <c r="G5" s="8">
         <v>0</v>
@@ -7810,7 +7810,7 @@
         <v>13</v>
       </c>
       <c r="B6" s="8">
-        <v>-1.59858668478833E-2</v>
+        <v>-3.471549104748E-2</v>
       </c>
       <c r="C6" s="8">
         <v>0</v>
@@ -7825,7 +7825,7 @@
         <v>0</v>
       </c>
       <c r="G6" s="8">
-        <v>1.9411499770913599E-2</v>
+        <v>2.1546619803242399E-2</v>
       </c>
       <c r="H6" s="8">
         <v>0</v>
@@ -7842,7 +7842,7 @@
         <v>14</v>
       </c>
       <c r="B7" s="8">
-        <v>0.40266992085993503</v>
+        <v>0.40218945718307902</v>
       </c>
       <c r="C7" s="8">
         <v>0</v>
@@ -7860,7 +7860,7 @@
         <v>0</v>
       </c>
       <c r="H7" s="8">
-        <v>2.9237827439913398E-2</v>
+        <v>3.19895238680055E-2</v>
       </c>
       <c r="I7" s="8">
         <v>0</v>
@@ -7874,7 +7874,7 @@
         <v>41</v>
       </c>
       <c r="B8" s="8">
-        <v>-1.0066024348329599E-2</v>
+        <v>-3.7644918767706799E-3</v>
       </c>
       <c r="C8" s="8">
         <v>0</v>
@@ -7895,7 +7895,7 @@
         <v>0</v>
       </c>
       <c r="I8" s="8">
-        <v>2.0598632667642299E-3</v>
+        <v>2.0772674429183399E-3</v>
       </c>
       <c r="J8" s="8">
         <v>0</v>
@@ -7906,7 +7906,7 @@
         <v>42</v>
       </c>
       <c r="B9" s="8">
-        <v>0.10115236592971399</v>
+        <v>0.105920616998777</v>
       </c>
       <c r="C9" s="8">
         <v>0</v>
@@ -7930,7 +7930,7 @@
         <v>0</v>
       </c>
       <c r="J9" s="8">
-        <v>1.4002819815411599E-3</v>
+        <v>1.5080772364612E-3</v>
       </c>
     </row>
   </sheetData>
@@ -7940,7 +7940,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7ECBB36B-232F-4A31-8AEF-9D7CFD3EA13C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{618F5F34-CE9A-4B0D-ADBB-1E566DDF28EA}">
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -7988,10 +7988,10 @@
         <v>9</v>
       </c>
       <c r="B2" s="8">
-        <v>1.6728629358760601</v>
+        <v>1.63854829591822</v>
       </c>
       <c r="C2" s="8">
-        <v>1.88914780318034E-2</v>
+        <v>2.0721283089929401E-2</v>
       </c>
       <c r="D2" s="8">
         <v>0</v>
@@ -8020,13 +8020,13 @@
         <v>10</v>
       </c>
       <c r="B3" s="8">
-        <v>-0.44548319657449997</v>
+        <v>-0.48559234836281201</v>
       </c>
       <c r="C3" s="8">
         <v>0</v>
       </c>
       <c r="D3" s="8">
-        <v>1.05565532877994E-2</v>
+        <v>1.1651368337091799E-2</v>
       </c>
       <c r="E3" s="8">
         <v>0</v>
@@ -8052,7 +8052,7 @@
         <v>11</v>
       </c>
       <c r="B4" s="8">
-        <v>0.95169013463812901</v>
+        <v>0.95419874562846696</v>
       </c>
       <c r="C4" s="8">
         <v>0</v>
@@ -8061,7 +8061,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="8">
-        <v>1.58763588328691E-2</v>
+        <v>1.6899289364673099E-2</v>
       </c>
       <c r="F4" s="8">
         <v>0</v>
@@ -8084,7 +8084,7 @@
         <v>12</v>
       </c>
       <c r="B5" s="8">
-        <v>0.26998623449775999</v>
+        <v>0.31066186805058998</v>
       </c>
       <c r="C5" s="8">
         <v>0</v>
@@ -8096,7 +8096,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="8">
-        <v>8.6524145528497493E-3</v>
+        <v>9.4749852583087199E-3</v>
       </c>
       <c r="G5" s="8">
         <v>0</v>
@@ -8116,7 +8116,7 @@
         <v>13</v>
       </c>
       <c r="B6" s="8">
-        <v>0.17229506571213199</v>
+        <v>0.21691732939406599</v>
       </c>
       <c r="C6" s="8">
         <v>0</v>
@@ -8131,7 +8131,7 @@
         <v>0</v>
       </c>
       <c r="G6" s="8">
-        <v>1.49355892382081E-2</v>
+        <v>1.6193911596461101E-2</v>
       </c>
       <c r="H6" s="8">
         <v>0</v>
@@ -8148,7 +8148,7 @@
         <v>14</v>
       </c>
       <c r="B7" s="8">
-        <v>0.34862296068892401</v>
+        <v>0.357628432789794</v>
       </c>
       <c r="C7" s="8">
         <v>0</v>
@@ -8166,7 +8166,7 @@
         <v>0</v>
       </c>
       <c r="H7" s="8">
-        <v>2.1201649772745499E-2</v>
+        <v>2.2852384035043499E-2</v>
       </c>
       <c r="I7" s="8">
         <v>0</v>
@@ -8180,7 +8180,7 @@
         <v>41</v>
       </c>
       <c r="B8" s="8">
-        <v>-0.11917880969466001</v>
+        <v>-0.12724822008849901</v>
       </c>
       <c r="C8" s="8">
         <v>0</v>
@@ -8201,7 +8201,7 @@
         <v>0</v>
       </c>
       <c r="I8" s="8">
-        <v>2.5261878188393501E-3</v>
+        <v>2.7320666605839001E-3</v>
       </c>
       <c r="J8" s="8">
         <v>0</v>
@@ -8212,7 +8212,7 @@
         <v>42</v>
       </c>
       <c r="B9" s="8">
-        <v>7.3629113682714104E-2</v>
+        <v>6.8646120858877696E-2</v>
       </c>
       <c r="C9" s="8">
         <v>0</v>
@@ -8236,7 +8236,7 @@
         <v>0</v>
       </c>
       <c r="J9" s="8">
-        <v>1.50493246916382E-3</v>
+        <v>1.65004864511128E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
longitudinal weighting in regressions
</commit_message>
<xml_diff>
--- a/input/reg_health_mental.xlsx
+++ b/input/reg_health_mental.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\andy_local\SimPaths project files\SimPaths\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E39558C1-59CF-44AF-94E9-2ECEEAEE101C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AF27609-5500-4E8F-A059-053D7C9F8DB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="2" r:id="rId1"/>
@@ -18,9 +18,9 @@
     <sheet name="UK_HM1_C" sheetId="7" r:id="rId3"/>
     <sheet name="UK_HM2_Males_C" sheetId="8" r:id="rId4"/>
     <sheet name="UK_HM2_Females_C" sheetId="9" r:id="rId5"/>
-    <sheet name="UK_HM1_L" sheetId="22" r:id="rId6"/>
-    <sheet name="UK_HM2_Males_L" sheetId="23" r:id="rId7"/>
-    <sheet name="UK_HM2_Females_L" sheetId="24" r:id="rId8"/>
+    <sheet name="UK_HM1_L" sheetId="25" r:id="rId6"/>
+    <sheet name="UK_HM2_Males_L" sheetId="26" r:id="rId7"/>
+    <sheet name="UK_HM2_Females_L" sheetId="27" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -4766,10 +4766,12 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD05762E-8E4A-4531-8778-2DDE3401ADAE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C367505C-FD84-46B3-9749-6444C1C58A26}">
   <dimension ref="A1:AE30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4877,94 +4879,94 @@
         <v>19</v>
       </c>
       <c r="B2" s="8">
-        <v>5.6748988544512704E-3</v>
+        <v>5.6069252495916502E-2</v>
       </c>
       <c r="C2" s="8">
-        <v>6.3126110626850901E-4</v>
+        <v>1.7242242921609999E-3</v>
       </c>
       <c r="D2" s="8">
-        <v>4.6396264246978099E-4</v>
+        <v>1.2249060768207099E-3</v>
       </c>
       <c r="E2" s="8">
-        <v>-1.3004541165257099E-4</v>
+        <v>-6.1874977376915003E-4</v>
       </c>
       <c r="F2" s="8">
-        <v>-9.6397417107954396E-5</v>
+        <v>-5.6039354151771702E-4</v>
       </c>
       <c r="G2" s="8">
-        <v>-8.1400804213283898E-5</v>
+        <v>-4.8636158035493001E-4</v>
       </c>
       <c r="H2" s="8">
-        <v>-1.25125408959879E-4</v>
+        <v>-6.3972541248677396E-4</v>
       </c>
       <c r="I2" s="8">
-        <v>-8.5622027362546E-5</v>
+        <v>-6.9331915164336201E-4</v>
       </c>
       <c r="J2" s="8">
-        <v>-9.4587619678724195E-5</v>
+        <v>-5.0078457317077104E-4</v>
       </c>
       <c r="K2" s="8">
-        <v>-7.4270576203027097E-5</v>
+        <v>-5.3208810089653603E-4</v>
       </c>
       <c r="L2" s="8">
-        <v>-9.2852913357332201E-5</v>
+        <v>-5.3880278431581402E-4</v>
       </c>
       <c r="M2" s="8">
-        <v>-9.7723831375078806E-5</v>
+        <v>-4.65112377182801E-4</v>
       </c>
       <c r="N2" s="8">
-        <v>-8.9147371597648803E-5</v>
+        <v>-3.72883661111065E-4</v>
       </c>
       <c r="O2" s="8">
-        <v>-9.6704789632620197E-5</v>
+        <v>-4.37032558332609E-4</v>
       </c>
       <c r="P2" s="8">
-        <v>-3.35944138396503E-6</v>
+        <v>6.3804742647886601E-5</v>
       </c>
       <c r="Q2" s="8">
-        <v>2.6694639089029299E-5</v>
+        <v>1.00876290308307E-4</v>
       </c>
       <c r="R2" s="8">
-        <v>-3.4739667835109602E-5</v>
+        <v>-8.8051519685915694E-5</v>
       </c>
       <c r="S2" s="8">
-        <v>-9.9279137317001898E-6</v>
+        <v>-3.1808198852995001E-5</v>
       </c>
       <c r="T2" s="8">
-        <v>-4.1350089656322197E-5</v>
+        <v>-2.6176963639023702E-4</v>
       </c>
       <c r="U2" s="8">
-        <v>1.91318083550039E-6</v>
+        <v>-1.22682453199426E-4</v>
       </c>
       <c r="V2" s="8">
-        <v>3.3041349502523199E-6</v>
+        <v>-5.1328063897944601E-5</v>
       </c>
       <c r="W2" s="8">
-        <v>4.6952328925989297E-5</v>
+        <v>1.37808615346704E-5</v>
       </c>
       <c r="X2" s="8">
-        <v>1.26673590139778E-4</v>
+        <v>2.6670464367964402E-4</v>
       </c>
       <c r="Y2" s="8">
-        <v>4.5839887235734501E-6</v>
+        <v>2.2311736444310899E-5</v>
       </c>
       <c r="Z2" s="8">
-        <v>1.45013491727407E-6</v>
+        <v>-9.4898716168457208E-6</v>
       </c>
       <c r="AA2" s="8">
-        <v>-2.47772683099099E-8</v>
+        <v>4.0925599950415701E-8</v>
       </c>
       <c r="AB2" s="8">
-        <v>4.2520475251047098E-6</v>
+        <v>2.5991923536983598E-5</v>
       </c>
       <c r="AC2" s="8">
-        <v>2.1251460495041098E-6</v>
+        <v>7.40382263859905E-6</v>
       </c>
       <c r="AD2" s="8">
-        <v>-1.9128150086190201E-6</v>
+        <v>-4.8026066892916801E-5</v>
       </c>
       <c r="AE2" s="8">
-        <v>-6.0671325234516705E-4</v>
+        <v>-1.3114087070277801E-3</v>
       </c>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.25">
@@ -4972,94 +4974,94 @@
         <v>20</v>
       </c>
       <c r="B3" s="8">
-        <v>4.58104364426219E-2</v>
+        <v>7.5473547908416094E-2</v>
       </c>
       <c r="C3" s="8">
-        <v>4.6396264246978099E-4</v>
+        <v>1.2249060768207099E-3</v>
       </c>
       <c r="D3" s="8">
-        <v>1.31059947545629E-3</v>
+        <v>3.4842597268040301E-3</v>
       </c>
       <c r="E3" s="8">
-        <v>-9.4289079430570294E-5</v>
+        <v>-6.5588943879255502E-4</v>
       </c>
       <c r="F3" s="8">
-        <v>-6.0208371812228003E-5</v>
+        <v>-4.1427058968705299E-4</v>
       </c>
       <c r="G3" s="8">
-        <v>-7.0781895239614901E-5</v>
+        <v>-3.4362202397918498E-4</v>
       </c>
       <c r="H3" s="8">
-        <v>-1.2473366291214101E-4</v>
+        <v>-5.1244344269862701E-4</v>
       </c>
       <c r="I3" s="8">
-        <v>-9.3338907756125307E-5</v>
+        <v>-7.2754453798821897E-4</v>
       </c>
       <c r="J3" s="8">
-        <v>-9.4309582073782804E-5</v>
+        <v>-5.2287959432338398E-4</v>
       </c>
       <c r="K3" s="8">
-        <v>-4.4411074543662501E-5</v>
+        <v>-4.2703408787423297E-4</v>
       </c>
       <c r="L3" s="8">
-        <v>-5.4190283143972801E-5</v>
+        <v>-3.5904815545663199E-4</v>
       </c>
       <c r="M3" s="8">
-        <v>-9.2512056332152902E-5</v>
+        <v>-5.12542980716846E-4</v>
       </c>
       <c r="N3" s="8">
-        <v>-4.3534145061445298E-5</v>
+        <v>-1.58026282325078E-4</v>
       </c>
       <c r="O3" s="8">
-        <v>-1.3578467718021399E-4</v>
+        <v>-7.2809303475764801E-4</v>
       </c>
       <c r="P3" s="8">
-        <v>3.2340782466820501E-6</v>
+        <v>5.8319911090376397E-5</v>
       </c>
       <c r="Q3" s="8">
-        <v>9.1837794212754694E-5</v>
+        <v>2.9892894561407701E-4</v>
       </c>
       <c r="R3" s="8">
-        <v>-4.24053282701221E-6</v>
+        <v>1.3495870467713901E-4</v>
       </c>
       <c r="S3" s="8">
-        <v>-2.13462856629145E-6</v>
+        <v>-1.669246459867E-5</v>
       </c>
       <c r="T3" s="8">
-        <v>-1.42209370920578E-5</v>
+        <v>-1.53762168743298E-4</v>
       </c>
       <c r="U3" s="8">
-        <v>3.5814952747186198E-5</v>
+        <v>-1.5661594761741801E-5</v>
       </c>
       <c r="V3" s="8">
-        <v>8.9611846726394003E-5</v>
+        <v>1.8177208523987001E-4</v>
       </c>
       <c r="W3" s="8">
-        <v>1.6642486668752901E-4</v>
+        <v>3.6057120221624198E-4</v>
       </c>
       <c r="X3" s="8">
-        <v>2.72846330738831E-4</v>
+        <v>6.8757980451412504E-4</v>
       </c>
       <c r="Y3" s="8">
-        <v>1.32370347400556E-5</v>
+        <v>5.7439378178796598E-5</v>
       </c>
       <c r="Z3" s="8">
-        <v>4.93913349409411E-6</v>
+        <v>2.8524472822873699E-5</v>
       </c>
       <c r="AA3" s="8">
-        <v>-1.2776962150714601E-7</v>
+        <v>-5.1436043815626398E-7</v>
       </c>
       <c r="AB3" s="8">
-        <v>2.6595676599196199E-6</v>
+        <v>2.2496862997745398E-5</v>
       </c>
       <c r="AC3" s="8">
-        <v>4.3413988867913702E-6</v>
+        <v>6.8988713607926301E-6</v>
       </c>
       <c r="AD3" s="8">
-        <v>2.25295374613286E-5</v>
+        <v>5.77422874847142E-5</v>
       </c>
       <c r="AE3" s="8">
-        <v>-9.6085385193366804E-4</v>
+        <v>-2.8149845667864602E-3</v>
       </c>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.25">
@@ -5067,94 +5069,94 @@
         <v>23</v>
       </c>
       <c r="B4" s="8">
-        <v>5.7585650605830097E-2</v>
+        <v>-7.5284067388650996E-2</v>
       </c>
       <c r="C4" s="8">
-        <v>-1.3004541165257099E-4</v>
+        <v>-6.1874977376915003E-4</v>
       </c>
       <c r="D4" s="8">
-        <v>-9.4289079430570294E-5</v>
+        <v>-6.5588943879255502E-4</v>
       </c>
       <c r="E4" s="8">
-        <v>4.2421007873033297E-3</v>
+        <v>1.2552883948655899E-2</v>
       </c>
       <c r="F4" s="8">
-        <v>1.30136794406968E-3</v>
+        <v>4.6586135347700102E-3</v>
       </c>
       <c r="G4" s="8">
-        <v>1.2982998800629699E-3</v>
+        <v>4.6619426744457298E-3</v>
       </c>
       <c r="H4" s="8">
-        <v>1.3094530308266801E-3</v>
+        <v>4.6953924011125204E-3</v>
       </c>
       <c r="I4" s="8">
-        <v>1.30494669899701E-3</v>
+        <v>4.7295446316709703E-3</v>
       </c>
       <c r="J4" s="8">
-        <v>1.29621750655437E-3</v>
+        <v>4.5867728662137798E-3</v>
       </c>
       <c r="K4" s="8">
-        <v>1.2886934092175401E-3</v>
+        <v>4.5851698551151602E-3</v>
       </c>
       <c r="L4" s="8">
-        <v>1.3066161794066499E-3</v>
+        <v>4.6522920331823403E-3</v>
       </c>
       <c r="M4" s="8">
-        <v>1.3189121274853801E-3</v>
+        <v>4.7474925607503098E-3</v>
       </c>
       <c r="N4" s="8">
-        <v>1.3026680835184199E-3</v>
+        <v>4.6017362528768396E-3</v>
       </c>
       <c r="O4" s="8">
-        <v>1.3041465695219901E-3</v>
+        <v>4.6812021264640404E-3</v>
       </c>
       <c r="P4" s="8">
-        <v>-2.75340398856397E-6</v>
+        <v>-1.14913679032E-4</v>
       </c>
       <c r="Q4" s="8">
-        <v>-1.40446383635702E-4</v>
+        <v>-5.3075190912500703E-4</v>
       </c>
       <c r="R4" s="8">
-        <v>6.8412831530912995E-5</v>
+        <v>2.1918894876310301E-4</v>
       </c>
       <c r="S4" s="8">
-        <v>-1.20138070365011E-5</v>
+        <v>1.00391979662983E-4</v>
       </c>
       <c r="T4" s="8">
-        <v>4.7438658382716498E-5</v>
+        <v>8.0537439077581996E-5</v>
       </c>
       <c r="U4" s="8">
-        <v>2.79489533657508E-6</v>
+        <v>-2.2737114469953E-4</v>
       </c>
       <c r="V4" s="8">
-        <v>2.2573849262117901E-5</v>
+        <v>-2.83534469208249E-5</v>
       </c>
       <c r="W4" s="8">
-        <v>5.2391126157177499E-5</v>
+        <v>-1.09671859748506E-4</v>
       </c>
       <c r="X4" s="8">
-        <v>8.9592986289246894E-5</v>
+        <v>1.9093646054300299E-4</v>
       </c>
       <c r="Y4" s="8">
-        <v>3.1332567222028001E-6</v>
+        <v>-3.82994438180937E-5</v>
       </c>
       <c r="Z4" s="8">
-        <v>7.68817234143558E-7</v>
+        <v>4.4985635076731103E-6</v>
       </c>
       <c r="AA4" s="8">
-        <v>-1.6172177507542401E-8</v>
+        <v>-3.7095477023163901E-8</v>
       </c>
       <c r="AB4" s="8">
-        <v>-3.80156139540954E-6</v>
+        <v>8.5625345480353595E-6</v>
       </c>
       <c r="AC4" s="8">
-        <v>-4.9403178871451397E-7</v>
+        <v>1.75452746457684E-6</v>
       </c>
       <c r="AD4" s="8">
-        <v>-5.7051324325327504E-6</v>
+        <v>9.7261481075393093E-5</v>
       </c>
       <c r="AE4" s="8">
-        <v>-1.12083588291062E-3</v>
+        <v>-3.5270488242725899E-3</v>
       </c>
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.25">
@@ -5162,94 +5164,94 @@
         <v>24</v>
       </c>
       <c r="B5" s="8">
-        <v>7.1134763037591101E-2</v>
+        <v>-0.100057026919231</v>
       </c>
       <c r="C5" s="8">
-        <v>-9.6397417107954396E-5</v>
+        <v>-5.6039354151771702E-4</v>
       </c>
       <c r="D5" s="8">
-        <v>-6.0208371812228003E-5</v>
+        <v>-4.1427058968705299E-4</v>
       </c>
       <c r="E5" s="8">
-        <v>1.30136794406968E-3</v>
+        <v>4.6586135347700102E-3</v>
       </c>
       <c r="F5" s="8">
-        <v>2.4701481765281698E-3</v>
+        <v>7.4128544696436503E-3</v>
       </c>
       <c r="G5" s="8">
-        <v>1.2923295063619401E-3</v>
+        <v>4.6339836579335101E-3</v>
       </c>
       <c r="H5" s="8">
-        <v>1.3000347035909399E-3</v>
+        <v>4.7040216373928599E-3</v>
       </c>
       <c r="I5" s="8">
-        <v>1.28907040787262E-3</v>
+        <v>4.7040736256787098E-3</v>
       </c>
       <c r="J5" s="8">
-        <v>1.2854996651937001E-3</v>
+        <v>4.5475338527812903E-3</v>
       </c>
       <c r="K5" s="8">
-        <v>1.2837201742287401E-3</v>
+        <v>4.5752739252167699E-3</v>
       </c>
       <c r="L5" s="8">
-        <v>1.2961002392839699E-3</v>
+        <v>4.6239097506404802E-3</v>
       </c>
       <c r="M5" s="8">
-        <v>1.2981937161402001E-3</v>
+        <v>4.7021186043901802E-3</v>
       </c>
       <c r="N5" s="8">
-        <v>1.2936548458679601E-3</v>
+        <v>4.5984331081739402E-3</v>
       </c>
       <c r="O5" s="8">
-        <v>1.28832358926761E-3</v>
+        <v>4.6573226722622704E-3</v>
       </c>
       <c r="P5" s="8">
-        <v>-2.71926192311181E-6</v>
+        <v>-2.0891575928672399E-4</v>
       </c>
       <c r="Q5" s="8">
-        <v>-1.27013501833536E-4</v>
+        <v>-5.8120856585848696E-4</v>
       </c>
       <c r="R5" s="8">
-        <v>8.7608382022937703E-5</v>
+        <v>3.5894655843644901E-4</v>
       </c>
       <c r="S5" s="8">
-        <v>-2.0077626985483901E-5</v>
+        <v>-2.3267827529382999E-4</v>
       </c>
       <c r="T5" s="8">
-        <v>5.5217612501320798E-5</v>
+        <v>4.0634834684957598E-4</v>
       </c>
       <c r="U5" s="8">
-        <v>-1.1855162827996501E-5</v>
+        <v>-5.5792132208191203E-5</v>
       </c>
       <c r="V5" s="8">
-        <v>-2.5019864470842898E-7</v>
+        <v>1.72448859064701E-5</v>
       </c>
       <c r="W5" s="8">
-        <v>1.3362115106098899E-5</v>
+        <v>-8.7808865050775895E-5</v>
       </c>
       <c r="X5" s="8">
-        <v>5.09529760875342E-5</v>
+        <v>2.0714690065796199E-4</v>
       </c>
       <c r="Y5" s="8">
-        <v>3.04745386287188E-6</v>
+        <v>-3.4986498382821998E-5</v>
       </c>
       <c r="Z5" s="8">
-        <v>4.2571390162228302E-6</v>
+        <v>3.3794828438001103E-5</v>
       </c>
       <c r="AA5" s="8">
-        <v>-4.27724312176736E-8</v>
+        <v>-2.3690207389474601E-7</v>
       </c>
       <c r="AB5" s="8">
-        <v>-4.1990539914227599E-6</v>
+        <v>-3.5368859764654901E-5</v>
       </c>
       <c r="AC5" s="8">
-        <v>-8.8823586269393703E-7</v>
+        <v>-3.0909265059234698E-7</v>
       </c>
       <c r="AD5" s="8">
-        <v>-6.9770188772042104E-6</v>
+        <v>1.53713222151612E-4</v>
       </c>
       <c r="AE5" s="8">
-        <v>-1.1979880361858901E-3</v>
+        <v>-3.9310536595509897E-3</v>
       </c>
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.25">
@@ -5257,94 +5259,94 @@
         <v>25</v>
       </c>
       <c r="B6" s="8">
-        <v>8.6622452509374198E-2</v>
+        <v>-5.6538402758405902E-2</v>
       </c>
       <c r="C6" s="8">
-        <v>-8.1400804213283898E-5</v>
+        <v>-4.8636158035493001E-4</v>
       </c>
       <c r="D6" s="8">
-        <v>-7.0781895239614901E-5</v>
+        <v>-3.4362202397918498E-4</v>
       </c>
       <c r="E6" s="8">
-        <v>1.2982998800629699E-3</v>
+        <v>4.6619426744457298E-3</v>
       </c>
       <c r="F6" s="8">
-        <v>1.2923295063619401E-3</v>
+        <v>4.6339836579335101E-3</v>
       </c>
       <c r="G6" s="8">
-        <v>2.7685921900003599E-3</v>
+        <v>9.4406822008959706E-3</v>
       </c>
       <c r="H6" s="8">
-        <v>1.29597561384749E-3</v>
+        <v>4.6437873015212298E-3</v>
       </c>
       <c r="I6" s="8">
-        <v>1.2941437470714899E-3</v>
+        <v>4.6905684461153096E-3</v>
       </c>
       <c r="J6" s="8">
-        <v>1.2850841153339799E-3</v>
+        <v>4.55757456725122E-3</v>
       </c>
       <c r="K6" s="8">
-        <v>1.2769342224300099E-3</v>
+        <v>4.5644297121687901E-3</v>
       </c>
       <c r="L6" s="8">
-        <v>1.29579702184705E-3</v>
+        <v>4.6257181545791603E-3</v>
       </c>
       <c r="M6" s="8">
-        <v>1.3049583145837401E-3</v>
+        <v>4.6956156273614798E-3</v>
       </c>
       <c r="N6" s="8">
-        <v>1.2902867839833501E-3</v>
+        <v>4.5761952720187998E-3</v>
       </c>
       <c r="O6" s="8">
-        <v>1.2925493656614001E-3</v>
+        <v>4.6245046333852702E-3</v>
       </c>
       <c r="P6" s="8">
-        <v>7.02354558046071E-6</v>
+        <v>-6.6421818947092994E-5</v>
       </c>
       <c r="Q6" s="8">
-        <v>-1.3232814886348501E-4</v>
+        <v>-3.6131142327128901E-4</v>
       </c>
       <c r="R6" s="8">
-        <v>9.4873922142014601E-5</v>
+        <v>4.3739155051898199E-4</v>
       </c>
       <c r="S6" s="8">
-        <v>-2.6096533285045499E-6</v>
+        <v>-9.2169724172065905E-5</v>
       </c>
       <c r="T6" s="8">
-        <v>7.1240931926224804E-5</v>
+        <v>3.0757428213766801E-4</v>
       </c>
       <c r="U6" s="8">
-        <v>2.11530738951042E-5</v>
+        <v>3.3486641410969298E-5</v>
       </c>
       <c r="V6" s="8">
-        <v>4.4813463677083998E-5</v>
+        <v>1.71640398250429E-4</v>
       </c>
       <c r="W6" s="8">
-        <v>6.0259661667862401E-5</v>
+        <v>1.09688348883064E-4</v>
       </c>
       <c r="X6" s="8">
-        <v>1.2557094002796701E-4</v>
+        <v>4.1452257141545799E-4</v>
       </c>
       <c r="Y6" s="8">
-        <v>1.4649771969649601E-6</v>
+        <v>-2.0452982035959601E-5</v>
       </c>
       <c r="Z6" s="8">
-        <v>5.2401916774154498E-6</v>
+        <v>2.5187695891426099E-5</v>
       </c>
       <c r="AA6" s="8">
-        <v>-4.5394718343653701E-8</v>
+        <v>-1.93505974880005E-7</v>
       </c>
       <c r="AB6" s="8">
-        <v>-4.1673943924848104E-6</v>
+        <v>1.28039239555633E-5</v>
       </c>
       <c r="AC6" s="8">
-        <v>-4.8435834400380895E-7</v>
+        <v>1.78258937571622E-7</v>
       </c>
       <c r="AD6" s="8">
-        <v>-1.70374440643536E-5</v>
+        <v>1.5001784691466401E-4</v>
       </c>
       <c r="AE6" s="8">
-        <v>-1.28786286519915E-3</v>
+        <v>-4.8546487627397104E-3</v>
       </c>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.25">
@@ -5352,94 +5354,94 @@
         <v>26</v>
       </c>
       <c r="B7" s="8">
-        <v>4.2575284947759001E-2</v>
+        <v>-0.117502551825893</v>
       </c>
       <c r="C7" s="8">
-        <v>-1.25125408959879E-4</v>
+        <v>-6.3972541248677396E-4</v>
       </c>
       <c r="D7" s="8">
-        <v>-1.2473366291214101E-4</v>
+        <v>-5.1244344269862701E-4</v>
       </c>
       <c r="E7" s="8">
-        <v>1.3094530308266801E-3</v>
+        <v>4.6953924011125204E-3</v>
       </c>
       <c r="F7" s="8">
-        <v>1.3000347035909399E-3</v>
+        <v>4.7040216373928599E-3</v>
       </c>
       <c r="G7" s="8">
-        <v>1.29597561384749E-3</v>
+        <v>4.6437873015212298E-3</v>
       </c>
       <c r="H7" s="8">
-        <v>2.7251852433988499E-3</v>
+        <v>7.7316708530574497E-3</v>
       </c>
       <c r="I7" s="8">
-        <v>1.3027014332871599E-3</v>
+        <v>4.7439120806390097E-3</v>
       </c>
       <c r="J7" s="8">
-        <v>1.29190877873002E-3</v>
+        <v>4.5792839866289599E-3</v>
       </c>
       <c r="K7" s="8">
-        <v>1.28652734718206E-3</v>
+        <v>4.5860629768034603E-3</v>
       </c>
       <c r="L7" s="8">
-        <v>1.30154538545347E-3</v>
+        <v>4.6365435666318204E-3</v>
       </c>
       <c r="M7" s="8">
-        <v>1.3091991139447599E-3</v>
+        <v>4.7587965252627604E-3</v>
       </c>
       <c r="N7" s="8">
-        <v>1.29894915018373E-3</v>
+        <v>4.6195962738988603E-3</v>
       </c>
       <c r="O7" s="8">
-        <v>1.2993399505758199E-3</v>
+        <v>4.6773788542485801E-3</v>
       </c>
       <c r="P7" s="8">
-        <v>1.7633481725585801E-6</v>
+        <v>-1.17807499792607E-4</v>
       </c>
       <c r="Q7" s="8">
-        <v>-1.3592364033937401E-4</v>
+        <v>-5.1041861966306099E-4</v>
       </c>
       <c r="R7" s="8">
-        <v>9.1749551588639203E-5</v>
+        <v>3.7754694188945698E-4</v>
       </c>
       <c r="S7" s="8">
-        <v>9.31943054430196E-7</v>
+        <v>-7.8217718445876006E-5</v>
       </c>
       <c r="T7" s="8">
-        <v>4.73286276623642E-5</v>
+        <v>3.6700038165785401E-4</v>
       </c>
       <c r="U7" s="8">
-        <v>2.6467123511162898E-5</v>
+        <v>1.2556181927753901E-4</v>
       </c>
       <c r="V7" s="8">
-        <v>2.4321109081398299E-5</v>
+        <v>1.8676267231375299E-4</v>
       </c>
       <c r="W7" s="8">
-        <v>3.89303830469338E-5</v>
+        <v>1.7356712356975999E-4</v>
       </c>
       <c r="X7" s="8">
-        <v>7.6712856723919597E-5</v>
+        <v>4.1377265378225302E-4</v>
       </c>
       <c r="Y7" s="8">
-        <v>4.0837088237694404E-6</v>
+        <v>-4.2004722811816402E-5</v>
       </c>
       <c r="Z7" s="8">
-        <v>3.2968869255359699E-6</v>
+        <v>4.3697872708440899E-5</v>
       </c>
       <c r="AA7" s="8">
-        <v>-3.2034436076023703E-8</v>
+        <v>-3.3135657783265498E-7</v>
       </c>
       <c r="AB7" s="8">
-        <v>-4.49737515273092E-6</v>
+        <v>-1.6995276677975299E-5</v>
       </c>
       <c r="AC7" s="8">
-        <v>-1.47788742481273E-6</v>
+        <v>-4.4141257197855896E-6</v>
       </c>
       <c r="AD7" s="8">
-        <v>-3.5177038467101101E-6</v>
+        <v>1.6233967290569601E-4</v>
       </c>
       <c r="AE7" s="8">
-        <v>-1.1607506186542299E-3</v>
+        <v>-4.2973740799262796E-3</v>
       </c>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.25">
@@ -5447,94 +5449,94 @@
         <v>27</v>
       </c>
       <c r="B8" s="8">
-        <v>0.14894778892507099</v>
+        <v>-0.12781623506305101</v>
       </c>
       <c r="C8" s="8">
-        <v>-8.5622027362546E-5</v>
+        <v>-6.9331915164336201E-4</v>
       </c>
       <c r="D8" s="8">
-        <v>-9.3338907756125307E-5</v>
+        <v>-7.2754453798821897E-4</v>
       </c>
       <c r="E8" s="8">
-        <v>1.30494669899701E-3</v>
+        <v>4.7295446316709703E-3</v>
       </c>
       <c r="F8" s="8">
-        <v>1.28907040787262E-3</v>
+        <v>4.7040736256787098E-3</v>
       </c>
       <c r="G8" s="8">
-        <v>1.2941437470714899E-3</v>
+        <v>4.6905684461153096E-3</v>
       </c>
       <c r="H8" s="8">
-        <v>1.3027014332871599E-3</v>
+        <v>4.7439120806390097E-3</v>
       </c>
       <c r="I8" s="8">
-        <v>2.7911699856796599E-3</v>
+        <v>8.3504719071305408E-3</v>
       </c>
       <c r="J8" s="8">
-        <v>1.28761235851701E-3</v>
+        <v>4.5946867809288699E-3</v>
       </c>
       <c r="K8" s="8">
-        <v>1.2835759116033799E-3</v>
+        <v>4.5988479791327502E-3</v>
       </c>
       <c r="L8" s="8">
-        <v>1.2986781211494301E-3</v>
+        <v>4.6805481706372097E-3</v>
       </c>
       <c r="M8" s="8">
-        <v>1.30359998232332E-3</v>
+        <v>4.7824037941729602E-3</v>
       </c>
       <c r="N8" s="8">
-        <v>1.29386872098737E-3</v>
+        <v>4.6229094517746903E-3</v>
       </c>
       <c r="O8" s="8">
-        <v>1.2932212755147701E-3</v>
+        <v>4.7184704429830198E-3</v>
       </c>
       <c r="P8" s="8">
-        <v>-5.6837817329262897E-6</v>
+        <v>-1.02206279997925E-4</v>
       </c>
       <c r="Q8" s="8">
-        <v>-1.3652221546392999E-4</v>
+        <v>-6.7517206836876001E-4</v>
       </c>
       <c r="R8" s="8">
-        <v>7.8347330977951007E-5</v>
+        <v>4.8733699352116898E-4</v>
       </c>
       <c r="S8" s="8">
-        <v>3.5997478630352902E-5</v>
+        <v>-4.6526879257784102E-6</v>
       </c>
       <c r="T8" s="8">
-        <v>4.56440488905475E-5</v>
+        <v>2.6750090122797701E-4</v>
       </c>
       <c r="U8" s="8">
-        <v>-9.1603580059529405E-6</v>
+        <v>1.3420596268146401E-4</v>
       </c>
       <c r="V8" s="8">
-        <v>1.3821006156554199E-5</v>
+        <v>1.55704907262598E-4</v>
       </c>
       <c r="W8" s="8">
-        <v>4.8494212442156504E-7</v>
+        <v>2.1338973945518101E-4</v>
       </c>
       <c r="X8" s="8">
-        <v>6.1647497147890998E-5</v>
+        <v>3.9750400907008102E-4</v>
       </c>
       <c r="Y8" s="8">
-        <v>3.1059261802282901E-6</v>
+        <v>-2.2889505325565101E-5</v>
       </c>
       <c r="Z8" s="8">
-        <v>5.2875855157522297E-6</v>
+        <v>4.4470806058258903E-5</v>
       </c>
       <c r="AA8" s="8">
-        <v>-5.46574582925461E-8</v>
+        <v>-3.3994716566817798E-7</v>
       </c>
       <c r="AB8" s="8">
-        <v>-5.8298771570024597E-6</v>
+        <v>-3.7121733156405898E-5</v>
       </c>
       <c r="AC8" s="8">
-        <v>-1.2703351873162499E-6</v>
+        <v>-3.67931621768857E-6</v>
       </c>
       <c r="AD8" s="8">
-        <v>8.1542893743484107E-6</v>
+        <v>2.38231632399397E-4</v>
       </c>
       <c r="AE8" s="8">
-        <v>-1.18797263085647E-3</v>
+        <v>-4.3130890938787303E-3</v>
       </c>
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.25">
@@ -5542,94 +5544,94 @@
         <v>28</v>
       </c>
       <c r="B9" s="8">
-        <v>8.5719182047086003E-3</v>
+        <v>-0.202805310355131</v>
       </c>
       <c r="C9" s="8">
-        <v>-9.4587619678724195E-5</v>
+        <v>-5.0078457317077104E-4</v>
       </c>
       <c r="D9" s="8">
-        <v>-9.4309582073782804E-5</v>
+        <v>-5.2287959432338398E-4</v>
       </c>
       <c r="E9" s="8">
-        <v>1.29621750655437E-3</v>
+        <v>4.5867728662137798E-3</v>
       </c>
       <c r="F9" s="8">
-        <v>1.2854996651937001E-3</v>
+        <v>4.5475338527812903E-3</v>
       </c>
       <c r="G9" s="8">
-        <v>1.2850841153339799E-3</v>
+        <v>4.55757456725122E-3</v>
       </c>
       <c r="H9" s="8">
-        <v>1.29190877873002E-3</v>
+        <v>4.5792839866289599E-3</v>
       </c>
       <c r="I9" s="8">
-        <v>1.28761235851701E-3</v>
+        <v>4.5946867809288699E-3</v>
       </c>
       <c r="J9" s="8">
-        <v>2.44439763622546E-3</v>
+        <v>7.0002106613082198E-3</v>
       </c>
       <c r="K9" s="8">
-        <v>1.2797589590688801E-3</v>
+        <v>4.4636439109215602E-3</v>
       </c>
       <c r="L9" s="8">
-        <v>1.29370124832082E-3</v>
+        <v>4.5258677708644099E-3</v>
       </c>
       <c r="M9" s="8">
-        <v>1.2966647950291401E-3</v>
+        <v>4.6315425947815901E-3</v>
       </c>
       <c r="N9" s="8">
-        <v>1.28855726345915E-3</v>
+        <v>4.5085763256857399E-3</v>
       </c>
       <c r="O9" s="8">
-        <v>1.2815773325711901E-3</v>
+        <v>4.5399577460164698E-3</v>
       </c>
       <c r="P9" s="8">
-        <v>2.2048112825075198E-6</v>
+        <v>-9.8718637540858606E-5</v>
       </c>
       <c r="Q9" s="8">
-        <v>-1.02328471792849E-4</v>
+        <v>-4.6551734133147701E-4</v>
       </c>
       <c r="R9" s="8">
-        <v>9.7611343526744199E-5</v>
+        <v>3.6778044567765798E-4</v>
       </c>
       <c r="S9" s="8">
-        <v>1.9209982023377301E-5</v>
+        <v>-3.37249260528351E-5</v>
       </c>
       <c r="T9" s="8">
-        <v>4.5609701434661802E-5</v>
+        <v>2.8550608575869798E-4</v>
       </c>
       <c r="U9" s="8">
-        <v>6.5073196545890401E-6</v>
+        <v>1.2358016961150101E-4</v>
       </c>
       <c r="V9" s="8">
-        <v>6.7853092412037403E-6</v>
+        <v>1.5746092611000601E-4</v>
       </c>
       <c r="W9" s="8">
-        <v>5.7886321222854198E-6</v>
+        <v>4.0396697694156298E-5</v>
       </c>
       <c r="X9" s="8">
-        <v>2.7925954255685498E-5</v>
+        <v>2.6402111972485403E-4</v>
       </c>
       <c r="Y9" s="8">
-        <v>4.1408426350238101E-6</v>
+        <v>-3.8244696355540303E-5</v>
       </c>
       <c r="Z9" s="8">
-        <v>5.85062025927404E-6</v>
+        <v>4.4865453907970602E-5</v>
       </c>
       <c r="AA9" s="8">
-        <v>-7.0482077364380495E-8</v>
+        <v>-3.8726745970202101E-7</v>
       </c>
       <c r="AB9" s="8">
-        <v>-5.8203358262003099E-6</v>
+        <v>-3.1013955799169801E-5</v>
       </c>
       <c r="AC9" s="8">
-        <v>-2.8497022323475301E-6</v>
+        <v>-4.1506026425287101E-6</v>
       </c>
       <c r="AD9" s="8">
-        <v>1.39895452850547E-5</v>
+        <v>2.1077922406536901E-4</v>
       </c>
       <c r="AE9" s="8">
-        <v>-1.1193177506530899E-3</v>
+        <v>-4.0646696534893502E-3</v>
       </c>
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.25">
@@ -5637,94 +5639,94 @@
         <v>29</v>
       </c>
       <c r="B10" s="8">
-        <v>6.7588677234638794E-2</v>
+        <v>-9.6672545223256606E-2</v>
       </c>
       <c r="C10" s="8">
-        <v>-7.4270576203027097E-5</v>
+        <v>-5.3208810089653603E-4</v>
       </c>
       <c r="D10" s="8">
-        <v>-4.4411074543662501E-5</v>
+        <v>-4.2703408787423297E-4</v>
       </c>
       <c r="E10" s="8">
-        <v>1.2886934092175401E-3</v>
+        <v>4.5851698551151602E-3</v>
       </c>
       <c r="F10" s="8">
-        <v>1.2837201742287401E-3</v>
+        <v>4.5752739252167699E-3</v>
       </c>
       <c r="G10" s="8">
-        <v>1.2769342224300099E-3</v>
+        <v>4.5644297121687901E-3</v>
       </c>
       <c r="H10" s="8">
-        <v>1.28652734718206E-3</v>
+        <v>4.5860629768034603E-3</v>
       </c>
       <c r="I10" s="8">
-        <v>1.2835759116033799E-3</v>
+        <v>4.5988479791327502E-3</v>
       </c>
       <c r="J10" s="8">
-        <v>1.2797589590688801E-3</v>
+        <v>4.4636439109215602E-3</v>
       </c>
       <c r="K10" s="8">
-        <v>2.1131102698408498E-3</v>
+        <v>6.2044272674097196E-3</v>
       </c>
       <c r="L10" s="8">
-        <v>1.29251967562771E-3</v>
+        <v>4.5503494587941003E-3</v>
       </c>
       <c r="M10" s="8">
-        <v>1.29063952169142E-3</v>
+        <v>4.6536226548409502E-3</v>
       </c>
       <c r="N10" s="8">
-        <v>1.29081836736936E-3</v>
+        <v>4.5618234636934703E-3</v>
       </c>
       <c r="O10" s="8">
-        <v>1.27566869938552E-3</v>
+        <v>4.5439775616713E-3</v>
       </c>
       <c r="P10" s="8">
-        <v>6.6994596507262299E-6</v>
+        <v>-1.4258418278965501E-4</v>
       </c>
       <c r="Q10" s="8">
-        <v>-1.23213370572212E-4</v>
+        <v>-4.5023443574356399E-4</v>
       </c>
       <c r="R10" s="8">
-        <v>9.1650821502225707E-5</v>
+        <v>3.8471512394693197E-4</v>
       </c>
       <c r="S10" s="8">
-        <v>9.1357707325113E-7</v>
+        <v>-1.08659360487395E-4</v>
       </c>
       <c r="T10" s="8">
-        <v>5.1540039121004997E-5</v>
+        <v>2.9271780352915203E-4</v>
       </c>
       <c r="U10" s="8">
-        <v>7.29068227473261E-7</v>
+        <v>7.0169636342636094E-5</v>
       </c>
       <c r="V10" s="8">
-        <v>-1.0732893964541201E-5</v>
+        <v>2.50149592917106E-5</v>
       </c>
       <c r="W10" s="8">
-        <v>-1.1850561039834101E-5</v>
+        <v>-6.5653464212292402E-5</v>
       </c>
       <c r="X10" s="8">
-        <v>-3.4716528760721099E-6</v>
+        <v>1.4479221834593601E-4</v>
       </c>
       <c r="Y10" s="8">
-        <v>5.7973963116998801E-6</v>
+        <v>-3.7604194075758998E-5</v>
       </c>
       <c r="Z10" s="8">
-        <v>5.9177157680461901E-6</v>
+        <v>4.57039339330066E-5</v>
       </c>
       <c r="AA10" s="8">
-        <v>-7.1322725498930402E-8</v>
+        <v>-3.9140830297956302E-7</v>
       </c>
       <c r="AB10" s="8">
-        <v>-5.1533565550716299E-6</v>
+        <v>-2.78108207754154E-5</v>
       </c>
       <c r="AC10" s="8">
-        <v>-1.5945129661537801E-6</v>
+        <v>-5.0610266882774496E-6</v>
       </c>
       <c r="AD10" s="8">
-        <v>1.3448601534204401E-6</v>
+        <v>1.5778377551462199E-4</v>
       </c>
       <c r="AE10" s="8">
-        <v>-1.19392147305834E-3</v>
+        <v>-3.9748938863043504E-3</v>
       </c>
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.25">
@@ -5732,94 +5734,94 @@
         <v>30</v>
       </c>
       <c r="B11" s="8">
-        <v>6.0921118677200098E-2</v>
+        <v>-8.0314668105884807E-2</v>
       </c>
       <c r="C11" s="8">
-        <v>-9.2852913357332201E-5</v>
+        <v>-5.3880278431581402E-4</v>
       </c>
       <c r="D11" s="8">
-        <v>-5.4190283143972801E-5</v>
+        <v>-3.5904815545663199E-4</v>
       </c>
       <c r="E11" s="8">
-        <v>1.3066161794066499E-3</v>
+        <v>4.6522920331823403E-3</v>
       </c>
       <c r="F11" s="8">
-        <v>1.2961002392839699E-3</v>
+        <v>4.6239097506404802E-3</v>
       </c>
       <c r="G11" s="8">
-        <v>1.29579702184705E-3</v>
+        <v>4.6257181545791603E-3</v>
       </c>
       <c r="H11" s="8">
-        <v>1.30154538545347E-3</v>
+        <v>4.6365435666318204E-3</v>
       </c>
       <c r="I11" s="8">
-        <v>1.2986781211494301E-3</v>
+        <v>4.6805481706372097E-3</v>
       </c>
       <c r="J11" s="8">
-        <v>1.29370124832082E-3</v>
+        <v>4.5258677708644099E-3</v>
       </c>
       <c r="K11" s="8">
-        <v>1.29251967562771E-3</v>
+        <v>4.5503494587941003E-3</v>
       </c>
       <c r="L11" s="8">
-        <v>2.59413864167336E-3</v>
+        <v>7.24020014164672E-3</v>
       </c>
       <c r="M11" s="8">
-        <v>1.3084285592283799E-3</v>
+        <v>4.6929919021581404E-3</v>
       </c>
       <c r="N11" s="8">
-        <v>1.3029770389990599E-3</v>
+        <v>4.58434977699765E-3</v>
       </c>
       <c r="O11" s="8">
-        <v>1.29267062937917E-3</v>
+        <v>4.6062291872849097E-3</v>
       </c>
       <c r="P11" s="8">
-        <v>1.4424023571250501E-7</v>
+        <v>-1.3435656663387499E-4</v>
       </c>
       <c r="Q11" s="8">
-        <v>-1.2748629259561799E-4</v>
+        <v>-5.3084061903522302E-4</v>
       </c>
       <c r="R11" s="8">
-        <v>1.11274825643679E-4</v>
+        <v>4.6235248202280499E-4</v>
       </c>
       <c r="S11" s="8">
-        <v>2.7147849673577502E-5</v>
+        <v>-1.11429842498554E-4</v>
       </c>
       <c r="T11" s="8">
-        <v>6.7701892225327306E-5</v>
+        <v>4.4397278691085299E-4</v>
       </c>
       <c r="U11" s="8">
-        <v>1.9143069186142902E-5</v>
+        <v>1.11464236300414E-4</v>
       </c>
       <c r="V11" s="8">
-        <v>2.56481346570062E-5</v>
+        <v>1.56321080429449E-4</v>
       </c>
       <c r="W11" s="8">
-        <v>3.7107748931661102E-5</v>
+        <v>7.98168599170357E-5</v>
       </c>
       <c r="X11" s="8">
-        <v>6.7646001507972196E-5</v>
+        <v>3.5776160519099601E-4</v>
       </c>
       <c r="Y11" s="8">
-        <v>6.3004410475683398E-6</v>
+        <v>-3.9897153704502299E-5</v>
       </c>
       <c r="Z11" s="8">
-        <v>3.8526359116769196E-6</v>
+        <v>5.1317099986123802E-5</v>
       </c>
       <c r="AA11" s="8">
-        <v>-4.9945772065316302E-8</v>
+        <v>-4.1336233720227401E-7</v>
       </c>
       <c r="AB11" s="8">
-        <v>-1.4690678157870599E-6</v>
+        <v>-1.5050465125816501E-5</v>
       </c>
       <c r="AC11" s="8">
-        <v>-2.1073328005879299E-6</v>
+        <v>-3.4540333228986501E-6</v>
       </c>
       <c r="AD11" s="8">
-        <v>1.0200241825056899E-5</v>
+        <v>2.1274685301022001E-4</v>
       </c>
       <c r="AE11" s="8">
-        <v>-1.21760671370202E-3</v>
+        <v>-4.5534873646774004E-3</v>
       </c>
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.25">
@@ -5827,94 +5829,94 @@
         <v>31</v>
       </c>
       <c r="B12" s="8">
-        <v>0.148302382075158</v>
+        <v>-3.7866369865852803E-2</v>
       </c>
       <c r="C12" s="8">
-        <v>-9.7723831375078806E-5</v>
+        <v>-4.65112377182801E-4</v>
       </c>
       <c r="D12" s="8">
-        <v>-9.2512056332152902E-5</v>
+        <v>-5.12542980716846E-4</v>
       </c>
       <c r="E12" s="8">
-        <v>1.3189121274853801E-3</v>
+        <v>4.7474925607503098E-3</v>
       </c>
       <c r="F12" s="8">
-        <v>1.2981937161402001E-3</v>
+        <v>4.7021186043901802E-3</v>
       </c>
       <c r="G12" s="8">
-        <v>1.3049583145837401E-3</v>
+        <v>4.6956156273614798E-3</v>
       </c>
       <c r="H12" s="8">
-        <v>1.3091991139447599E-3</v>
+        <v>4.7587965252627604E-3</v>
       </c>
       <c r="I12" s="8">
-        <v>1.30359998232332E-3</v>
+        <v>4.7824037941729602E-3</v>
       </c>
       <c r="J12" s="8">
-        <v>1.2966647950291401E-3</v>
+        <v>4.6315425947815901E-3</v>
       </c>
       <c r="K12" s="8">
-        <v>1.29063952169142E-3</v>
+        <v>4.6536226548409502E-3</v>
       </c>
       <c r="L12" s="8">
-        <v>1.3084285592283799E-3</v>
+        <v>4.6929919021581404E-3</v>
       </c>
       <c r="M12" s="8">
-        <v>3.0335787278375301E-3</v>
+        <v>1.31357060877366E-2</v>
       </c>
       <c r="N12" s="8">
-        <v>1.3036665411146899E-3</v>
+        <v>4.6213022801124097E-3</v>
       </c>
       <c r="O12" s="8">
-        <v>1.3040664415036301E-3</v>
+        <v>4.6924022896410603E-3</v>
       </c>
       <c r="P12" s="8">
-        <v>2.3862405777066701E-6</v>
+        <v>-5.3372605941057797E-5</v>
       </c>
       <c r="Q12" s="8">
-        <v>-1.3852243966605299E-4</v>
+        <v>-6.6211331224123697E-4</v>
       </c>
       <c r="R12" s="8">
-        <v>8.74754242440102E-5</v>
+        <v>1.0325659136683301E-3</v>
       </c>
       <c r="S12" s="8">
-        <v>6.6818445092609104E-6</v>
+        <v>4.7919923180192E-5</v>
       </c>
       <c r="T12" s="8">
-        <v>6.1627571517514302E-5</v>
+        <v>2.48939172184444E-4</v>
       </c>
       <c r="U12" s="8">
-        <v>-2.5422105778243801E-5</v>
+        <v>-1.51675858598852E-4</v>
       </c>
       <c r="V12" s="8">
-        <v>-3.45555222942537E-6</v>
+        <v>-2.9559364974210999E-5</v>
       </c>
       <c r="W12" s="8">
-        <v>3.3956283051879098E-6</v>
+        <v>-8.2044600952654599E-5</v>
       </c>
       <c r="X12" s="8">
-        <v>7.0502876225044396E-5</v>
+        <v>2.3955425578765099E-4</v>
       </c>
       <c r="Y12" s="8">
-        <v>4.8920983458875596E-6</v>
+        <v>-1.9339000536294E-5</v>
       </c>
       <c r="Z12" s="8">
-        <v>4.9961814672834201E-6</v>
+        <v>9.2545590245435199E-5</v>
       </c>
       <c r="AA12" s="8">
-        <v>-5.4976619710327598E-8</v>
+        <v>-7.5420500605248499E-7</v>
       </c>
       <c r="AB12" s="8">
-        <v>-3.4019366937590902E-6</v>
+        <v>-2.2610561517657399E-5</v>
       </c>
       <c r="AC12" s="8">
-        <v>-1.6643838646635601E-7</v>
+        <v>-1.0130633931063E-7</v>
       </c>
       <c r="AD12" s="8">
-        <v>-7.4381384278055399E-6</v>
+        <v>2.2969195168983701E-4</v>
       </c>
       <c r="AE12" s="8">
-        <v>-1.2731586149253901E-3</v>
+        <v>-6.0942464371640404E-3</v>
       </c>
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.25">
@@ -5922,94 +5924,94 @@
         <v>32</v>
       </c>
       <c r="B13" s="8">
-        <v>-2.0758980700733801E-2</v>
+        <v>-5.5438436330447899E-2</v>
       </c>
       <c r="C13" s="8">
-        <v>-8.9147371597648803E-5</v>
+        <v>-3.72883661111065E-4</v>
       </c>
       <c r="D13" s="8">
-        <v>-4.3534145061445298E-5</v>
+        <v>-1.58026282325078E-4</v>
       </c>
       <c r="E13" s="8">
-        <v>1.3026680835184199E-3</v>
+        <v>4.6017362528768396E-3</v>
       </c>
       <c r="F13" s="8">
-        <v>1.2936548458679601E-3</v>
+        <v>4.5984331081739402E-3</v>
       </c>
       <c r="G13" s="8">
-        <v>1.2902867839833501E-3</v>
+        <v>4.5761952720187998E-3</v>
       </c>
       <c r="H13" s="8">
-        <v>1.29894915018373E-3</v>
+        <v>4.6195962738988603E-3</v>
       </c>
       <c r="I13" s="8">
-        <v>1.29386872098737E-3</v>
+        <v>4.6229094517746903E-3</v>
       </c>
       <c r="J13" s="8">
-        <v>1.28855726345915E-3</v>
+        <v>4.5085763256857399E-3</v>
       </c>
       <c r="K13" s="8">
-        <v>1.29081836736936E-3</v>
+        <v>4.5618234636934703E-3</v>
       </c>
       <c r="L13" s="8">
-        <v>1.3029770389990599E-3</v>
+        <v>4.58434977699765E-3</v>
       </c>
       <c r="M13" s="8">
-        <v>1.3036665411146899E-3</v>
+        <v>4.6213022801124097E-3</v>
       </c>
       <c r="N13" s="8">
-        <v>2.5302177579442E-3</v>
+        <v>9.6275680887160792E-3</v>
       </c>
       <c r="O13" s="8">
-        <v>1.2912300793394E-3</v>
+        <v>4.5791215824155396E-3</v>
       </c>
       <c r="P13" s="8">
-        <v>7.4036241391915499E-6</v>
+        <v>-1.67857133624813E-4</v>
       </c>
       <c r="Q13" s="8">
-        <v>-1.3606083045981601E-4</v>
+        <v>-5.4745476505908104E-4</v>
       </c>
       <c r="R13" s="8">
-        <v>5.9030668521752803E-5</v>
+        <v>2.5507047357712802E-4</v>
       </c>
       <c r="S13" s="8">
-        <v>-1.16746316912147E-6</v>
+        <v>-2.4007612806709901E-4</v>
       </c>
       <c r="T13" s="8">
-        <v>4.5440106257838403E-5</v>
+        <v>2.2081113337179899E-4</v>
       </c>
       <c r="U13" s="8">
-        <v>-4.5794108509856701E-6</v>
+        <v>-5.6234941144648201E-5</v>
       </c>
       <c r="V13" s="8">
-        <v>-2.83720642714685E-7</v>
+        <v>-9.0408377853806504E-5</v>
       </c>
       <c r="W13" s="8">
-        <v>-1.26631378195263E-6</v>
+        <v>-1.85044920229045E-4</v>
       </c>
       <c r="X13" s="8">
-        <v>4.3319296740491001E-5</v>
+        <v>1.6683581296006201E-4</v>
       </c>
       <c r="Y13" s="8">
-        <v>5.4380420427733802E-6</v>
+        <v>-2.1964002949837601E-5</v>
       </c>
       <c r="Z13" s="8">
-        <v>1.47030293991179E-6</v>
+        <v>1.9132547138385999E-5</v>
       </c>
       <c r="AA13" s="8">
-        <v>-3.3706719453285902E-8</v>
+        <v>-1.5228414308471601E-7</v>
       </c>
       <c r="AB13" s="8">
-        <v>-2.6203158692545499E-6</v>
+        <v>5.0566289404939798E-6</v>
       </c>
       <c r="AC13" s="8">
-        <v>-1.32505428609314E-6</v>
+        <v>-1.3863126759049801E-6</v>
       </c>
       <c r="AD13" s="8">
-        <v>-4.9611933504497303E-6</v>
+        <v>1.07030937656175E-4</v>
       </c>
       <c r="AE13" s="8">
-        <v>-1.1148422422248799E-3</v>
+        <v>-4.0630029790011696E-3</v>
       </c>
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.25">
@@ -6017,94 +6019,94 @@
         <v>33</v>
       </c>
       <c r="B14" s="8">
-        <v>-9.82459964541533E-2</v>
+        <v>-0.31971391799535798</v>
       </c>
       <c r="C14" s="8">
-        <v>-9.6704789632620197E-5</v>
+        <v>-4.37032558332609E-4</v>
       </c>
       <c r="D14" s="8">
-        <v>-1.3578467718021399E-4</v>
+        <v>-7.2809303475764801E-4</v>
       </c>
       <c r="E14" s="8">
-        <v>1.3041465695219901E-3</v>
+        <v>4.6812021264640404E-3</v>
       </c>
       <c r="F14" s="8">
-        <v>1.28832358926761E-3</v>
+        <v>4.6573226722622704E-3</v>
       </c>
       <c r="G14" s="8">
-        <v>1.2925493656614001E-3</v>
+        <v>4.6245046333852702E-3</v>
       </c>
       <c r="H14" s="8">
-        <v>1.2993399505758199E-3</v>
+        <v>4.6773788542485801E-3</v>
       </c>
       <c r="I14" s="8">
-        <v>1.2932212755147701E-3</v>
+        <v>4.7184704429830198E-3</v>
       </c>
       <c r="J14" s="8">
-        <v>1.2815773325711901E-3</v>
+        <v>4.5399577460164698E-3</v>
       </c>
       <c r="K14" s="8">
-        <v>1.27566869938552E-3</v>
+        <v>4.5439775616713E-3</v>
       </c>
       <c r="L14" s="8">
-        <v>1.29267062937917E-3</v>
+        <v>4.6062291872849097E-3</v>
       </c>
       <c r="M14" s="8">
-        <v>1.3040664415036301E-3</v>
+        <v>4.6924022896410603E-3</v>
       </c>
       <c r="N14" s="8">
-        <v>1.2912300793394E-3</v>
+        <v>4.5791215824155396E-3</v>
       </c>
       <c r="O14" s="8">
-        <v>3.0787666932401898E-3</v>
+        <v>1.4476673660923801E-2</v>
       </c>
       <c r="P14" s="8">
-        <v>-2.5543163594054799E-5</v>
+        <v>-1.72886599949718E-4</v>
       </c>
       <c r="Q14" s="8">
-        <v>-1.3085217877330401E-4</v>
+        <v>-6.5980354108986197E-4</v>
       </c>
       <c r="R14" s="8">
-        <v>8.8456103967881892E-6</v>
+        <v>1.23138896392694E-4</v>
       </c>
       <c r="S14" s="8">
-        <v>-3.6702645094146201E-5</v>
+        <v>-2.8251685128063601E-4</v>
       </c>
       <c r="T14" s="8">
-        <v>4.0131854807533302E-5</v>
+        <v>2.7217038121784702E-4</v>
       </c>
       <c r="U14" s="8">
-        <v>2.0148854559633401E-5</v>
+        <v>2.5458435466619997E-4</v>
       </c>
       <c r="V14" s="8">
-        <v>9.9248871066617208E-6</v>
+        <v>2.36169593408335E-4</v>
       </c>
       <c r="W14" s="8">
-        <v>2.5526520505940499E-5</v>
+        <v>1.47296158392432E-4</v>
       </c>
       <c r="X14" s="8">
-        <v>9.1333861271211605E-5</v>
+        <v>4.8766945431540798E-4</v>
       </c>
       <c r="Y14" s="8">
-        <v>5.73017255860853E-6</v>
+        <v>-2.6794691721633299E-5</v>
       </c>
       <c r="Z14" s="8">
-        <v>3.00894646192022E-6</v>
+        <v>1.8423051342490199E-5</v>
       </c>
       <c r="AA14" s="8">
-        <v>-3.2335581412306199E-8</v>
+        <v>-5.5499427766562402E-8</v>
       </c>
       <c r="AB14" s="8">
-        <v>-1.4195240517000101E-6</v>
+        <v>-2.5208575074361601E-5</v>
       </c>
       <c r="AC14" s="8">
-        <v>-4.2340734423215199E-7</v>
+        <v>1.0487845794638701E-5</v>
       </c>
       <c r="AD14" s="8">
-        <v>1.40510150203083E-5</v>
+        <v>5.2957405081868802E-7</v>
       </c>
       <c r="AE14" s="8">
-        <v>-1.2355023172130101E-3</v>
+        <v>-4.5002541772588799E-3</v>
       </c>
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.25">
@@ -6112,94 +6114,94 @@
         <v>34</v>
       </c>
       <c r="B15" s="8">
-        <v>0.15445920579865899</v>
+        <v>0.15200989687963301</v>
       </c>
       <c r="C15" s="8">
-        <v>-3.35944138396503E-6</v>
+        <v>6.3804742647886601E-5</v>
       </c>
       <c r="D15" s="8">
-        <v>3.2340782466820501E-6</v>
+        <v>5.8319911090376397E-5</v>
       </c>
       <c r="E15" s="8">
-        <v>-2.75340398856397E-6</v>
+        <v>-1.14913679032E-4</v>
       </c>
       <c r="F15" s="8">
-        <v>-2.71926192311181E-6</v>
+        <v>-2.0891575928672399E-4</v>
       </c>
       <c r="G15" s="8">
-        <v>7.02354558046071E-6</v>
+        <v>-6.6421818947092994E-5</v>
       </c>
       <c r="H15" s="8">
-        <v>1.7633481725585801E-6</v>
+        <v>-1.17807499792607E-4</v>
       </c>
       <c r="I15" s="8">
-        <v>-5.6837817329262897E-6</v>
+        <v>-1.02206279997925E-4</v>
       </c>
       <c r="J15" s="8">
-        <v>2.2048112825075198E-6</v>
+        <v>-9.8718637540858606E-5</v>
       </c>
       <c r="K15" s="8">
-        <v>6.6994596507262299E-6</v>
+        <v>-1.4258418278965501E-4</v>
       </c>
       <c r="L15" s="8">
-        <v>1.4424023571250501E-7</v>
+        <v>-1.3435656663387499E-4</v>
       </c>
       <c r="M15" s="8">
-        <v>2.3862405777066701E-6</v>
+        <v>-5.3372605941057797E-5</v>
       </c>
       <c r="N15" s="8">
-        <v>7.4036241391915499E-6</v>
+        <v>-1.67857133624813E-4</v>
       </c>
       <c r="O15" s="8">
-        <v>-2.5543163594054799E-5</v>
+        <v>-1.72886599949718E-4</v>
       </c>
       <c r="P15" s="8">
-        <v>5.5139287901010802E-4</v>
+        <v>1.5157567595481701E-3</v>
       </c>
       <c r="Q15" s="8">
-        <v>-1.22243367497054E-5</v>
+        <v>-8.72099016357545E-5</v>
       </c>
       <c r="R15" s="8">
-        <v>1.00926604144321E-4</v>
+        <v>4.8507231855980898E-4</v>
       </c>
       <c r="S15" s="8">
-        <v>4.5175697167543002E-5</v>
+        <v>1.7379090929626399E-4</v>
       </c>
       <c r="T15" s="8">
-        <v>-1.1116496459388299E-4</v>
+        <v>-3.87505459933383E-4</v>
       </c>
       <c r="U15" s="8">
-        <v>-7.9562596322946299E-6</v>
+        <v>-1.3517918330719299E-4</v>
       </c>
       <c r="V15" s="8">
-        <v>2.6046774834424301E-5</v>
+        <v>-4.5860129205188301E-5</v>
       </c>
       <c r="W15" s="8">
-        <v>7.9411022508725301E-5</v>
+        <v>1.87842739536983E-4</v>
       </c>
       <c r="X15" s="8">
-        <v>1.50806604864911E-4</v>
+        <v>3.1962367565496503E-4</v>
       </c>
       <c r="Y15" s="8">
-        <v>4.0475815549796298E-6</v>
+        <v>1.9772562492767699E-5</v>
       </c>
       <c r="Z15" s="8">
-        <v>1.3188581899491499E-5</v>
+        <v>4.90632899913266E-5</v>
       </c>
       <c r="AA15" s="8">
-        <v>-1.61178425341575E-7</v>
+        <v>-5.63315086948683E-7</v>
       </c>
       <c r="AB15" s="8">
-        <v>1.08003792716457E-7</v>
+        <v>1.15285388801926E-5</v>
       </c>
       <c r="AC15" s="8">
-        <v>4.0612989300254797E-8</v>
+        <v>2.0022474940849E-7</v>
       </c>
       <c r="AD15" s="8">
-        <v>2.2312841529307998E-5</v>
+        <v>7.8746906126219096E-5</v>
       </c>
       <c r="AE15" s="8">
-        <v>-7.24661402033632E-4</v>
+        <v>-2.3610714720251401E-3</v>
       </c>
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.25">
@@ -6207,94 +6209,94 @@
         <v>51</v>
       </c>
       <c r="B16" s="8">
-        <v>-0.38246461430940898</v>
+        <v>-0.36824257932494597</v>
       </c>
       <c r="C16" s="8">
-        <v>2.6694639089029299E-5</v>
+        <v>1.00876290308307E-4</v>
       </c>
       <c r="D16" s="8">
-        <v>9.1837794212754694E-5</v>
+        <v>2.9892894561407701E-4</v>
       </c>
       <c r="E16" s="8">
-        <v>-1.40446383635702E-4</v>
+        <v>-5.3075190912500703E-4</v>
       </c>
       <c r="F16" s="8">
-        <v>-1.27013501833536E-4</v>
+        <v>-5.8120856585848696E-4</v>
       </c>
       <c r="G16" s="8">
-        <v>-1.3232814886348501E-4</v>
+        <v>-3.6131142327128901E-4</v>
       </c>
       <c r="H16" s="8">
-        <v>-1.3592364033937401E-4</v>
+        <v>-5.1041861966306099E-4</v>
       </c>
       <c r="I16" s="8">
-        <v>-1.3652221546392999E-4</v>
+        <v>-6.7517206836876001E-4</v>
       </c>
       <c r="J16" s="8">
-        <v>-1.02328471792849E-4</v>
+        <v>-4.6551734133147701E-4</v>
       </c>
       <c r="K16" s="8">
-        <v>-1.23213370572212E-4</v>
+        <v>-4.5023443574356399E-4</v>
       </c>
       <c r="L16" s="8">
-        <v>-1.2748629259561799E-4</v>
+        <v>-5.3084061903522302E-4</v>
       </c>
       <c r="M16" s="8">
-        <v>-1.3852243966605299E-4</v>
+        <v>-6.6211331224123697E-4</v>
       </c>
       <c r="N16" s="8">
-        <v>-1.3606083045981601E-4</v>
+        <v>-5.4745476505908104E-4</v>
       </c>
       <c r="O16" s="8">
-        <v>-1.3085217877330401E-4</v>
+        <v>-6.5980354108986197E-4</v>
       </c>
       <c r="P16" s="8">
-        <v>-1.22243367497054E-5</v>
+        <v>-8.72099016357545E-5</v>
       </c>
       <c r="Q16" s="8">
-        <v>8.526481737517E-4</v>
+        <v>2.46271263361724E-3</v>
       </c>
       <c r="R16" s="8">
-        <v>4.4593789898424797E-5</v>
+        <v>-6.7727749857465194E-5</v>
       </c>
       <c r="S16" s="8">
-        <v>9.0764600119650697E-5</v>
+        <v>3.1825643819842801E-4</v>
       </c>
       <c r="T16" s="8">
-        <v>-6.21584990709412E-5</v>
+        <v>-1.5900647852027099E-4</v>
       </c>
       <c r="U16" s="8">
-        <v>-7.0927252510696604E-5</v>
+        <v>-5.1123552812945002E-5</v>
       </c>
       <c r="V16" s="8">
-        <v>-1.2588526729479999E-4</v>
+        <v>-3.2667234141214499E-4</v>
       </c>
       <c r="W16" s="8">
-        <v>-1.72374252316291E-4</v>
+        <v>-5.0881424142339398E-4</v>
       </c>
       <c r="X16" s="8">
-        <v>-1.95533003974164E-4</v>
+        <v>-5.7523419281928895E-4</v>
       </c>
       <c r="Y16" s="8">
-        <v>8.9358621184339395E-7</v>
+        <v>-2.3392786639677001E-5</v>
       </c>
       <c r="Z16" s="8">
-        <v>-6.1393077011780697E-6</v>
+        <v>-2.0375575511255301E-5</v>
       </c>
       <c r="AA16" s="8">
-        <v>1.67171893853106E-8</v>
+        <v>7.7803698616034002E-8</v>
       </c>
       <c r="AB16" s="8">
-        <v>6.0791082894465997E-6</v>
+        <v>3.2946140489506902E-5</v>
       </c>
       <c r="AC16" s="8">
-        <v>-2.5556461319865701E-6</v>
+        <v>-7.46671580140853E-6</v>
       </c>
       <c r="AD16" s="8">
-        <v>2.01561690940573E-5</v>
+        <v>6.2007918261008902E-5</v>
       </c>
       <c r="AE16" s="8">
-        <v>-1.7533681058695E-4</v>
+        <v>-1.0819653516032401E-4</v>
       </c>
     </row>
     <row r="17" spans="1:31" x14ac:dyDescent="0.25">
@@ -6302,94 +6304,94 @@
         <v>52</v>
       </c>
       <c r="B17" s="8">
-        <v>0.16876760694648901</v>
+        <v>0.17275100177917599</v>
       </c>
       <c r="C17" s="8">
-        <v>-3.4739667835109602E-5</v>
+        <v>-8.8051519685915694E-5</v>
       </c>
       <c r="D17" s="8">
-        <v>-4.24053282701221E-6</v>
+        <v>1.3495870467713901E-4</v>
       </c>
       <c r="E17" s="8">
-        <v>6.8412831530912995E-5</v>
+        <v>2.1918894876310301E-4</v>
       </c>
       <c r="F17" s="8">
-        <v>8.7608382022937703E-5</v>
+        <v>3.5894655843644901E-4</v>
       </c>
       <c r="G17" s="8">
-        <v>9.4873922142014601E-5</v>
+        <v>4.3739155051898199E-4</v>
       </c>
       <c r="H17" s="8">
-        <v>9.1749551588639203E-5</v>
+        <v>3.7754694188945698E-4</v>
       </c>
       <c r="I17" s="8">
-        <v>7.8347330977951007E-5</v>
+        <v>4.8733699352116898E-4</v>
       </c>
       <c r="J17" s="8">
-        <v>9.7611343526744199E-5</v>
+        <v>3.6778044567765798E-4</v>
       </c>
       <c r="K17" s="8">
-        <v>9.1650821502225707E-5</v>
+        <v>3.8471512394693197E-4</v>
       </c>
       <c r="L17" s="8">
-        <v>1.11274825643679E-4</v>
+        <v>4.6235248202280499E-4</v>
       </c>
       <c r="M17" s="8">
-        <v>8.74754242440102E-5</v>
+        <v>1.0325659136683301E-3</v>
       </c>
       <c r="N17" s="8">
-        <v>5.9030668521752803E-5</v>
+        <v>2.5507047357712802E-4</v>
       </c>
       <c r="O17" s="8">
-        <v>8.8456103967881892E-6</v>
+        <v>1.23138896392694E-4</v>
       </c>
       <c r="P17" s="8">
-        <v>1.00926604144321E-4</v>
+        <v>4.8507231855980898E-4</v>
       </c>
       <c r="Q17" s="8">
-        <v>4.4593789898424797E-5</v>
+        <v>-6.7727749857465194E-5</v>
       </c>
       <c r="R17" s="8">
-        <v>1.27141641491935E-3</v>
+        <v>4.1498970342714898E-3</v>
       </c>
       <c r="S17" s="8">
-        <v>1.3331231485431199E-4</v>
+        <v>3.19338489304387E-4</v>
       </c>
       <c r="T17" s="8">
-        <v>-7.7289099348945803E-5</v>
+        <v>-2.4655955176100601E-4</v>
       </c>
       <c r="U17" s="8">
-        <v>2.61524329992401E-5</v>
+        <v>1.8057245597323101E-4</v>
       </c>
       <c r="V17" s="8">
-        <v>4.9679280082472199E-5</v>
+        <v>3.4347119074027902E-4</v>
       </c>
       <c r="W17" s="8">
-        <v>7.3722909038106301E-5</v>
+        <v>5.1647441917057602E-4</v>
       </c>
       <c r="X17" s="8">
-        <v>8.4890527292015696E-5</v>
+        <v>4.3677476528932601E-4</v>
       </c>
       <c r="Y17" s="8">
-        <v>-2.9009467812494298E-6</v>
+        <v>4.6739706083266199E-6</v>
       </c>
       <c r="Z17" s="8">
-        <v>6.3330501774483893E-5</v>
+        <v>2.2507723154183601E-4</v>
       </c>
       <c r="AA17" s="8">
-        <v>-5.3640170479163096E-7</v>
+        <v>-1.9169430934189101E-6</v>
       </c>
       <c r="AB17" s="8">
-        <v>3.2967375013854098E-7</v>
+        <v>-3.7641510449400098E-6</v>
       </c>
       <c r="AC17" s="8">
-        <v>-3.9180601223586898E-7</v>
+        <v>-1.8781613042605E-6</v>
       </c>
       <c r="AD17" s="8">
-        <v>-1.97430502566085E-5</v>
+        <v>9.1834849694763106E-5</v>
       </c>
       <c r="AE17" s="8">
-        <v>-2.02747983557493E-3</v>
+        <v>-7.4990084814649301E-3</v>
       </c>
     </row>
     <row r="18" spans="1:31" x14ac:dyDescent="0.25">
@@ -6397,94 +6399,94 @@
         <v>53</v>
       </c>
       <c r="B18" s="8">
-        <v>0.100193867695943</v>
+        <v>2.69305135531397E-2</v>
       </c>
       <c r="C18" s="8">
-        <v>-9.9279137317001898E-6</v>
+        <v>-3.1808198852995001E-5</v>
       </c>
       <c r="D18" s="8">
-        <v>-2.13462856629145E-6</v>
+        <v>-1.669246459867E-5</v>
       </c>
       <c r="E18" s="8">
-        <v>-1.20138070365011E-5</v>
+        <v>1.00391979662983E-4</v>
       </c>
       <c r="F18" s="8">
-        <v>-2.0077626985483901E-5</v>
+        <v>-2.3267827529382999E-4</v>
       </c>
       <c r="G18" s="8">
-        <v>-2.6096533285045499E-6</v>
+        <v>-9.2169724172065905E-5</v>
       </c>
       <c r="H18" s="8">
-        <v>9.31943054430196E-7</v>
+        <v>-7.8217718445876006E-5</v>
       </c>
       <c r="I18" s="8">
-        <v>3.5997478630352902E-5</v>
+        <v>-4.6526879257784102E-6</v>
       </c>
       <c r="J18" s="8">
-        <v>1.9209982023377301E-5</v>
+        <v>-3.37249260528351E-5</v>
       </c>
       <c r="K18" s="8">
-        <v>9.1357707325113E-7</v>
+        <v>-1.08659360487395E-4</v>
       </c>
       <c r="L18" s="8">
-        <v>2.7147849673577502E-5</v>
+        <v>-1.11429842498554E-4</v>
       </c>
       <c r="M18" s="8">
-        <v>6.6818445092609104E-6</v>
+        <v>4.7919923180192E-5</v>
       </c>
       <c r="N18" s="8">
-        <v>-1.16746316912147E-6</v>
+        <v>-2.4007612806709901E-4</v>
       </c>
       <c r="O18" s="8">
-        <v>-3.6702645094146201E-5</v>
+        <v>-2.8251685128063601E-4</v>
       </c>
       <c r="P18" s="8">
-        <v>4.5175697167543002E-5</v>
+        <v>1.7379090929626399E-4</v>
       </c>
       <c r="Q18" s="8">
-        <v>9.0764600119650697E-5</v>
+        <v>3.1825643819842801E-4</v>
       </c>
       <c r="R18" s="8">
-        <v>1.3331231485431199E-4</v>
+        <v>3.19338489304387E-4</v>
       </c>
       <c r="S18" s="8">
-        <v>1.18927491267012E-3</v>
+        <v>2.8485954857367401E-3</v>
       </c>
       <c r="T18" s="8">
-        <v>-4.0794433910680801E-6</v>
+        <v>-5.3345889575927601E-5</v>
       </c>
       <c r="U18" s="8">
-        <v>2.9071024613942401E-5</v>
+        <v>6.5931382929637695E-5</v>
       </c>
       <c r="V18" s="8">
-        <v>5.0188364917226199E-5</v>
+        <v>1.32176915490165E-4</v>
       </c>
       <c r="W18" s="8">
-        <v>7.3108646647776794E-5</v>
+        <v>2.2768379689142899E-4</v>
       </c>
       <c r="X18" s="8">
-        <v>1.09129645541733E-4</v>
+        <v>2.9966941519071402E-4</v>
       </c>
       <c r="Y18" s="8">
-        <v>5.4847932434880296E-6</v>
+        <v>6.5584630574713697E-6</v>
       </c>
       <c r="Z18" s="8">
-        <v>1.42629328627203E-5</v>
+        <v>3.3900225066220798E-5</v>
       </c>
       <c r="AA18" s="8">
-        <v>-2.0701672798139601E-7</v>
+        <v>-5.0378692838769298E-7</v>
       </c>
       <c r="AB18" s="8">
-        <v>-2.4172064832221799E-6</v>
+        <v>2.9117752851039301E-7</v>
       </c>
       <c r="AC18" s="8">
-        <v>6.1002342600027205E-7</v>
+        <v>5.6802974003689501E-6</v>
       </c>
       <c r="AD18" s="8">
-        <v>7.7126497176866198E-5</v>
+        <v>2.0784403889541499E-4</v>
       </c>
       <c r="AE18" s="8">
-        <v>-5.8930728573233597E-4</v>
+        <v>-1.61211490268085E-3</v>
       </c>
     </row>
     <row r="19" spans="1:31" x14ac:dyDescent="0.25">
@@ -6492,94 +6494,94 @@
         <v>16</v>
       </c>
       <c r="B19" s="8">
-        <v>-2.2352681955837301E-2</v>
+        <v>-2.4902749365253399E-2</v>
       </c>
       <c r="C19" s="8">
-        <v>-4.1350089656322197E-5</v>
+        <v>-2.6176963639023702E-4</v>
       </c>
       <c r="D19" s="8">
-        <v>-1.42209370920578E-5</v>
+        <v>-1.53762168743298E-4</v>
       </c>
       <c r="E19" s="8">
-        <v>4.7438658382716498E-5</v>
+        <v>8.0537439077581996E-5</v>
       </c>
       <c r="F19" s="8">
-        <v>5.5217612501320798E-5</v>
+        <v>4.0634834684957598E-4</v>
       </c>
       <c r="G19" s="8">
-        <v>7.1240931926224804E-5</v>
+        <v>3.0757428213766801E-4</v>
       </c>
       <c r="H19" s="8">
-        <v>4.73286276623642E-5</v>
+        <v>3.6700038165785401E-4</v>
       </c>
       <c r="I19" s="8">
-        <v>4.56440488905475E-5</v>
+        <v>2.6750090122797701E-4</v>
       </c>
       <c r="J19" s="8">
-        <v>4.5609701434661802E-5</v>
+        <v>2.8550608575869798E-4</v>
       </c>
       <c r="K19" s="8">
-        <v>5.1540039121004997E-5</v>
+        <v>2.9271780352915203E-4</v>
       </c>
       <c r="L19" s="8">
-        <v>6.7701892225327306E-5</v>
+        <v>4.4397278691085299E-4</v>
       </c>
       <c r="M19" s="8">
-        <v>6.1627571517514302E-5</v>
+        <v>2.48939172184444E-4</v>
       </c>
       <c r="N19" s="8">
-        <v>4.5440106257838403E-5</v>
+        <v>2.2081113337179899E-4</v>
       </c>
       <c r="O19" s="8">
-        <v>4.0131854807533302E-5</v>
+        <v>2.7217038121784702E-4</v>
       </c>
       <c r="P19" s="8">
-        <v>-1.1116496459388299E-4</v>
+        <v>-3.87505459933383E-4</v>
       </c>
       <c r="Q19" s="8">
-        <v>-6.21584990709412E-5</v>
+        <v>-1.5900647852027099E-4</v>
       </c>
       <c r="R19" s="8">
-        <v>-7.7289099348945803E-5</v>
+        <v>-2.4655955176100601E-4</v>
       </c>
       <c r="S19" s="8">
-        <v>-4.0794433910680801E-6</v>
+        <v>-5.3345889575927601E-5</v>
       </c>
       <c r="T19" s="8">
-        <v>1.0236473165117499E-3</v>
+        <v>2.7813388441253902E-3</v>
       </c>
       <c r="U19" s="8">
-        <v>2.2627095769220101E-5</v>
+        <v>2.4519102840085601E-4</v>
       </c>
       <c r="V19" s="8">
-        <v>4.3429198083065101E-5</v>
+        <v>2.5271235672727997E-4</v>
       </c>
       <c r="W19" s="8">
-        <v>6.4314317233292296E-5</v>
+        <v>2.9043772160630298E-4</v>
       </c>
       <c r="X19" s="8">
-        <v>6.7791680830807098E-5</v>
+        <v>2.8642769858823399E-4</v>
       </c>
       <c r="Y19" s="8">
-        <v>3.4875306348864399E-6</v>
+        <v>-1.43664513990799E-5</v>
       </c>
       <c r="Z19" s="8">
-        <v>8.2888908876588401E-6</v>
+        <v>4.4352496490171199E-5</v>
       </c>
       <c r="AA19" s="8">
-        <v>-3.9323794267271799E-8</v>
+        <v>-2.6619085507972503E-7</v>
       </c>
       <c r="AB19" s="8">
-        <v>-1.5749482770519299E-6</v>
+        <v>-3.1262552035122699E-5</v>
       </c>
       <c r="AC19" s="8">
-        <v>-7.3721064632517403E-7</v>
+        <v>-6.3965576374768197E-6</v>
       </c>
       <c r="AD19" s="8">
-        <v>-9.0163730052424107E-6</v>
+        <v>-7.3842093483555802E-6</v>
       </c>
       <c r="AE19" s="8">
-        <v>-3.2003691452027298E-4</v>
+        <v>-8.4121578678384205E-4</v>
       </c>
     </row>
     <row r="20" spans="1:31" x14ac:dyDescent="0.25">
@@ -6587,94 +6589,94 @@
         <v>36</v>
       </c>
       <c r="B20" s="8">
-        <v>2.2309259737625101E-2</v>
+        <v>-7.2532388765864696E-3</v>
       </c>
       <c r="C20" s="8">
-        <v>1.91318083550039E-6</v>
+        <v>-1.22682453199426E-4</v>
       </c>
       <c r="D20" s="8">
-        <v>3.5814952747186198E-5</v>
+        <v>-1.5661594761741801E-5</v>
       </c>
       <c r="E20" s="8">
-        <v>2.79489533657508E-6</v>
+        <v>-2.2737114469953E-4</v>
       </c>
       <c r="F20" s="8">
-        <v>-1.1855162827996501E-5</v>
+        <v>-5.5792132208191203E-5</v>
       </c>
       <c r="G20" s="8">
-        <v>2.11530738951042E-5</v>
+        <v>3.3486641410969298E-5</v>
       </c>
       <c r="H20" s="8">
-        <v>2.6467123511162898E-5</v>
+        <v>1.2556181927753901E-4</v>
       </c>
       <c r="I20" s="8">
-        <v>-9.1603580059529405E-6</v>
+        <v>1.3420596268146401E-4</v>
       </c>
       <c r="J20" s="8">
-        <v>6.5073196545890401E-6</v>
+        <v>1.2358016961150101E-4</v>
       </c>
       <c r="K20" s="8">
-        <v>7.29068227473261E-7</v>
+        <v>7.0169636342636094E-5</v>
       </c>
       <c r="L20" s="8">
-        <v>1.9143069186142902E-5</v>
+        <v>1.11464236300414E-4</v>
       </c>
       <c r="M20" s="8">
-        <v>-2.5422105778243801E-5</v>
+        <v>-1.51675858598852E-4</v>
       </c>
       <c r="N20" s="8">
-        <v>-4.5794108509856701E-6</v>
+        <v>-5.6234941144648201E-5</v>
       </c>
       <c r="O20" s="8">
-        <v>2.0148854559633401E-5</v>
+        <v>2.5458435466619997E-4</v>
       </c>
       <c r="P20" s="8">
-        <v>-7.9562596322946299E-6</v>
+        <v>-1.3517918330719299E-4</v>
       </c>
       <c r="Q20" s="8">
-        <v>-7.0927252510696604E-5</v>
+        <v>-5.1123552812945002E-5</v>
       </c>
       <c r="R20" s="8">
-        <v>2.61524329992401E-5</v>
+        <v>1.8057245597323101E-4</v>
       </c>
       <c r="S20" s="8">
-        <v>2.9071024613942401E-5</v>
+        <v>6.5931382929637695E-5</v>
       </c>
       <c r="T20" s="8">
-        <v>2.2627095769220101E-5</v>
+        <v>2.4519102840085601E-4</v>
       </c>
       <c r="U20" s="8">
-        <v>1.15659631093541E-3</v>
+        <v>3.40977753780993E-3</v>
       </c>
       <c r="V20" s="8">
-        <v>6.8600375327326399E-4</v>
+        <v>2.2410414108183299E-3</v>
       </c>
       <c r="W20" s="8">
-        <v>6.8789877969865898E-4</v>
+        <v>2.2385691406754502E-3</v>
       </c>
       <c r="X20" s="8">
-        <v>6.9197556917172001E-4</v>
+        <v>2.1817657934399401E-3</v>
       </c>
       <c r="Y20" s="8">
-        <v>1.0755515773576001E-6</v>
+        <v>-1.43772382047475E-5</v>
       </c>
       <c r="Z20" s="8">
-        <v>-1.6790683410450901E-6</v>
+        <v>7.6478268761163497E-6</v>
       </c>
       <c r="AA20" s="8">
-        <v>2.1457284703336802E-8</v>
+        <v>2.8830653596794502E-9</v>
       </c>
       <c r="AB20" s="8">
-        <v>4.3895491149337898E-7</v>
+        <v>-8.6704005843760001E-6</v>
       </c>
       <c r="AC20" s="8">
-        <v>-4.2427498088028702E-7</v>
+        <v>-3.8144947964685899E-6</v>
       </c>
       <c r="AD20" s="8">
-        <v>-2.3246166410971702E-6</v>
+        <v>1.9057031304725001E-5</v>
       </c>
       <c r="AE20" s="8">
-        <v>-6.0343873500080401E-4</v>
+        <v>-1.9832797107782602E-3</v>
       </c>
     </row>
     <row r="21" spans="1:31" x14ac:dyDescent="0.25">
@@ -6682,94 +6684,94 @@
         <v>37</v>
       </c>
       <c r="B21" s="8">
-        <v>-2.0425244106391498E-2</v>
+        <v>-9.4496986876251299E-2</v>
       </c>
       <c r="C21" s="8">
-        <v>3.3041349502523199E-6</v>
+        <v>-5.1328063897944601E-5</v>
       </c>
       <c r="D21" s="8">
-        <v>8.9611846726394003E-5</v>
+        <v>1.8177208523987001E-4</v>
       </c>
       <c r="E21" s="8">
-        <v>2.2573849262117901E-5</v>
+        <v>-2.83534469208249E-5</v>
       </c>
       <c r="F21" s="8">
-        <v>-2.5019864470842898E-7</v>
+        <v>1.72448859064701E-5</v>
       </c>
       <c r="G21" s="8">
-        <v>4.4813463677083998E-5</v>
+        <v>1.71640398250429E-4</v>
       </c>
       <c r="H21" s="8">
-        <v>2.4321109081398299E-5</v>
+        <v>1.8676267231375299E-4</v>
       </c>
       <c r="I21" s="8">
-        <v>1.3821006156554199E-5</v>
+        <v>1.55704907262598E-4</v>
       </c>
       <c r="J21" s="8">
-        <v>6.7853092412037403E-6</v>
+        <v>1.5746092611000601E-4</v>
       </c>
       <c r="K21" s="8">
-        <v>-1.0732893964541201E-5</v>
+        <v>2.50149592917106E-5</v>
       </c>
       <c r="L21" s="8">
-        <v>2.56481346570062E-5</v>
+        <v>1.56321080429449E-4</v>
       </c>
       <c r="M21" s="8">
-        <v>-3.45555222942537E-6</v>
+        <v>-2.9559364974210999E-5</v>
       </c>
       <c r="N21" s="8">
-        <v>-2.83720642714685E-7</v>
+        <v>-9.0408377853806504E-5</v>
       </c>
       <c r="O21" s="8">
-        <v>9.9248871066617208E-6</v>
+        <v>2.36169593408335E-4</v>
       </c>
       <c r="P21" s="8">
-        <v>2.6046774834424301E-5</v>
+        <v>-4.5860129205188301E-5</v>
       </c>
       <c r="Q21" s="8">
-        <v>-1.2588526729479999E-4</v>
+        <v>-3.2667234141214499E-4</v>
       </c>
       <c r="R21" s="8">
-        <v>4.9679280082472199E-5</v>
+        <v>3.4347119074027902E-4</v>
       </c>
       <c r="S21" s="8">
-        <v>5.0188364917226199E-5</v>
+        <v>1.32176915490165E-4</v>
       </c>
       <c r="T21" s="8">
-        <v>4.3429198083065101E-5</v>
+        <v>2.5271235672727997E-4</v>
       </c>
       <c r="U21" s="8">
-        <v>6.8600375327326399E-4</v>
+        <v>2.2410414108183299E-3</v>
       </c>
       <c r="V21" s="8">
-        <v>1.1650979497605999E-3</v>
+        <v>3.56757793241688E-3</v>
       </c>
       <c r="W21" s="8">
-        <v>7.6258045902615596E-4</v>
+        <v>2.5638426675269402E-3</v>
       </c>
       <c r="X21" s="8">
-        <v>7.6432702239074602E-4</v>
+        <v>2.48091810430411E-3</v>
       </c>
       <c r="Y21" s="8">
-        <v>1.6172225943054599E-6</v>
+        <v>4.2225664681111201E-7</v>
       </c>
       <c r="Z21" s="8">
-        <v>-2.0082828324227799E-6</v>
+        <v>1.2428868764528301E-5</v>
       </c>
       <c r="AA21" s="8">
-        <v>2.7251499691834201E-8</v>
+        <v>-3.3990391284824898E-8</v>
       </c>
       <c r="AB21" s="8">
-        <v>3.1611865645414502E-7</v>
+        <v>-5.2253166969438403E-7</v>
       </c>
       <c r="AC21" s="8">
-        <v>-6.7520325707067597E-7</v>
+        <v>-2.2037858423240101E-6</v>
       </c>
       <c r="AD21" s="8">
-        <v>-3.7027571161401702E-6</v>
+        <v>8.5782145321438097E-5</v>
       </c>
       <c r="AE21" s="8">
-        <v>-6.4662214277764096E-4</v>
+        <v>-2.6982551204772199E-3</v>
       </c>
     </row>
     <row r="22" spans="1:31" x14ac:dyDescent="0.25">
@@ -6777,94 +6779,94 @@
         <v>39</v>
       </c>
       <c r="B22" s="8">
-        <v>-7.3517302034389304E-2</v>
+        <v>-0.112476767151477</v>
       </c>
       <c r="C22" s="8">
-        <v>4.6952328925989297E-5</v>
+        <v>1.37808615346704E-5</v>
       </c>
       <c r="D22" s="8">
-        <v>1.6642486668752901E-4</v>
+        <v>3.6057120221624198E-4</v>
       </c>
       <c r="E22" s="8">
-        <v>5.2391126157177499E-5</v>
+        <v>-1.09671859748506E-4</v>
       </c>
       <c r="F22" s="8">
-        <v>1.3362115106098899E-5</v>
+        <v>-8.7808865050775895E-5</v>
       </c>
       <c r="G22" s="8">
-        <v>6.0259661667862401E-5</v>
+        <v>1.09688348883064E-4</v>
       </c>
       <c r="H22" s="8">
-        <v>3.89303830469338E-5</v>
+        <v>1.7356712356975999E-4</v>
       </c>
       <c r="I22" s="8">
-        <v>4.8494212442156504E-7</v>
+        <v>2.1338973945518101E-4</v>
       </c>
       <c r="J22" s="8">
-        <v>5.7886321222854198E-6</v>
+        <v>4.0396697694156298E-5</v>
       </c>
       <c r="K22" s="8">
-        <v>-1.1850561039834101E-5</v>
+        <v>-6.5653464212292402E-5</v>
       </c>
       <c r="L22" s="8">
-        <v>3.7107748931661102E-5</v>
+        <v>7.98168599170357E-5</v>
       </c>
       <c r="M22" s="8">
-        <v>3.3956283051879098E-6</v>
+        <v>-8.2044600952654599E-5</v>
       </c>
       <c r="N22" s="8">
-        <v>-1.26631378195263E-6</v>
+        <v>-1.85044920229045E-4</v>
       </c>
       <c r="O22" s="8">
-        <v>2.5526520505940499E-5</v>
+        <v>1.47296158392432E-4</v>
       </c>
       <c r="P22" s="8">
-        <v>7.9411022508725301E-5</v>
+        <v>1.87842739536983E-4</v>
       </c>
       <c r="Q22" s="8">
-        <v>-1.72374252316291E-4</v>
+        <v>-5.0881424142339398E-4</v>
       </c>
       <c r="R22" s="8">
-        <v>7.3722909038106301E-5</v>
+        <v>5.1647441917057602E-4</v>
       </c>
       <c r="S22" s="8">
-        <v>7.3108646647776794E-5</v>
+        <v>2.2768379689142899E-4</v>
       </c>
       <c r="T22" s="8">
-        <v>6.4314317233292296E-5</v>
+        <v>2.9043772160630298E-4</v>
       </c>
       <c r="U22" s="8">
-        <v>6.8789877969865898E-4</v>
+        <v>2.2385691406754502E-3</v>
       </c>
       <c r="V22" s="8">
-        <v>7.6258045902615596E-4</v>
+        <v>2.5638426675269402E-3</v>
       </c>
       <c r="W22" s="8">
-        <v>1.20493905098047E-3</v>
+        <v>3.8306822409799601E-3</v>
       </c>
       <c r="X22" s="8">
-        <v>8.5029326638424801E-4</v>
+        <v>2.73751557320012E-3</v>
       </c>
       <c r="Y22" s="8">
-        <v>3.23297719815847E-6</v>
+        <v>1.71157883522571E-5</v>
       </c>
       <c r="Z22" s="8">
-        <v>-3.5967480327397998E-6</v>
+        <v>1.5466329563506301E-5</v>
       </c>
       <c r="AA22" s="8">
-        <v>4.2421803351244302E-8</v>
+        <v>-6.84626953266624E-8</v>
       </c>
       <c r="AB22" s="8">
-        <v>1.05480574777121E-6</v>
+        <v>3.9565577872333896E-6</v>
       </c>
       <c r="AC22" s="8">
-        <v>-1.5233223652456701E-6</v>
+        <v>-4.7159729258686503E-6</v>
       </c>
       <c r="AD22" s="8">
-        <v>-5.8971570598778703E-6</v>
+        <v>5.6801925958415799E-5</v>
       </c>
       <c r="AE22" s="8">
-        <v>-6.8990241620984203E-4</v>
+        <v>-3.0962587631466298E-3</v>
       </c>
     </row>
     <row r="23" spans="1:31" x14ac:dyDescent="0.25">
@@ -6872,94 +6874,94 @@
         <v>40</v>
       </c>
       <c r="B23" s="8">
-        <v>-0.111862436797608</v>
+        <v>-0.161010158606473</v>
       </c>
       <c r="C23" s="8">
-        <v>1.26673590139778E-4</v>
+        <v>2.6670464367964402E-4</v>
       </c>
       <c r="D23" s="8">
-        <v>2.72846330738831E-4</v>
+        <v>6.8757980451412504E-4</v>
       </c>
       <c r="E23" s="8">
-        <v>8.9592986289246894E-5</v>
+        <v>1.9093646054300299E-4</v>
       </c>
       <c r="F23" s="8">
-        <v>5.09529760875342E-5</v>
+        <v>2.0714690065796199E-4</v>
       </c>
       <c r="G23" s="8">
-        <v>1.2557094002796701E-4</v>
+        <v>4.1452257141545799E-4</v>
       </c>
       <c r="H23" s="8">
-        <v>7.6712856723919597E-5</v>
+        <v>4.1377265378225302E-4</v>
       </c>
       <c r="I23" s="8">
-        <v>6.1647497147890998E-5</v>
+        <v>3.9750400907008102E-4</v>
       </c>
       <c r="J23" s="8">
-        <v>2.7925954255685498E-5</v>
+        <v>2.6402111972485403E-4</v>
       </c>
       <c r="K23" s="8">
-        <v>-3.4716528760721099E-6</v>
+        <v>1.4479221834593601E-4</v>
       </c>
       <c r="L23" s="8">
-        <v>6.7646001507972196E-5</v>
+        <v>3.5776160519099601E-4</v>
       </c>
       <c r="M23" s="8">
-        <v>7.0502876225044396E-5</v>
+        <v>2.3955425578765099E-4</v>
       </c>
       <c r="N23" s="8">
-        <v>4.3319296740491001E-5</v>
+        <v>1.6683581296006201E-4</v>
       </c>
       <c r="O23" s="8">
-        <v>9.1333861271211605E-5</v>
+        <v>4.8766945431540798E-4</v>
       </c>
       <c r="P23" s="8">
-        <v>1.50806604864911E-4</v>
+        <v>3.1962367565496503E-4</v>
       </c>
       <c r="Q23" s="8">
-        <v>-1.95533003974164E-4</v>
+        <v>-5.7523419281928895E-4</v>
       </c>
       <c r="R23" s="8">
-        <v>8.4890527292015696E-5</v>
+        <v>4.3677476528932601E-4</v>
       </c>
       <c r="S23" s="8">
-        <v>1.09129645541733E-4</v>
+        <v>2.9966941519071402E-4</v>
       </c>
       <c r="T23" s="8">
-        <v>6.7791680830807098E-5</v>
+        <v>2.8642769858823399E-4</v>
       </c>
       <c r="U23" s="8">
-        <v>6.9197556917172001E-4</v>
+        <v>2.1817657934399401E-3</v>
       </c>
       <c r="V23" s="8">
-        <v>7.6432702239074602E-4</v>
+        <v>2.48091810430411E-3</v>
       </c>
       <c r="W23" s="8">
-        <v>8.5029326638424801E-4</v>
+        <v>2.73751557320012E-3</v>
       </c>
       <c r="X23" s="8">
-        <v>1.2805826737165599E-3</v>
+        <v>3.7743225970113198E-3</v>
       </c>
       <c r="Y23" s="8">
-        <v>5.9471859720296402E-6</v>
+        <v>1.10848542735282E-5</v>
       </c>
       <c r="Z23" s="8">
-        <v>-4.4497951762676798E-6</v>
+        <v>1.4178425208033201E-5</v>
       </c>
       <c r="AA23" s="8">
-        <v>3.70618181247553E-8</v>
+        <v>-9.8588443623185394E-8</v>
       </c>
       <c r="AB23" s="8">
-        <v>2.1344625515066801E-6</v>
+        <v>4.6883855760179402E-6</v>
       </c>
       <c r="AC23" s="8">
-        <v>-2.10778213698244E-6</v>
+        <v>-7.6268194260970204E-6</v>
       </c>
       <c r="AD23" s="8">
-        <v>-1.56869463954917E-5</v>
+        <v>2.4376716060478E-5</v>
       </c>
       <c r="AE23" s="8">
-        <v>-8.1528135790835102E-4</v>
+        <v>-3.1777611495323998E-3</v>
       </c>
     </row>
     <row r="24" spans="1:31" x14ac:dyDescent="0.25">
@@ -6967,94 +6969,94 @@
         <v>38</v>
       </c>
       <c r="B24" s="8">
-        <v>3.1499827611078501E-2</v>
+        <v>2.9527355353348401E-2</v>
       </c>
       <c r="C24" s="8">
-        <v>4.5839887235734501E-6</v>
+        <v>2.2311736444310899E-5</v>
       </c>
       <c r="D24" s="8">
-        <v>1.32370347400556E-5</v>
+        <v>5.7439378178796598E-5</v>
       </c>
       <c r="E24" s="8">
-        <v>3.1332567222028001E-6</v>
+        <v>-3.82994438180937E-5</v>
       </c>
       <c r="F24" s="8">
-        <v>3.04745386287188E-6</v>
+        <v>-3.4986498382821998E-5</v>
       </c>
       <c r="G24" s="8">
-        <v>1.4649771969649601E-6</v>
+        <v>-2.0452982035959601E-5</v>
       </c>
       <c r="H24" s="8">
-        <v>4.0837088237694404E-6</v>
+        <v>-4.2004722811816402E-5</v>
       </c>
       <c r="I24" s="8">
-        <v>3.1059261802282901E-6</v>
+        <v>-2.2889505325565101E-5</v>
       </c>
       <c r="J24" s="8">
-        <v>4.1408426350238101E-6</v>
+        <v>-3.8244696355540303E-5</v>
       </c>
       <c r="K24" s="8">
-        <v>5.7973963116998801E-6</v>
+        <v>-3.7604194075758998E-5</v>
       </c>
       <c r="L24" s="8">
-        <v>6.3004410475683398E-6</v>
+        <v>-3.9897153704502299E-5</v>
       </c>
       <c r="M24" s="8">
-        <v>4.8920983458875596E-6</v>
+        <v>-1.9339000536294E-5</v>
       </c>
       <c r="N24" s="8">
-        <v>5.4380420427733802E-6</v>
+        <v>-2.1964002949837601E-5</v>
       </c>
       <c r="O24" s="8">
-        <v>5.73017255860853E-6</v>
+        <v>-2.6794691721633299E-5</v>
       </c>
       <c r="P24" s="8">
-        <v>4.0475815549796298E-6</v>
+        <v>1.9772562492767699E-5</v>
       </c>
       <c r="Q24" s="8">
-        <v>8.9358621184339395E-7</v>
+        <v>-2.3392786639677001E-5</v>
       </c>
       <c r="R24" s="8">
-        <v>-2.9009467812494298E-6</v>
+        <v>4.6739706083266199E-6</v>
       </c>
       <c r="S24" s="8">
-        <v>5.4847932434880296E-6</v>
+        <v>6.5584630574713697E-6</v>
       </c>
       <c r="T24" s="8">
-        <v>3.4875306348864399E-6</v>
+        <v>-1.43664513990799E-5</v>
       </c>
       <c r="U24" s="8">
-        <v>1.0755515773576001E-6</v>
+        <v>-1.43772382047475E-5</v>
       </c>
       <c r="V24" s="8">
-        <v>1.6172225943054599E-6</v>
+        <v>4.2225664681111201E-7</v>
       </c>
       <c r="W24" s="8">
-        <v>3.23297719815847E-6</v>
+        <v>1.71157883522571E-5</v>
       </c>
       <c r="X24" s="8">
-        <v>5.9471859720296402E-6</v>
+        <v>1.10848542735282E-5</v>
       </c>
       <c r="Y24" s="8">
-        <v>1.0350666141442901E-5</v>
+        <v>3.0699232814009897E-5</v>
       </c>
       <c r="Z24" s="8">
-        <v>-1.14461256540696E-7</v>
+        <v>-1.9998044292343899E-6</v>
       </c>
       <c r="AA24" s="8">
-        <v>-3.02704311298918E-9</v>
+        <v>1.8380501427824601E-9</v>
       </c>
       <c r="AB24" s="8">
-        <v>-1.04691264626086E-7</v>
+        <v>2.1337350776016201E-6</v>
       </c>
       <c r="AC24" s="8">
-        <v>1.9117712640044601E-8</v>
+        <v>3.99198813375145E-8</v>
       </c>
       <c r="AD24" s="8">
-        <v>7.5244011205111602E-7</v>
+        <v>1.3964968192175099E-6</v>
       </c>
       <c r="AE24" s="8">
-        <v>-1.5302013977393599E-4</v>
+        <v>-3.3848296783398199E-4</v>
       </c>
     </row>
     <row r="25" spans="1:31" x14ac:dyDescent="0.25">
@@ -7062,94 +7064,94 @@
         <v>48</v>
       </c>
       <c r="B25" s="8">
-        <v>4.5049355726028799E-2</v>
+        <v>4.6221602675515797E-2</v>
       </c>
       <c r="C25" s="8">
-        <v>1.45013491727407E-6</v>
+        <v>-9.4898716168457208E-6</v>
       </c>
       <c r="D25" s="8">
-        <v>4.93913349409411E-6</v>
+        <v>2.8524472822873699E-5</v>
       </c>
       <c r="E25" s="8">
-        <v>7.68817234143558E-7</v>
+        <v>4.4985635076731103E-6</v>
       </c>
       <c r="F25" s="8">
-        <v>4.2571390162228302E-6</v>
+        <v>3.3794828438001103E-5</v>
       </c>
       <c r="G25" s="8">
-        <v>5.2401916774154498E-6</v>
+        <v>2.5187695891426099E-5</v>
       </c>
       <c r="H25" s="8">
-        <v>3.2968869255359699E-6</v>
+        <v>4.3697872708440899E-5</v>
       </c>
       <c r="I25" s="8">
-        <v>5.2875855157522297E-6</v>
+        <v>4.4470806058258903E-5</v>
       </c>
       <c r="J25" s="8">
-        <v>5.85062025927404E-6</v>
+        <v>4.4865453907970602E-5</v>
       </c>
       <c r="K25" s="8">
-        <v>5.9177157680461901E-6</v>
+        <v>4.57039339330066E-5</v>
       </c>
       <c r="L25" s="8">
-        <v>3.8526359116769196E-6</v>
+        <v>5.1317099986123802E-5</v>
       </c>
       <c r="M25" s="8">
-        <v>4.9961814672834201E-6</v>
+        <v>9.2545590245435199E-5</v>
       </c>
       <c r="N25" s="8">
-        <v>1.47030293991179E-6</v>
+        <v>1.9132547138385999E-5</v>
       </c>
       <c r="O25" s="8">
-        <v>3.00894646192022E-6</v>
+        <v>1.8423051342490199E-5</v>
       </c>
       <c r="P25" s="8">
-        <v>1.3188581899491499E-5</v>
+        <v>4.90632899913266E-5</v>
       </c>
       <c r="Q25" s="8">
-        <v>-6.1393077011780697E-6</v>
+        <v>-2.0375575511255301E-5</v>
       </c>
       <c r="R25" s="8">
-        <v>6.3330501774483893E-5</v>
+        <v>2.2507723154183601E-4</v>
       </c>
       <c r="S25" s="8">
-        <v>1.42629328627203E-5</v>
+        <v>3.3900225066220798E-5</v>
       </c>
       <c r="T25" s="8">
-        <v>8.2888908876588401E-6</v>
+        <v>4.4352496490171199E-5</v>
       </c>
       <c r="U25" s="8">
-        <v>-1.6790683410450901E-6</v>
+        <v>7.6478268761163497E-6</v>
       </c>
       <c r="V25" s="8">
-        <v>-2.0082828324227799E-6</v>
+        <v>1.2428868764528301E-5</v>
       </c>
       <c r="W25" s="8">
-        <v>-3.5967480327397998E-6</v>
+        <v>1.5466329563506301E-5</v>
       </c>
       <c r="X25" s="8">
-        <v>-4.4497951762676798E-6</v>
+        <v>1.4178425208033201E-5</v>
       </c>
       <c r="Y25" s="8">
-        <v>-1.14461256540696E-7</v>
+        <v>-1.9998044292343899E-6</v>
       </c>
       <c r="Z25" s="8">
-        <v>1.39805020942688E-5</v>
+        <v>4.2632751870482203E-5</v>
       </c>
       <c r="AA25" s="8">
-        <v>-1.32089135050812E-7</v>
+        <v>-3.9515841732911299E-7</v>
       </c>
       <c r="AB25" s="8">
-        <v>-3.6573957757971702E-7</v>
+        <v>-3.7123067398777002E-6</v>
       </c>
       <c r="AC25" s="8">
-        <v>-4.1793257396012402E-7</v>
+        <v>-1.7179438057105301E-6</v>
       </c>
       <c r="AD25" s="8">
-        <v>3.1822258948493501E-7</v>
+        <v>2.1273421699361599E-5</v>
       </c>
       <c r="AE25" s="8">
-        <v>-3.2109578282953202E-4</v>
+        <v>-9.9664994795096106E-4</v>
       </c>
     </row>
     <row r="26" spans="1:31" x14ac:dyDescent="0.25">
@@ -7157,94 +7159,94 @@
         <v>49</v>
       </c>
       <c r="B26" s="8">
-        <v>-6.7431571214193698E-4</v>
+        <v>-6.86606951369517E-4</v>
       </c>
       <c r="C26" s="8">
-        <v>-2.47772683099099E-8</v>
+        <v>4.0925599950415701E-8</v>
       </c>
       <c r="D26" s="8">
-        <v>-1.2776962150714601E-7</v>
+        <v>-5.1436043815626398E-7</v>
       </c>
       <c r="E26" s="8">
-        <v>-1.6172177507542401E-8</v>
+        <v>-3.7095477023163901E-8</v>
       </c>
       <c r="F26" s="8">
-        <v>-4.27724312176736E-8</v>
+        <v>-2.3690207389474601E-7</v>
       </c>
       <c r="G26" s="8">
-        <v>-4.5394718343653701E-8</v>
+        <v>-1.93505974880005E-7</v>
       </c>
       <c r="H26" s="8">
-        <v>-3.2034436076023703E-8</v>
+        <v>-3.3135657783265498E-7</v>
       </c>
       <c r="I26" s="8">
-        <v>-5.46574582925461E-8</v>
+        <v>-3.3994716566817798E-7</v>
       </c>
       <c r="J26" s="8">
-        <v>-7.0482077364380495E-8</v>
+        <v>-3.8726745970202101E-7</v>
       </c>
       <c r="K26" s="8">
-        <v>-7.1322725498930402E-8</v>
+        <v>-3.9140830297956302E-7</v>
       </c>
       <c r="L26" s="8">
-        <v>-4.9945772065316302E-8</v>
+        <v>-4.1336233720227401E-7</v>
       </c>
       <c r="M26" s="8">
-        <v>-5.4976619710327598E-8</v>
+        <v>-7.5420500605248499E-7</v>
       </c>
       <c r="N26" s="8">
-        <v>-3.3706719453285902E-8</v>
+        <v>-1.5228414308471601E-7</v>
       </c>
       <c r="O26" s="8">
-        <v>-3.2335581412306199E-8</v>
+        <v>-5.5499427766562402E-8</v>
       </c>
       <c r="P26" s="8">
-        <v>-1.61178425341575E-7</v>
+        <v>-5.63315086948683E-7</v>
       </c>
       <c r="Q26" s="8">
-        <v>1.67171893853106E-8</v>
+        <v>7.7803698616034002E-8</v>
       </c>
       <c r="R26" s="8">
-        <v>-5.3640170479163096E-7</v>
+        <v>-1.9169430934189101E-6</v>
       </c>
       <c r="S26" s="8">
-        <v>-2.0701672798139601E-7</v>
+        <v>-5.0378692838769298E-7</v>
       </c>
       <c r="T26" s="8">
-        <v>-3.9323794267271799E-8</v>
+        <v>-2.6619085507972503E-7</v>
       </c>
       <c r="U26" s="8">
-        <v>2.1457284703336802E-8</v>
+        <v>2.8830653596794502E-9</v>
       </c>
       <c r="V26" s="8">
-        <v>2.7251499691834201E-8</v>
+        <v>-3.3990391284824898E-8</v>
       </c>
       <c r="W26" s="8">
-        <v>4.2421803351244302E-8</v>
+        <v>-6.84626953266624E-8</v>
       </c>
       <c r="X26" s="8">
-        <v>3.70618181247553E-8</v>
+        <v>-9.8588443623185394E-8</v>
       </c>
       <c r="Y26" s="8">
-        <v>-3.02704311298918E-9</v>
+        <v>1.8380501427824601E-9</v>
       </c>
       <c r="Z26" s="8">
-        <v>-1.32089135050812E-7</v>
+        <v>-3.9515841732911299E-7</v>
       </c>
       <c r="AA26" s="8">
-        <v>1.30749754927767E-9</v>
+        <v>3.8289055883269798E-9</v>
       </c>
       <c r="AB26" s="8">
-        <v>6.9132346830288197E-9</v>
+        <v>3.9808241967133103E-8</v>
       </c>
       <c r="AC26" s="8">
-        <v>7.0457598686589896E-9</v>
+        <v>2.3741115434956502E-8</v>
       </c>
       <c r="AD26" s="8">
-        <v>-1.2779040095727899E-8</v>
+        <v>-2.1684165839640399E-7</v>
       </c>
       <c r="AE26" s="8">
-        <v>2.8115420070873301E-6</v>
+        <v>8.6458425788635301E-6</v>
       </c>
     </row>
     <row r="27" spans="1:31" x14ac:dyDescent="0.25">
@@ -7252,94 +7254,94 @@
         <v>18</v>
       </c>
       <c r="B27" s="8">
-        <v>0.51922278051236304</v>
+        <v>0.526057048058441</v>
       </c>
       <c r="C27" s="8">
-        <v>4.2520475251047098E-6</v>
+        <v>2.5991923536983598E-5</v>
       </c>
       <c r="D27" s="8">
-        <v>2.6595676599196199E-6</v>
+        <v>2.2496862997745398E-5</v>
       </c>
       <c r="E27" s="8">
-        <v>-3.80156139540954E-6</v>
+        <v>8.5625345480353595E-6</v>
       </c>
       <c r="F27" s="8">
-        <v>-4.1990539914227599E-6</v>
+        <v>-3.5368859764654901E-5</v>
       </c>
       <c r="G27" s="8">
-        <v>-4.1673943924848104E-6</v>
+        <v>1.28039239555633E-5</v>
       </c>
       <c r="H27" s="8">
-        <v>-4.49737515273092E-6</v>
+        <v>-1.6995276677975299E-5</v>
       </c>
       <c r="I27" s="8">
-        <v>-5.8298771570024597E-6</v>
+        <v>-3.7121733156405898E-5</v>
       </c>
       <c r="J27" s="8">
-        <v>-5.8203358262003099E-6</v>
+        <v>-3.1013955799169801E-5</v>
       </c>
       <c r="K27" s="8">
-        <v>-5.1533565550716299E-6</v>
+        <v>-2.78108207754154E-5</v>
       </c>
       <c r="L27" s="8">
-        <v>-1.4690678157870599E-6</v>
+        <v>-1.5050465125816501E-5</v>
       </c>
       <c r="M27" s="8">
-        <v>-3.4019366937590902E-6</v>
+        <v>-2.2610561517657399E-5</v>
       </c>
       <c r="N27" s="8">
-        <v>-2.6203158692545499E-6</v>
+        <v>5.0566289404939798E-6</v>
       </c>
       <c r="O27" s="8">
-        <v>-1.4195240517000101E-6</v>
+        <v>-2.5208575074361601E-5</v>
       </c>
       <c r="P27" s="8">
-        <v>1.08003792716457E-7</v>
+        <v>1.15285388801926E-5</v>
       </c>
       <c r="Q27" s="8">
-        <v>6.0791082894465997E-6</v>
+        <v>3.2946140489506902E-5</v>
       </c>
       <c r="R27" s="8">
-        <v>3.2967375013854098E-7</v>
+        <v>-3.7641510449400098E-6</v>
       </c>
       <c r="S27" s="8">
-        <v>-2.4172064832221799E-6</v>
+        <v>2.9117752851039301E-7</v>
       </c>
       <c r="T27" s="8">
-        <v>-1.5749482770519299E-6</v>
+        <v>-3.1262552035122699E-5</v>
       </c>
       <c r="U27" s="8">
-        <v>4.3895491149337898E-7</v>
+        <v>-8.6704005843760001E-6</v>
       </c>
       <c r="V27" s="8">
-        <v>3.1611865645414502E-7</v>
+        <v>-5.2253166969438403E-7</v>
       </c>
       <c r="W27" s="8">
-        <v>1.05480574777121E-6</v>
+        <v>3.9565577872333896E-6</v>
       </c>
       <c r="X27" s="8">
-        <v>2.1344625515066801E-6</v>
+        <v>4.6883855760179402E-6</v>
       </c>
       <c r="Y27" s="8">
-        <v>-1.04691264626086E-7</v>
+        <v>2.1337350776016201E-6</v>
       </c>
       <c r="Z27" s="8">
-        <v>-3.6573957757971702E-7</v>
+        <v>-3.7123067398777002E-6</v>
       </c>
       <c r="AA27" s="8">
-        <v>6.9132346830288197E-9</v>
+        <v>3.9808241967133103E-8</v>
       </c>
       <c r="AB27" s="8">
-        <v>1.0418663537171999E-5</v>
+        <v>3.0475755629161901E-5</v>
       </c>
       <c r="AC27" s="8">
-        <v>5.6560584577999205E-7</v>
+        <v>1.9907806098561198E-6</v>
       </c>
       <c r="AD27" s="8">
-        <v>1.02766494514438E-5</v>
+        <v>2.3221912121004099E-5</v>
       </c>
       <c r="AE27" s="8">
-        <v>-1.41865162949764E-4</v>
+        <v>-4.0515264223235702E-4</v>
       </c>
     </row>
     <row r="28" spans="1:31" x14ac:dyDescent="0.25">
@@ -7347,94 +7349,94 @@
         <v>50</v>
       </c>
       <c r="B28" s="8">
-        <v>-5.51414225038949E-2</v>
+        <v>-5.6516321748449401E-2</v>
       </c>
       <c r="C28" s="8">
-        <v>2.1251460495041098E-6</v>
+        <v>7.40382263859905E-6</v>
       </c>
       <c r="D28" s="8">
-        <v>4.3413988867913702E-6</v>
+        <v>6.8988713607926301E-6</v>
       </c>
       <c r="E28" s="8">
-        <v>-4.9403178871451397E-7</v>
+        <v>1.75452746457684E-6</v>
       </c>
       <c r="F28" s="8">
-        <v>-8.8823586269393703E-7</v>
+        <v>-3.0909265059234698E-7</v>
       </c>
       <c r="G28" s="8">
-        <v>-4.8435834400380895E-7</v>
+        <v>1.78258937571622E-7</v>
       </c>
       <c r="H28" s="8">
-        <v>-1.47788742481273E-6</v>
+        <v>-4.4141257197855896E-6</v>
       </c>
       <c r="I28" s="8">
-        <v>-1.2703351873162499E-6</v>
+        <v>-3.67931621768857E-6</v>
       </c>
       <c r="J28" s="8">
-        <v>-2.8497022323475301E-6</v>
+        <v>-4.1506026425287101E-6</v>
       </c>
       <c r="K28" s="8">
-        <v>-1.5945129661537801E-6</v>
+        <v>-5.0610266882774496E-6</v>
       </c>
       <c r="L28" s="8">
-        <v>-2.1073328005879299E-6</v>
+        <v>-3.4540333228986501E-6</v>
       </c>
       <c r="M28" s="8">
-        <v>-1.6643838646635601E-7</v>
+        <v>-1.0130633931063E-7</v>
       </c>
       <c r="N28" s="8">
-        <v>-1.32505428609314E-6</v>
+        <v>-1.3863126759049801E-6</v>
       </c>
       <c r="O28" s="8">
-        <v>-4.2340734423215199E-7</v>
+        <v>1.0487845794638701E-5</v>
       </c>
       <c r="P28" s="8">
-        <v>4.0612989300254797E-8</v>
+        <v>2.0022474940849E-7</v>
       </c>
       <c r="Q28" s="8">
-        <v>-2.5556461319865701E-6</v>
+        <v>-7.46671580140853E-6</v>
       </c>
       <c r="R28" s="8">
-        <v>-3.9180601223586898E-7</v>
+        <v>-1.8781613042605E-6</v>
       </c>
       <c r="S28" s="8">
-        <v>6.1002342600027205E-7</v>
+        <v>5.6802974003689501E-6</v>
       </c>
       <c r="T28" s="8">
-        <v>-7.3721064632517403E-7</v>
+        <v>-6.3965576374768197E-6</v>
       </c>
       <c r="U28" s="8">
-        <v>-4.2427498088028702E-7</v>
+        <v>-3.8144947964685899E-6</v>
       </c>
       <c r="V28" s="8">
-        <v>-6.7520325707067597E-7</v>
+        <v>-2.2037858423240101E-6</v>
       </c>
       <c r="W28" s="8">
-        <v>-1.5233223652456701E-6</v>
+        <v>-4.7159729258686503E-6</v>
       </c>
       <c r="X28" s="8">
-        <v>-2.10778213698244E-6</v>
+        <v>-7.6268194260970204E-6</v>
       </c>
       <c r="Y28" s="8">
-        <v>1.9117712640044601E-8</v>
+        <v>3.99198813375145E-8</v>
       </c>
       <c r="Z28" s="8">
-        <v>-4.1793257396012402E-7</v>
+        <v>-1.7179438057105301E-6</v>
       </c>
       <c r="AA28" s="8">
-        <v>7.0457598686589896E-9</v>
+        <v>2.3741115434956502E-8</v>
       </c>
       <c r="AB28" s="8">
-        <v>5.6560584577999205E-7</v>
+        <v>1.9907806098561198E-6</v>
       </c>
       <c r="AC28" s="8">
-        <v>1.5956473406324001E-6</v>
+        <v>4.26427895494281E-6</v>
       </c>
       <c r="AD28" s="8">
-        <v>-2.93388171338196E-7</v>
+        <v>-4.4892553353969296E-6</v>
       </c>
       <c r="AE28" s="8">
-        <v>-8.4235765194742295E-5</v>
+        <v>-2.11891036359431E-4</v>
       </c>
     </row>
     <row r="29" spans="1:31" x14ac:dyDescent="0.25">
@@ -7442,94 +7444,94 @@
         <v>4</v>
       </c>
       <c r="B29" s="8">
-        <v>-0.44139471763670501</v>
+        <v>-0.49544866460460202</v>
       </c>
       <c r="C29" s="8">
-        <v>-1.9128150086190201E-6</v>
+        <v>-4.8026066892916801E-5</v>
       </c>
       <c r="D29" s="8">
-        <v>2.25295374613286E-5</v>
+        <v>5.77422874847142E-5</v>
       </c>
       <c r="E29" s="8">
-        <v>-5.7051324325327504E-6</v>
+        <v>9.7261481075393093E-5</v>
       </c>
       <c r="F29" s="8">
-        <v>-6.9770188772042104E-6</v>
+        <v>1.53713222151612E-4</v>
       </c>
       <c r="G29" s="8">
-        <v>-1.70374440643536E-5</v>
+        <v>1.5001784691466401E-4</v>
       </c>
       <c r="H29" s="8">
-        <v>-3.5177038467101101E-6</v>
+        <v>1.6233967290569601E-4</v>
       </c>
       <c r="I29" s="8">
-        <v>8.1542893743484107E-6</v>
+        <v>2.38231632399397E-4</v>
       </c>
       <c r="J29" s="8">
-        <v>1.39895452850547E-5</v>
+        <v>2.1077922406536901E-4</v>
       </c>
       <c r="K29" s="8">
-        <v>1.3448601534204401E-6</v>
+        <v>1.5778377551462199E-4</v>
       </c>
       <c r="L29" s="8">
-        <v>1.0200241825056899E-5</v>
+        <v>2.1274685301022001E-4</v>
       </c>
       <c r="M29" s="8">
-        <v>-7.4381384278055399E-6</v>
+        <v>2.2969195168983701E-4</v>
       </c>
       <c r="N29" s="8">
-        <v>-4.9611933504497303E-6</v>
+        <v>1.07030937656175E-4</v>
       </c>
       <c r="O29" s="8">
-        <v>1.40510150203083E-5</v>
+        <v>5.2957405081868802E-7</v>
       </c>
       <c r="P29" s="8">
-        <v>2.2312841529307998E-5</v>
+        <v>7.8746906126219096E-5</v>
       </c>
       <c r="Q29" s="8">
-        <v>2.01561690940573E-5</v>
+        <v>6.2007918261008902E-5</v>
       </c>
       <c r="R29" s="8">
-        <v>-1.97430502566085E-5</v>
+        <v>9.1834849694763106E-5</v>
       </c>
       <c r="S29" s="8">
-        <v>7.7126497176866198E-5</v>
+        <v>2.0784403889541499E-4</v>
       </c>
       <c r="T29" s="8">
-        <v>-9.0163730052424107E-6</v>
+        <v>-7.3842093483555802E-6</v>
       </c>
       <c r="U29" s="8">
-        <v>-2.3246166410971702E-6</v>
+        <v>1.9057031304725001E-5</v>
       </c>
       <c r="V29" s="8">
-        <v>-3.7027571161401702E-6</v>
+        <v>8.5782145321438097E-5</v>
       </c>
       <c r="W29" s="8">
-        <v>-5.8971570598778703E-6</v>
+        <v>5.6801925958415799E-5</v>
       </c>
       <c r="X29" s="8">
-        <v>-1.56869463954917E-5</v>
+        <v>2.4376716060478E-5</v>
       </c>
       <c r="Y29" s="8">
-        <v>7.5244011205111602E-7</v>
+        <v>1.3964968192175099E-6</v>
       </c>
       <c r="Z29" s="8">
-        <v>3.1822258948493501E-7</v>
+        <v>2.1273421699361599E-5</v>
       </c>
       <c r="AA29" s="8">
-        <v>-1.2779040095727899E-8</v>
+        <v>-2.1684165839640399E-7</v>
       </c>
       <c r="AB29" s="8">
-        <v>1.02766494514438E-5</v>
+        <v>2.3221912121004099E-5</v>
       </c>
       <c r="AC29" s="8">
-        <v>-2.93388171338196E-7</v>
+        <v>-4.4892553353969296E-6</v>
       </c>
       <c r="AD29" s="8">
-        <v>4.6776097726605802E-4</v>
+        <v>1.33355987347836E-3</v>
       </c>
       <c r="AE29" s="8">
-        <v>-3.4106762755969298E-4</v>
+        <v>-1.4332835738693199E-3</v>
       </c>
     </row>
     <row r="30" spans="1:31" x14ac:dyDescent="0.25">
@@ -7537,94 +7539,94 @@
         <v>8</v>
       </c>
       <c r="B30" s="8">
-        <v>7.5327132209720302</v>
+        <v>7.7225735958606903</v>
       </c>
       <c r="C30" s="8">
-        <v>-6.0671325234516705E-4</v>
+        <v>-1.3114087070277801E-3</v>
       </c>
       <c r="D30" s="8">
-        <v>-9.6085385193366804E-4</v>
+        <v>-2.8149845667864602E-3</v>
       </c>
       <c r="E30" s="8">
-        <v>-1.12083588291062E-3</v>
+        <v>-3.5270488242725899E-3</v>
       </c>
       <c r="F30" s="8">
-        <v>-1.1979880361858901E-3</v>
+        <v>-3.9310536595509897E-3</v>
       </c>
       <c r="G30" s="8">
-        <v>-1.28786286519915E-3</v>
+        <v>-4.8546487627397104E-3</v>
       </c>
       <c r="H30" s="8">
-        <v>-1.1607506186542299E-3</v>
+        <v>-4.2973740799262796E-3</v>
       </c>
       <c r="I30" s="8">
-        <v>-1.18797263085647E-3</v>
+        <v>-4.3130890938787303E-3</v>
       </c>
       <c r="J30" s="8">
-        <v>-1.1193177506530899E-3</v>
+        <v>-4.0646696534893502E-3</v>
       </c>
       <c r="K30" s="8">
-        <v>-1.19392147305834E-3</v>
+        <v>-3.9748938863043504E-3</v>
       </c>
       <c r="L30" s="8">
-        <v>-1.21760671370202E-3</v>
+        <v>-4.5534873646774004E-3</v>
       </c>
       <c r="M30" s="8">
-        <v>-1.2731586149253901E-3</v>
+        <v>-6.0942464371640404E-3</v>
       </c>
       <c r="N30" s="8">
-        <v>-1.1148422422248799E-3</v>
+        <v>-4.0630029790011696E-3</v>
       </c>
       <c r="O30" s="8">
-        <v>-1.2355023172130101E-3</v>
+        <v>-4.5002541772588799E-3</v>
       </c>
       <c r="P30" s="8">
-        <v>-7.24661402033632E-4</v>
+        <v>-2.3610714720251401E-3</v>
       </c>
       <c r="Q30" s="8">
-        <v>-1.7533681058695E-4</v>
+        <v>-1.0819653516032401E-4</v>
       </c>
       <c r="R30" s="8">
-        <v>-2.02747983557493E-3</v>
+        <v>-7.4990084814649301E-3</v>
       </c>
       <c r="S30" s="8">
-        <v>-5.8930728573233597E-4</v>
+        <v>-1.61211490268085E-3</v>
       </c>
       <c r="T30" s="8">
-        <v>-3.2003691452027298E-4</v>
+        <v>-8.4121578678384205E-4</v>
       </c>
       <c r="U30" s="8">
-        <v>-6.0343873500080401E-4</v>
+        <v>-1.9832797107782602E-3</v>
       </c>
       <c r="V30" s="8">
-        <v>-6.4662214277764096E-4</v>
+        <v>-2.6982551204772199E-3</v>
       </c>
       <c r="W30" s="8">
-        <v>-6.8990241620984203E-4</v>
+        <v>-3.0962587631466298E-3</v>
       </c>
       <c r="X30" s="8">
-        <v>-8.1528135790835102E-4</v>
+        <v>-3.1777611495323998E-3</v>
       </c>
       <c r="Y30" s="8">
-        <v>-1.5302013977393599E-4</v>
+        <v>-3.3848296783398199E-4</v>
       </c>
       <c r="Z30" s="8">
-        <v>-3.2109578282953202E-4</v>
+        <v>-9.9664994795096106E-4</v>
       </c>
       <c r="AA30" s="8">
-        <v>2.8115420070873301E-6</v>
+        <v>8.6458425788635301E-6</v>
       </c>
       <c r="AB30" s="8">
-        <v>-1.41865162949764E-4</v>
+        <v>-4.0515264223235702E-4</v>
       </c>
       <c r="AC30" s="8">
-        <v>-8.4235765194742295E-5</v>
+        <v>-2.11891036359431E-4</v>
       </c>
       <c r="AD30" s="8">
-        <v>-3.4106762755969298E-4</v>
+        <v>-1.4332835738693199E-3</v>
       </c>
       <c r="AE30" s="8">
-        <v>1.9665745745903001E-2</v>
+        <v>5.70983634775485E-2</v>
       </c>
     </row>
   </sheetData>
@@ -7634,7 +7636,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B47509E5-1D6F-4320-9093-19C3760C2BB0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90524CD9-FC25-43D3-A993-DE235AB6CC61}">
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -7682,10 +7684,10 @@
         <v>9</v>
       </c>
       <c r="B2" s="8">
-        <v>2.7622687751800701</v>
+        <v>2.35467496679941</v>
       </c>
       <c r="C2" s="8">
-        <v>3.3858357918848003E-2</v>
+        <v>6.9069456464306803E-2</v>
       </c>
       <c r="D2" s="8">
         <v>0</v>
@@ -7714,13 +7716,13 @@
         <v>10</v>
       </c>
       <c r="B3" s="8">
-        <v>-3.5538705948887798E-2</v>
+        <v>-0.24198337491288899</v>
       </c>
       <c r="C3" s="8">
         <v>0</v>
       </c>
       <c r="D3" s="8">
-        <v>2.2439382908269301E-2</v>
+        <v>7.5403388623418305E-2</v>
       </c>
       <c r="E3" s="8">
         <v>0</v>
@@ -7746,7 +7748,7 @@
         <v>11</v>
       </c>
       <c r="B4" s="8">
-        <v>2.4179001655162198</v>
+        <v>2.2243870676080899</v>
       </c>
       <c r="C4" s="8">
         <v>0</v>
@@ -7755,7 +7757,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="8">
-        <v>4.7363239388380697E-2</v>
+        <v>0.120428313054354</v>
       </c>
       <c r="F4" s="8">
         <v>0</v>
@@ -7778,7 +7780,7 @@
         <v>12</v>
       </c>
       <c r="B5" s="8">
-        <v>0.28837240198177899</v>
+        <v>0.46931929008701301</v>
       </c>
       <c r="C5" s="8">
         <v>0</v>
@@ -7790,7 +7792,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="8">
-        <v>1.1776504736085399E-2</v>
+        <v>3.7609571473982903E-2</v>
       </c>
       <c r="G5" s="8">
         <v>0</v>
@@ -7810,7 +7812,7 @@
         <v>13</v>
       </c>
       <c r="B6" s="8">
-        <v>-3.471549104748E-2</v>
+        <v>0.32963971401742198</v>
       </c>
       <c r="C6" s="8">
         <v>0</v>
@@ -7825,7 +7827,7 @@
         <v>0</v>
       </c>
       <c r="G6" s="8">
-        <v>2.1546619803242399E-2</v>
+        <v>7.8868177962366004E-2</v>
       </c>
       <c r="H6" s="8">
         <v>0</v>
@@ -7842,7 +7844,7 @@
         <v>14</v>
       </c>
       <c r="B7" s="8">
-        <v>0.40218945718307902</v>
+        <v>0.50881870912696703</v>
       </c>
       <c r="C7" s="8">
         <v>0</v>
@@ -7860,7 +7862,7 @@
         <v>0</v>
       </c>
       <c r="H7" s="8">
-        <v>3.19895238680055E-2</v>
+        <v>9.6615858761655807E-2</v>
       </c>
       <c r="I7" s="8">
         <v>0</v>
@@ -7874,7 +7876,7 @@
         <v>41</v>
       </c>
       <c r="B8" s="8">
-        <v>-3.7644918767706799E-3</v>
+        <v>-4.8297154669191801E-2</v>
       </c>
       <c r="C8" s="8">
         <v>0</v>
@@ -7895,7 +7897,7 @@
         <v>0</v>
       </c>
       <c r="I8" s="8">
-        <v>2.0772674429183399E-3</v>
+        <v>6.2309351345657699E-3</v>
       </c>
       <c r="J8" s="8">
         <v>0</v>
@@ -7906,7 +7908,7 @@
         <v>42</v>
       </c>
       <c r="B9" s="8">
-        <v>0.105920616998777</v>
+        <v>9.3530220184674898E-2</v>
       </c>
       <c r="C9" s="8">
         <v>0</v>
@@ -7930,7 +7932,7 @@
         <v>0</v>
       </c>
       <c r="J9" s="8">
-        <v>1.5080772364612E-3</v>
+        <v>4.7043339317226502E-3</v>
       </c>
     </row>
   </sheetData>
@@ -7940,7 +7942,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{618F5F34-CE9A-4B0D-ADBB-1E566DDF28EA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AC91F47-2228-4CD9-A074-8E6E16867A5F}">
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -7988,10 +7990,10 @@
         <v>9</v>
       </c>
       <c r="B2" s="8">
-        <v>1.63854829591822</v>
+        <v>1.5139328433578501</v>
       </c>
       <c r="C2" s="8">
-        <v>2.0721283089929401E-2</v>
+        <v>4.7236552700516299E-2</v>
       </c>
       <c r="D2" s="8">
         <v>0</v>
@@ -8020,13 +8022,13 @@
         <v>10</v>
       </c>
       <c r="B3" s="8">
-        <v>-0.48559234836281201</v>
+        <v>-0.48073948127084398</v>
       </c>
       <c r="C3" s="8">
         <v>0</v>
       </c>
       <c r="D3" s="8">
-        <v>1.1651368337091799E-2</v>
+        <v>3.7014332213409301E-2</v>
       </c>
       <c r="E3" s="8">
         <v>0</v>
@@ -8052,7 +8054,7 @@
         <v>11</v>
       </c>
       <c r="B4" s="8">
-        <v>0.95419874562846696</v>
+        <v>1.01828935240596</v>
       </c>
       <c r="C4" s="8">
         <v>0</v>
@@ -8061,7 +8063,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="8">
-        <v>1.6899289364673099E-2</v>
+        <v>4.4210426742189599E-2</v>
       </c>
       <c r="F4" s="8">
         <v>0</v>
@@ -8084,7 +8086,7 @@
         <v>12</v>
       </c>
       <c r="B5" s="8">
-        <v>0.31066186805058998</v>
+        <v>0.27098592511367098</v>
       </c>
       <c r="C5" s="8">
         <v>0</v>
@@ -8096,7 +8098,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="8">
-        <v>9.4749852583087199E-3</v>
+        <v>2.73448397678396E-2</v>
       </c>
       <c r="G5" s="8">
         <v>0</v>
@@ -8116,7 +8118,7 @@
         <v>13</v>
       </c>
       <c r="B6" s="8">
-        <v>0.21691732939406599</v>
+        <v>0.57419350826948201</v>
       </c>
       <c r="C6" s="8">
         <v>0</v>
@@ -8131,7 +8133,7 @@
         <v>0</v>
       </c>
       <c r="G6" s="8">
-        <v>1.6193911596461101E-2</v>
+        <v>5.4247573191936703E-2</v>
       </c>
       <c r="H6" s="8">
         <v>0</v>
@@ -8148,7 +8150,7 @@
         <v>14</v>
       </c>
       <c r="B7" s="8">
-        <v>0.357628432789794</v>
+        <v>0.89789769015377296</v>
       </c>
       <c r="C7" s="8">
         <v>0</v>
@@ -8166,7 +8168,7 @@
         <v>0</v>
       </c>
       <c r="H7" s="8">
-        <v>2.2852384035043499E-2</v>
+        <v>6.9945951727442598E-2</v>
       </c>
       <c r="I7" s="8">
         <v>0</v>
@@ -8180,7 +8182,7 @@
         <v>41</v>
       </c>
       <c r="B8" s="8">
-        <v>-0.12724822008849901</v>
+        <v>-0.17522919144738</v>
       </c>
       <c r="C8" s="8">
         <v>0</v>
@@ -8201,7 +8203,7 @@
         <v>0</v>
       </c>
       <c r="I8" s="8">
-        <v>2.7320666605839001E-3</v>
+        <v>7.5243458978919804E-3</v>
       </c>
       <c r="J8" s="8">
         <v>0</v>
@@ -8212,7 +8214,7 @@
         <v>42</v>
       </c>
       <c r="B9" s="8">
-        <v>6.8646120858877696E-2</v>
+        <v>3.6751492737489899E-2</v>
       </c>
       <c r="C9" s="8">
         <v>0</v>
@@ -8236,7 +8238,7 @@
         <v>0</v>
       </c>
       <c r="J9" s="8">
-        <v>1.65004864511128E-3</v>
+        <v>4.4853158471408801E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>